<commit_message>
"Adding Notifications, System Constrain, ID Constrain, ADMIN Constrain CRS"
</commit_message>
<xml_diff>
--- a/LH_REQUIREMENTS/LH_CRS.xlsx
+++ b/LH_REQUIREMENTS/LH_CRS.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>ID</t>
   </si>
@@ -27,6 +27,9 @@
     <t>Requirment</t>
   </si>
   <si>
+    <t xml:space="preserve">web-based system/PC based </t>
+  </si>
+  <si>
     <t>users must be able to create an account using email, unique username, and a strong password</t>
   </si>
   <si>
@@ -36,6 +39,12 @@
     <t>users should be able to publish articles, upload videos, or record audio content</t>
   </si>
   <si>
+    <t>users can follow specific categories to receive notifications when new content is added</t>
+  </si>
+  <si>
+    <t>admin features must be available for content and user management</t>
+  </si>
+  <si>
     <t>Feature</t>
   </si>
   <si>
@@ -45,9 +54,24 @@
     <t>Publish and upload</t>
   </si>
   <si>
+    <t>Notifications</t>
+  </si>
+  <si>
+    <t>ID Constrain</t>
+  </si>
+  <si>
+    <t>ADMIN Constrain</t>
+  </si>
+  <si>
+    <t>System Constrain</t>
+  </si>
+  <si>
     <t>Registration</t>
   </si>
   <si>
+    <t>each user must be assigned a unique user ID after creating an account</t>
+  </si>
+  <si>
     <t>LH_CRS_REGISTRATION_001</t>
   </si>
   <si>
@@ -55,13 +79,25 @@
   </si>
   <si>
     <t>LH_CRS_PUBLISH_003</t>
+  </si>
+  <si>
+    <t>LH_CRS_NOTIFICATIONS_004</t>
+  </si>
+  <si>
+    <t>LH_CRS_SYSTEM-CONSTRAINS_005</t>
+  </si>
+  <si>
+    <t>LH_CRS_ID-CONSTRAINS_006</t>
+  </si>
+  <si>
+    <t>LH_CRS_ADMIN-CONSTRAINS_007</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -91,6 +127,13 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -100,7 +143,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -184,11 +227,46 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -205,31 +283,15 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="7">
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
     <dxf>
       <font>
         <b/>
@@ -269,6 +331,44 @@
         <right style="thin">
           <color indexed="64"/>
         </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
         <top style="thin">
           <color indexed="64"/>
         </top>
@@ -291,22 +391,6 @@
       </border>
     </dxf>
     <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
       <border>
         <bottom style="thin">
           <color indexed="64"/>
@@ -321,14 +405,12 @@
         <right style="thin">
           <color indexed="64"/>
         </right>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
       </border>
     </dxf>
   </dxfs>
@@ -345,12 +427,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:C4" totalsRowShown="0" headerRowDxfId="6" headerRowBorderDxfId="5" tableBorderDxfId="4" totalsRowBorderDxfId="3">
-  <autoFilter ref="A1:C4"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:C8" totalsRowShown="0" headerRowDxfId="1" headerRowBorderDxfId="5" tableBorderDxfId="6" totalsRowBorderDxfId="4">
+  <autoFilter ref="A1:C8"/>
   <tableColumns count="3">
-    <tableColumn id="2" name="Feature" dataDxfId="2"/>
-    <tableColumn id="1" name="ID" dataDxfId="1"/>
-    <tableColumn id="3" name="Requirment" dataDxfId="0"/>
+    <tableColumn id="2" name="Feature" dataDxfId="3"/>
+    <tableColumn id="1" name="ID" dataDxfId="0"/>
+    <tableColumn id="3" name="Requirment" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -619,10 +701,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -635,7 +717,7 @@
   <sheetData>
     <row r="1" spans="1:3" s="2" customFormat="1" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>0</v>
@@ -646,40 +728,84 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="11" t="s">
         <v>7</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>4</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation allowBlank="1" showDropDown="1" sqref="A2:A3"/>
+    <dataValidation allowBlank="1" showDropDown="1" sqref="A5 A7:A8 A2:A3"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
adding owner section to CRS sheet
</commit_message>
<xml_diff>
--- a/LH_REQUIREMENTS/LH_CRS.xlsx
+++ b/LH_REQUIREMENTS/LH_CRS.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="27">
   <si>
     <t>ID</t>
   </si>
@@ -91,13 +91,22 @@
   </si>
   <si>
     <t>LH_CRS_ADMIN-CONSTRAINS_007</t>
+  </si>
+  <si>
+    <t>Owner</t>
+  </si>
+  <si>
+    <t>Ahmed Abuzaid</t>
+  </si>
+  <si>
+    <t>Omar Sherif</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -125,6 +134,7 @@
       <sz val="15"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -134,16 +144,36 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -262,11 +292,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -287,11 +330,37 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="7">
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -331,44 +400,6 @@
         <right style="thin">
           <color indexed="64"/>
         </right>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
         <top style="thin">
           <color indexed="64"/>
         </top>
@@ -391,6 +422,22 @@
       </border>
     </dxf>
     <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <border>
         <bottom style="thin">
           <color indexed="64"/>
@@ -405,12 +452,14 @@
         <right style="thin">
           <color indexed="64"/>
         </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
       </border>
     </dxf>
   </dxfs>
@@ -427,12 +476,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:C8" totalsRowShown="0" headerRowDxfId="1" headerRowBorderDxfId="5" tableBorderDxfId="6" totalsRowBorderDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:C8" totalsRowShown="0" headerRowDxfId="6" headerRowBorderDxfId="5" tableBorderDxfId="4" totalsRowBorderDxfId="3">
   <autoFilter ref="A1:C8"/>
   <tableColumns count="3">
-    <tableColumn id="2" name="Feature" dataDxfId="3"/>
-    <tableColumn id="1" name="ID" dataDxfId="0"/>
-    <tableColumn id="3" name="Requirment" dataDxfId="2"/>
+    <tableColumn id="2" name="Feature" dataDxfId="2"/>
+    <tableColumn id="1" name="ID" dataDxfId="1"/>
+    <tableColumn id="3" name="Requirment" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -701,10 +750,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -712,10 +761,10 @@
     <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="32.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="86" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="86.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="2" customFormat="1" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" s="2" customFormat="1" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>8</v>
       </c>
@@ -725,8 +774,11 @@
       <c r="C1" s="5" t="s">
         <v>1</v>
       </c>
+      <c r="D1" s="14" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>15</v>
       </c>
@@ -736,8 +788,11 @@
       <c r="C2" s="7" t="s">
         <v>3</v>
       </c>
+      <c r="D2" s="12" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -747,8 +802,11 @@
       <c r="C3" s="7" t="s">
         <v>4</v>
       </c>
+      <c r="D3" s="13" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
@@ -758,8 +816,11 @@
       <c r="C4" s="7" t="s">
         <v>5</v>
       </c>
+      <c r="D4" s="12" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
@@ -769,8 +830,11 @@
       <c r="C5" s="7" t="s">
         <v>6</v>
       </c>
+      <c r="D5" s="13" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>14</v>
       </c>
@@ -780,8 +844,11 @@
       <c r="C6" s="7" t="s">
         <v>2</v>
       </c>
+      <c r="D6" s="12" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
@@ -791,8 +858,11 @@
       <c r="C7" t="s">
         <v>16</v>
       </c>
+      <c r="D7" s="15" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
         <v>13</v>
       </c>
@@ -801,11 +871,14 @@
       </c>
       <c r="C8" s="11" t="s">
         <v>7</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation allowBlank="1" showDropDown="1" sqref="A5 A7:A8 A2:A3"/>
+    <dataValidation allowBlank="1" showDropDown="1" sqref="A5 A7:A8 A2:A3 D2:D8"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Assigned Ahmed to review the updated changes
I've made the required adjustments based on the open review comments on CRS.
 I've also added a task for Ahmed to review the updated changes.
</commit_message>
<xml_diff>
--- a/LH_REQUIREMENTS/LH_CRS.xlsx
+++ b/LH_REQUIREMENTS/LH_CRS.xlsx
@@ -1,13 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E5921E1-7085-42A9-9B59-CA744F11FE9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="LH_CRS" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="27">
   <si>
     <t>ID</t>
   </si>
@@ -27,9 +28,6 @@
     <t>Requirment</t>
   </si>
   <si>
-    <t xml:space="preserve">web-based system/PC based </t>
-  </si>
-  <si>
     <t>users must be able to create an account using email, unique username, and a strong password</t>
   </si>
   <si>
@@ -81,23 +79,35 @@
     <t>LH_CRS_PUBLISH_003</t>
   </si>
   <si>
-    <t>LH_CRS_NOTIFICATIONS_004</t>
-  </si>
-  <si>
-    <t>LH_CRS_SYSTEM-CONSTRAINS_005</t>
-  </si>
-  <si>
-    <t>LH_CRS_ID-CONSTRAINS_006</t>
-  </si>
-  <si>
-    <t>LH_CRS_ADMIN-CONSTRAINS_007</t>
+    <t>Owner</t>
+  </si>
+  <si>
+    <t>Ahmed Abuzaid</t>
+  </si>
+  <si>
+    <t>Omar Sherif</t>
+  </si>
+  <si>
+    <t>LH-CRS-NOTIFICATIONS-004</t>
+  </si>
+  <si>
+    <t>LH-CRS-SYSTEM-CONSTRAINS-005</t>
+  </si>
+  <si>
+    <t>LH-CRS-ID-CONSTRAINS-006</t>
+  </si>
+  <si>
+    <t>LH-CRS-ADMIN-CONSTRAINS-007</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The system should be either web-based or PC-based. </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -125,6 +135,7 @@
       <sz val="15"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -134,16 +145,43 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -262,11 +300,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -287,11 +338,37 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="7">
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -331,44 +408,6 @@
         <right style="thin">
           <color indexed="64"/>
         </right>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
         <top style="thin">
           <color indexed="64"/>
         </top>
@@ -391,6 +430,22 @@
       </border>
     </dxf>
     <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <border>
         <bottom style="thin">
           <color indexed="64"/>
@@ -405,12 +460,14 @@
         <right style="thin">
           <color indexed="64"/>
         </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
       </border>
     </dxf>
   </dxfs>
@@ -427,12 +484,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:C8" totalsRowShown="0" headerRowDxfId="1" headerRowBorderDxfId="5" tableBorderDxfId="6" totalsRowBorderDxfId="4">
-  <autoFilter ref="A1:C8"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:C9" totalsRowShown="0" headerRowDxfId="6" headerRowBorderDxfId="5" tableBorderDxfId="4" totalsRowBorderDxfId="3">
+  <autoFilter ref="A1:C9" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="3">
-    <tableColumn id="2" name="Feature" dataDxfId="3"/>
-    <tableColumn id="1" name="ID" dataDxfId="0"/>
-    <tableColumn id="3" name="Requirment" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Feature" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ID" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Requirment" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -700,24 +757,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="86" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="86.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="2" customFormat="1" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" s="2" customFormat="1" ht="19.8" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>0</v>
@@ -725,87 +782,116 @@
       <c r="C1" s="5" t="s">
         <v>1</v>
       </c>
+      <c r="D1" s="13" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>3</v>
+      <c r="D7" s="14" t="s">
+        <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>4</v>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="C7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="C8" s="11" t="s">
-        <v>7</v>
-      </c>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="10"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="11"/>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation allowBlank="1" showDropDown="1" sqref="A5 A7:A8 A2:A3"/>
+    <dataValidation allowBlank="1" showDropDown="1" sqref="A5 A7:A8 A2:A3 D2:D8" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
modifiy registration,navigation and publish CRS after get the comments
</commit_message>
<xml_diff>
--- a/LH_REQUIREMENTS/LH_CRS.xlsx
+++ b/LH_REQUIREMENTS/LH_CRS.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E5921E1-7085-42A9-9B59-CA744F11FE9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12450"/>
   </bookViews>
   <sheets>
     <sheet name="LH_CRS" sheetId="1" r:id="rId1"/>
@@ -70,15 +69,6 @@
     <t>each user must be assigned a unique user ID after creating an account</t>
   </si>
   <si>
-    <t>LH_CRS_REGISTRATION_001</t>
-  </si>
-  <si>
-    <t>LH_CRS_NAVIGATION_002</t>
-  </si>
-  <si>
-    <t>LH_CRS_PUBLISH_003</t>
-  </si>
-  <si>
     <t>Owner</t>
   </si>
   <si>
@@ -101,12 +91,21 @@
   </si>
   <si>
     <t xml:space="preserve">The system should be either web-based or PC-based. </t>
+  </si>
+  <si>
+    <t>LH-CRS-REGISTRATION-001</t>
+  </si>
+  <si>
+    <t>LH-CRS-NAVIGATION-002</t>
+  </si>
+  <si>
+    <t>LH-CRS-PUBLISH-003</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -484,12 +483,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:C9" totalsRowShown="0" headerRowDxfId="6" headerRowBorderDxfId="5" tableBorderDxfId="4" totalsRowBorderDxfId="3">
-  <autoFilter ref="A1:C9" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:C9" totalsRowShown="0" headerRowDxfId="6" headerRowBorderDxfId="5" tableBorderDxfId="4" totalsRowBorderDxfId="3">
+  <autoFilter ref="A1:C9"/>
   <tableColumns count="3">
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Feature" dataDxfId="2"/>
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ID" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Requirment" dataDxfId="0"/>
+    <tableColumn id="2" name="Feature" dataDxfId="2"/>
+    <tableColumn id="1" name="ID" dataDxfId="1"/>
+    <tableColumn id="3" name="Requirment" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -757,22 +756,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="86" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="2" customFormat="1" ht="19.8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" s="2" customFormat="1" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>7</v>
       </c>
@@ -783,115 +782,115 @@
         <v>1</v>
       </c>
       <c r="D1" s="13" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>2</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>3</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>4</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>5</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>13</v>
       </c>
       <c r="B6" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="7" t="s">
-        <v>26</v>
-      </c>
       <c r="D6" s="12" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C7" t="s">
         <v>15</v>
       </c>
       <c r="D7" s="14" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
         <v>12</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C8" s="11" t="s">
         <v>6</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="10"/>
       <c r="B9" s="15"/>
       <c r="C9" s="11"/>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation allowBlank="1" showDropDown="1" sqref="A5 A7:A8 A2:A3 D2:D8" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
+    <dataValidation allowBlank="1" showDropDown="1" sqref="A5 A7:A8 A2:A3 D2:D8"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
v1.4 CRS for registration, navigation and publish after SIQ
add more requirements for registration, navigation and publish depend on SIQ
</commit_message>
<xml_diff>
--- a/LH_REQUIREMENTS/LH_CRS.xlsx
+++ b/LH_REQUIREMENTS/LH_CRS.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12450"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12450" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="LH_CRS" sheetId="1" r:id="rId1"/>
+    <sheet name="LH_CRS_VERSION_HISTORY" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="61">
   <si>
     <t>ID</t>
   </si>
@@ -100,13 +101,115 @@
   </si>
   <si>
     <t>LH-CRS-PUBLISH-003</t>
+  </si>
+  <si>
+    <t>The password must be at least 8 characters long.</t>
+  </si>
+  <si>
+    <t>The password must include a combination of numbers, characters, and special characters.</t>
+  </si>
+  <si>
+    <t>The system must display a message showing password requirements to the user.</t>
+  </si>
+  <si>
+    <t>The system must show an indicator if a username is already used.</t>
+  </si>
+  <si>
+    <t>The system must show an indicator if an email is already used.</t>
+  </si>
+  <si>
+    <t>The website must include a header navigation bar with tabs for each section and dropdowns for subsections.</t>
+  </si>
+  <si>
+    <t>The maximum allowed audio recording upload size must be 20 MB.</t>
+  </si>
+  <si>
+    <t>The maximum number of words in an article must be 1000 words.</t>
+  </si>
+  <si>
+    <t>The accepted video format must be MP4.</t>
+  </si>
+  <si>
+    <t>The accepted audio format must be MP3.</t>
+  </si>
+  <si>
+    <t>LH-CRS-REGISTRATION-002</t>
+  </si>
+  <si>
+    <t>LH-CRS-REGISTRATION-003</t>
+  </si>
+  <si>
+    <t>LH-CRS-REGISTRATION-004</t>
+  </si>
+  <si>
+    <t>LH-CRS-REGISTRATION-005</t>
+  </si>
+  <si>
+    <t>LH-CRS-REGISTRATION-006</t>
+  </si>
+  <si>
+    <t>LH-CRS-NAVIGATION-001</t>
+  </si>
+  <si>
+    <t>LH-CRS-NAVIGATION-003</t>
+  </si>
+  <si>
+    <t>LH-CRS-PUBLISH-001</t>
+  </si>
+  <si>
+    <t>LH-CRS-PUBLISH-002</t>
+  </si>
+  <si>
+    <t>LH-CRS-PUBLISH-004</t>
+  </si>
+  <si>
+    <t>LH-CRS-PUBLISH-005</t>
+  </si>
+  <si>
+    <t>LH-CRS-PUBLISH-006</t>
+  </si>
+  <si>
+    <t>The website must include exactly 4 content categories.</t>
+  </si>
+  <si>
+    <t>The maximum allowed video upload size must be 100 MB.</t>
+  </si>
+  <si>
+    <t>Version number</t>
+  </si>
+  <si>
+    <t>Author</t>
+  </si>
+  <si>
+    <t>Updated section</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>create intial CRS for registration,navigation and publich</t>
+  </si>
+  <si>
+    <t>v1.0</t>
+  </si>
+  <si>
+    <t>v1.1</t>
+  </si>
+  <si>
+    <t>Adding Notifications, System Constrain, ID Constrain, ADMIN Constrain CRS</t>
+  </si>
+  <si>
+    <t>v1.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CRS for registration,navigation and publich after SIQ assumption </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -131,13 +234,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="15"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -145,22 +241,46 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="15"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
       <b/>
       <sz val="15"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="0"/>
+      <name val="Roboto"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="0"/>
+      <name val="Roboto"/>
+    </font>
+    <font>
+      <sz val="16"/>
       <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -169,18 +289,30 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor theme="4"/>
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor theme="4" tint="0.79998168889431442"/>
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF6F8F9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -204,7 +336,9 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -218,10 +352,10 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -231,41 +365,6 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -279,9 +378,7 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
+      <right/>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -292,184 +389,96 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </top>
-      <bottom style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="4" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -480,18 +489,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:C9" totalsRowShown="0" headerRowDxfId="6" headerRowBorderDxfId="5" tableBorderDxfId="4" totalsRowBorderDxfId="3">
-  <autoFilter ref="A1:C9"/>
-  <tableColumns count="3">
-    <tableColumn id="2" name="Feature" dataDxfId="2"/>
-    <tableColumn id="1" name="ID" dataDxfId="1"/>
-    <tableColumn id="3" name="Requirment" dataDxfId="0"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -757,145 +754,362 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="32.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="86" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="99.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="2" customFormat="1" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:4" s="2" customFormat="1" ht="19.5">
+      <c r="A1" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="27" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:4">
+      <c r="A2" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="12" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="D2" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="21"/>
+      <c r="B3" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="21"/>
+      <c r="B4" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="21"/>
+      <c r="B5" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="21"/>
+      <c r="B6" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="22"/>
+      <c r="B7" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B8" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="24"/>
+      <c r="B9" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="C9" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="25"/>
+      <c r="B10" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B11" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="C11" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="21"/>
+      <c r="B12" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="21"/>
+      <c r="B13" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="12" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="C13" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="21"/>
+      <c r="B14" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="21"/>
+      <c r="B15" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="C15" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="22"/>
+      <c r="B16" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="C16" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B17" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C17" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D17" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
+    <row r="18" spans="1:4">
+      <c r="A18" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B18" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C18" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="D18" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+    <row r="19" spans="1:4">
+      <c r="A19" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B19" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C19" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="14" t="s">
+      <c r="D19" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="10" t="s">
+    <row r="20" spans="1:4">
+      <c r="A20" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B20" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C20" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="12" t="s">
+      <c r="D20" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="10"/>
-      <c r="B9" s="15"/>
-      <c r="C9" s="11"/>
-    </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A2:A7"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="A11:A16"/>
+  </mergeCells>
   <dataValidations count="1">
-    <dataValidation allowBlank="1" showDropDown="1" sqref="A5 A7:A8 A2:A3 D2:D8"/>
+    <dataValidation allowBlank="1" showDropDown="1" sqref="A17 A19:A20 D17:D20 D2 D8 D11 A2 A8"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <tableParts count="1">
-    <tablePart r:id="rId2"/>
-  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="15.42578125" customWidth="1"/>
+    <col min="2" max="2" width="22.7109375" customWidth="1"/>
+    <col min="3" max="3" width="54.7109375" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="32" customFormat="1" ht="40.5">
+      <c r="A1" s="30" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" s="30" t="s">
+        <v>52</v>
+      </c>
+      <c r="C1" s="31" t="s">
+        <v>53</v>
+      </c>
+      <c r="D1" s="30" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="37.5">
+      <c r="A2" s="28" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="D2" s="7">
+        <v>45754</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="37.5">
+      <c r="A3" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="D3" s="9">
+        <v>45754</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="37.5">
+      <c r="A4" s="28" t="s">
+        <v>59</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="D4" s="9">
+        <v>45759</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
v1.5 CRS for login after SIQ
CRS for login and adjust admin constrains, and notifications according to SIQ assumption
</commit_message>
<xml_diff>
--- a/LH_REQUIREMENTS/LH_CRS.xlsx
+++ b/LH_REQUIREMENTS/LH_CRS.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CB3DA8F-7C06-4E0E-BA94-5C4059231471}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12450" activeTab="1"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LH_CRS" sheetId="1" r:id="rId1"/>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="76">
   <si>
     <t>ID</t>
   </si>
@@ -40,9 +41,6 @@
     <t>users can follow specific categories to receive notifications when new content is added</t>
   </si>
   <si>
-    <t>admin features must be available for content and user management</t>
-  </si>
-  <si>
     <t>Feature</t>
   </si>
   <si>
@@ -79,18 +77,6 @@
     <t>Omar Sherif</t>
   </si>
   <si>
-    <t>LH-CRS-NOTIFICATIONS-004</t>
-  </si>
-  <si>
-    <t>LH-CRS-SYSTEM-CONSTRAINS-005</t>
-  </si>
-  <si>
-    <t>LH-CRS-ID-CONSTRAINS-006</t>
-  </si>
-  <si>
-    <t>LH-CRS-ADMIN-CONSTRAINS-007</t>
-  </si>
-  <si>
     <t xml:space="preserve">The system should be either web-based or PC-based. </t>
   </si>
   <si>
@@ -199,17 +185,77 @@
     <t>Adding Notifications, System Constrain, ID Constrain, ADMIN Constrain CRS</t>
   </si>
   <si>
-    <t>v1.2</t>
-  </si>
-  <si>
     <t xml:space="preserve">CRS for registration,navigation and publich after SIQ assumption </t>
+  </si>
+  <si>
+    <t>v1.4</t>
+  </si>
+  <si>
+    <t>LH-CRS-NOTIFICATIONS-001</t>
+  </si>
+  <si>
+    <t>LH-CRS-SYSTEM-CONSTRAINS-001</t>
+  </si>
+  <si>
+    <t>LH-CRS-ID-CONSTRAINS-001</t>
+  </si>
+  <si>
+    <t>LH-CRS-ADMIN-CONSTRAINS-001</t>
+  </si>
+  <si>
+    <t>LH-CRS-NOTIFICATIONS-002</t>
+  </si>
+  <si>
+    <t>The website must provide a notification system for users.</t>
+  </si>
+  <si>
+    <t>Admin features must include the ability to remove articles, videos, and audio files.</t>
+  </si>
+  <si>
+    <t>LH-CRS-ADMIN-CONSTRAINS-002</t>
+  </si>
+  <si>
+    <t>Admin features must include the ability to delete users.</t>
+  </si>
+  <si>
+    <t>Login</t>
+  </si>
+  <si>
+    <t>LH-CRS-LOGIN-001</t>
+  </si>
+  <si>
+    <t>LH-CRS-LOGIN-002</t>
+  </si>
+  <si>
+    <t>LH-CRS-LOGIN-003</t>
+  </si>
+  <si>
+    <t>LH-CRS-LOGIN-004</t>
+  </si>
+  <si>
+    <t>Users must log in using their email and password.</t>
+  </si>
+  <si>
+    <t>Store passwords using hashing and salting techniques.</t>
+  </si>
+  <si>
+    <t>Show a generic error message for login failures including incorrect password, empty fields, or unregistered email.</t>
+  </si>
+  <si>
+    <t>Only registered users can log in.</t>
+  </si>
+  <si>
+    <t>v1.5</t>
+  </si>
+  <si>
+    <t>CRS for login and adjust admin constrains, and notifications according to SIQ assumption</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="10">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -279,8 +325,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -311,8 +363,32 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="7">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -335,80 +411,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -421,44 +429,6 @@
     <xf numFmtId="15" fontId="4" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -473,6 +443,48 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -753,283 +765,364 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="99.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.109375" style="31" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.33203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="99.44140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.88671875" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="2" customFormat="1" ht="19.5">
-      <c r="A1" s="26" t="s">
+    <row r="1" spans="1:4" s="18" customFormat="1" ht="19.2" x14ac:dyDescent="0.35">
+      <c r="A1" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="19"/>
+      <c r="B3" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="19"/>
+      <c r="B4" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="19"/>
+      <c r="B5" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="19"/>
+      <c r="B6" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="19"/>
+      <c r="B7" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="26" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="27" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="20" t="s">
+      <c r="B8" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="24"/>
+      <c r="B9" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="24"/>
+      <c r="B10" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="19"/>
+      <c r="B12" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="19"/>
+      <c r="B13" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="19"/>
+      <c r="B14" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="C14" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="19"/>
+      <c r="B15" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="19"/>
+      <c r="B16" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="C16" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D17" s="12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="24"/>
+      <c r="B18" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="C18" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="D18" s="13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="27" t="s">
+        <v>12</v>
+      </c>
+      <c r="B19" s="28" t="s">
+        <v>57</v>
+      </c>
+      <c r="C19" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="D19" s="14" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="B20" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="C20" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="3" t="s">
+      <c r="D20" s="13" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="21"/>
-      <c r="B3" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="C3" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="D3" s="1" t="s">
+    <row r="21" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="B21" s="28" t="s">
+        <v>59</v>
+      </c>
+      <c r="C21" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="D21" s="14" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="21"/>
-      <c r="B4" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="C4" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="D4" s="3" t="s">
+    <row r="22" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="19"/>
+      <c r="B22" s="30" t="s">
+        <v>63</v>
+      </c>
+      <c r="C22" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="D22" s="15" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="21"/>
-      <c r="B5" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="C5" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="D5" s="1" t="s">
+    <row r="23" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="B23" s="28" t="s">
+        <v>66</v>
+      </c>
+      <c r="C23" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="D23" s="14" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="21"/>
-      <c r="B6" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="C6" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="D6" s="3" t="s">
+    <row r="24" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="24"/>
+      <c r="B24" s="30" t="s">
+        <v>67</v>
+      </c>
+      <c r="C24" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="D24" s="15" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="22"/>
-      <c r="B7" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="C7" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="D7" s="1" t="s">
+    <row r="25" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="24"/>
+      <c r="B25" s="28" t="s">
+        <v>68</v>
+      </c>
+      <c r="C25" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="D25" s="14" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
-      <c r="A8" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="C8" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="D8" s="3" t="s">
+    <row r="26" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="24"/>
+      <c r="B26" s="30" t="s">
+        <v>69</v>
+      </c>
+      <c r="C26" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="D26" s="15" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
-      <c r="A9" s="24"/>
-      <c r="B9" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="C9" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="25"/>
-      <c r="B10" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="C10" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="C11" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" s="21"/>
-      <c r="B12" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="C12" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13" s="21"/>
-      <c r="B13" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="C13" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14" s="21"/>
-      <c r="B14" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="C14" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15" s="21"/>
-      <c r="B15" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="C15" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16" s="22"/>
-      <c r="B16" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="C16" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="B17" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="C17" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="B18" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C18" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="B19" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="C19" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
-      <c r="A20" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="B20" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="6">
+    <mergeCell ref="A23:A26"/>
     <mergeCell ref="A2:A7"/>
     <mergeCell ref="A8:A10"/>
     <mergeCell ref="A11:A16"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="A21:A22"/>
   </mergeCells>
+  <phoneticPr fontId="10" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation allowBlank="1" showDropDown="1" sqref="A17 A19:A20 D17:D20 D2 D8 D11 A2 A8"/>
+    <dataValidation allowBlank="1" showDropDown="1" sqref="A17 A8 D2 D8 D11 A2 D17:D26 A20:A21" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1037,78 +1130,93 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" customWidth="1"/>
-    <col min="2" max="2" width="22.7109375" customWidth="1"/>
-    <col min="3" max="3" width="54.7109375" customWidth="1"/>
-    <col min="4" max="4" width="18.7109375" customWidth="1"/>
+    <col min="1" max="1" width="15.44140625" customWidth="1"/>
+    <col min="2" max="2" width="22.6640625" customWidth="1"/>
+    <col min="3" max="3" width="54.6640625" customWidth="1"/>
+    <col min="4" max="4" width="18.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="32" customFormat="1" ht="40.5">
-      <c r="A1" s="30" t="s">
+    <row r="1" spans="1:4" s="9" customFormat="1" ht="42" x14ac:dyDescent="0.4">
+      <c r="A1" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="37.200000000000003" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="B1" s="30" t="s">
+      <c r="B2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D2" s="2">
+        <v>45754</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="37.200000000000003" x14ac:dyDescent="0.3">
+      <c r="A3" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="C1" s="31" t="s">
+      <c r="B3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="D1" s="30" t="s">
+      <c r="D3" s="4">
+        <v>45754</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="37.200000000000003" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="37.5">
-      <c r="A2" s="28" t="s">
-        <v>56</v>
-      </c>
-      <c r="B2" s="6" t="s">
+      <c r="D4" s="4">
+        <v>45759</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="55.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="D2" s="7">
-        <v>45754</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="37.5">
-      <c r="A3" s="29" t="s">
-        <v>57</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="D3" s="9">
-        <v>45754</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="37.5">
-      <c r="A4" s="28" t="s">
-        <v>59</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="D4" s="9">
+      <c r="C5" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D5" s="4">
         <v>45759</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
v1.6 Adding more CRSs depends on last SIQ version
Adding more CRSs for registration and ID constrains depends on last SIQ version
</commit_message>
<xml_diff>
--- a/LH_REQUIREMENTS/LH_CRS.xlsx
+++ b/LH_REQUIREMENTS/LH_CRS.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CB3DA8F-7C06-4E0E-BA94-5C4059231471}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12450" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="LH_CRS" sheetId="1" r:id="rId1"/>
@@ -21,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="86">
   <si>
     <t>ID</t>
   </si>
@@ -249,13 +248,43 @@
   </si>
   <si>
     <t>CRS for login and adjust admin constrains, and notifications according to SIQ assumption</t>
+  </si>
+  <si>
+    <t>the registration form require all fields (email, username, and password) to be filled out?</t>
+  </si>
+  <si>
+    <t>LH-CRS-REGISTRATION-007</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> the username have specific constraints</t>
+  </si>
+  <si>
+    <t>m prevent multiple registrations using the same email or username</t>
+  </si>
+  <si>
+    <t>the system automatically assign user IDs in a simple, consistent format (e.g., U001, U002)</t>
+  </si>
+  <si>
+    <t>LH-CRS-REGISTRATION-008</t>
+  </si>
+  <si>
+    <t>LH-CRS-REGISTRATION-009</t>
+  </si>
+  <si>
+    <t>LH-CRS-ID-CONSTRAINS-002</t>
+  </si>
+  <si>
+    <t>v1.6</t>
+  </si>
+  <si>
+    <t>Adding more CRSs for registration and ID constrains depends on last SIQ version</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -388,7 +417,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -411,11 +440,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -459,9 +525,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -470,20 +533,37 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -765,23 +845,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D26"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.109375" style="31" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.33203125" style="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="99.44140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.109375" style="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.88671875" style="11"/>
+    <col min="1" max="1" width="18.140625" style="28" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.28515625" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="104" style="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.85546875" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="18" customFormat="1" ht="19.2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" s="18" customFormat="1" ht="19.5">
       <c r="A1" s="16" t="s">
         <v>6</v>
       </c>
@@ -795,11 +875,11 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="19" t="s">
+    <row r="2" spans="1:4">
+      <c r="A2" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="19" t="s">
         <v>19</v>
       </c>
       <c r="C2" s="10" t="s">
@@ -809,57 +889,57 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="19"/>
-      <c r="B3" s="21" t="s">
+    <row r="3" spans="1:4">
+      <c r="A3" s="32"/>
+      <c r="B3" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="21" t="s">
         <v>22</v>
       </c>
       <c r="D3" s="11" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="19"/>
-      <c r="B4" s="20" t="s">
+    <row r="4" spans="1:4">
+      <c r="A4" s="32"/>
+      <c r="B4" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="C4" s="23" t="s">
+      <c r="C4" s="22" t="s">
         <v>23</v>
       </c>
       <c r="D4" s="10" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="19"/>
-      <c r="B5" s="21" t="s">
+    <row r="5" spans="1:4">
+      <c r="A5" s="32"/>
+      <c r="B5" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="C5" s="22" t="s">
+      <c r="C5" s="21" t="s">
         <v>24</v>
       </c>
       <c r="D5" s="11" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="19"/>
-      <c r="B6" s="20" t="s">
+    <row r="6" spans="1:4">
+      <c r="A6" s="32"/>
+      <c r="B6" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="C6" s="23" t="s">
+      <c r="C6" s="22" t="s">
         <v>25</v>
       </c>
       <c r="D6" s="10" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="19"/>
-      <c r="B7" s="21" t="s">
+    <row r="7" spans="1:4">
+      <c r="A7" s="32"/>
+      <c r="B7" s="20" t="s">
         <v>36</v>
       </c>
       <c r="C7" s="11" t="s">
@@ -869,260 +949,309 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="24" t="s">
+    <row r="8" spans="1:4">
+      <c r="A8" s="32"/>
+      <c r="B8" s="19" t="s">
+        <v>77</v>
+      </c>
+      <c r="C8" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="32"/>
+      <c r="B9" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="33"/>
+      <c r="B10" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="C10" s="22" t="s">
+        <v>79</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="20" t="s">
+      <c r="B11" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C11" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="10" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="24"/>
-      <c r="B9" s="21" t="s">
+      <c r="D11" s="10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="29"/>
+      <c r="B12" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="22" t="s">
+      <c r="C12" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="D9" s="11" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="24"/>
-      <c r="B10" s="20" t="s">
+      <c r="D12" s="11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="29"/>
+      <c r="B13" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="C13" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="D10" s="10" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="19" t="s">
+      <c r="D13" s="10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="21" t="s">
+      <c r="B14" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="C14" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D11" s="11" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="19"/>
-      <c r="B12" s="20" t="s">
+      <c r="D14" s="11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="30"/>
+      <c r="B15" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="C12" s="23" t="s">
+      <c r="C15" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="D12" s="10" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="19"/>
-      <c r="B13" s="21" t="s">
+      <c r="D15" s="10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="30"/>
+      <c r="B16" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="C13" s="11" t="s">
+      <c r="C16" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="D13" s="11" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="19"/>
-      <c r="B14" s="20" t="s">
+      <c r="D16" s="11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="30"/>
+      <c r="B17" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="C14" s="23" t="s">
+      <c r="C17" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="D14" s="10" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="19"/>
-      <c r="B15" s="21" t="s">
+      <c r="D17" s="10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="30"/>
+      <c r="B18" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="C15" s="11" t="s">
+      <c r="C18" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="D15" s="11" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" s="19"/>
-      <c r="B16" s="20" t="s">
+      <c r="D18" s="11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="30"/>
+      <c r="B19" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="C16" s="23" t="s">
+      <c r="C19" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="D16" s="10" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="24" t="s">
+      <c r="D19" s="10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" s="12" customFormat="1">
+      <c r="A20" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="B17" s="25" t="s">
+      <c r="B20" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="C17" s="12" t="s">
+      <c r="C20" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="D17" s="12" t="s">
+      <c r="D20" s="12" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="24"/>
-      <c r="B18" s="26" t="s">
+    <row r="21" spans="1:4" s="13" customFormat="1">
+      <c r="A21" s="29"/>
+      <c r="B21" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="C18" s="13" t="s">
+      <c r="C21" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="D18" s="13" t="s">
+      <c r="D21" s="13" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="27" t="s">
+    <row r="22" spans="1:4" s="12" customFormat="1">
+      <c r="A22" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="28" t="s">
+      <c r="B22" s="26" t="s">
         <v>57</v>
       </c>
-      <c r="C19" s="14" t="s">
+      <c r="C22" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="D19" s="14" t="s">
+      <c r="D22" s="14" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="29" t="s">
+    <row r="23" spans="1:4" s="13" customFormat="1">
+      <c r="A23" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="B20" s="26" t="s">
+      <c r="B23" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="C20" s="13" t="s">
+      <c r="C23" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="D20" s="13" t="s">
+      <c r="D23" s="13" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="19" t="s">
+    <row r="24" spans="1:4" s="13" customFormat="1">
+      <c r="A24" s="37"/>
+      <c r="B24" s="34" t="s">
+        <v>83</v>
+      </c>
+      <c r="C24" s="35" t="s">
+        <v>80</v>
+      </c>
+      <c r="D24" s="35" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" s="12" customFormat="1">
+      <c r="A25" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="B21" s="28" t="s">
+      <c r="B25" s="26" t="s">
         <v>59</v>
       </c>
-      <c r="C21" s="14" t="s">
+      <c r="C25" s="14" t="s">
         <v>62</v>
-      </c>
-      <c r="D21" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="19"/>
-      <c r="B22" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="C22" s="15" t="s">
-        <v>64</v>
-      </c>
-      <c r="D22" s="15" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="24" t="s">
-        <v>65</v>
-      </c>
-      <c r="B23" s="28" t="s">
-        <v>66</v>
-      </c>
-      <c r="C23" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="D23" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="24"/>
-      <c r="B24" s="30" t="s">
-        <v>67</v>
-      </c>
-      <c r="C24" s="13" t="s">
-        <v>73</v>
-      </c>
-      <c r="D24" s="15" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="24"/>
-      <c r="B25" s="28" t="s">
-        <v>68</v>
-      </c>
-      <c r="C25" s="12" t="s">
-        <v>72</v>
       </c>
       <c r="D25" s="14" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="26" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="24"/>
-      <c r="B26" s="30" t="s">
-        <v>69</v>
+    <row r="26" spans="1:4" s="13" customFormat="1">
+      <c r="A26" s="30"/>
+      <c r="B26" s="27" t="s">
+        <v>63</v>
       </c>
       <c r="C26" s="15" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="D26" s="15" t="s">
         <v>17</v>
       </c>
     </row>
+    <row r="27" spans="1:4" s="12" customFormat="1">
+      <c r="A27" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="B27" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="C27" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="D27" s="14" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" s="13" customFormat="1">
+      <c r="A28" s="29"/>
+      <c r="B28" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="C28" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="D28" s="15" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" s="12" customFormat="1">
+      <c r="A29" s="29"/>
+      <c r="B29" s="26" t="s">
+        <v>68</v>
+      </c>
+      <c r="C29" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="D29" s="14" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" s="13" customFormat="1">
+      <c r="A30" s="29"/>
+      <c r="B30" s="27" t="s">
+        <v>69</v>
+      </c>
+      <c r="C30" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="D30" s="15" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="A23:A26"/>
-    <mergeCell ref="A2:A7"/>
-    <mergeCell ref="A8:A10"/>
-    <mergeCell ref="A11:A16"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="A21:A22"/>
+  <mergeCells count="7">
+    <mergeCell ref="A27:A30"/>
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="A14:A19"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="A2:A10"/>
+    <mergeCell ref="A23:A24"/>
   </mergeCells>
   <phoneticPr fontId="10" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation allowBlank="1" showDropDown="1" sqref="A17 A8 D2 D8 D11 A2 D17:D26 A20:A21" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
+    <dataValidation allowBlank="1" showDropDown="1" sqref="A20 A11 D2 D11 D14 A2 D20:D30 A23 A25"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1130,22 +1259,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15.44140625" customWidth="1"/>
-    <col min="2" max="2" width="22.6640625" customWidth="1"/>
-    <col min="3" max="3" width="54.6640625" customWidth="1"/>
-    <col min="4" max="4" width="18.6640625" customWidth="1"/>
+    <col min="1" max="1" width="15.42578125" customWidth="1"/>
+    <col min="2" max="2" width="22.7109375" customWidth="1"/>
+    <col min="3" max="3" width="62.140625" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="9" customFormat="1" ht="42" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4" s="9" customFormat="1" ht="40.5">
       <c r="A1" s="7" t="s">
         <v>46</v>
       </c>
@@ -1159,7 +1288,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="37.200000000000003" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="37.5">
       <c r="A2" s="5" t="s">
         <v>51</v>
       </c>
@@ -1173,7 +1302,7 @@
         <v>45754</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="37.200000000000003" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="37.5">
       <c r="A3" s="6" t="s">
         <v>52</v>
       </c>
@@ -1187,7 +1316,7 @@
         <v>45754</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="37.200000000000003" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="37.5">
       <c r="A4" s="5" t="s">
         <v>55</v>
       </c>
@@ -1201,7 +1330,7 @@
         <v>45759</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="55.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="37.5">
       <c r="A5" s="5" t="s">
         <v>74</v>
       </c>
@@ -1213,6 +1342,20 @@
       </c>
       <c r="D5" s="4">
         <v>45759</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="37.5">
+      <c r="A6" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D6" s="4">
+        <v>45765</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
v1.7 modify some CRSs
modify system constrains CRSs because there was a misunderstanding of the main concept
</commit_message>
<xml_diff>
--- a/LH_REQUIREMENTS/LH_CRS.xlsx
+++ b/LH_REQUIREMENTS/LH_CRS.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="88">
   <si>
     <t>ID</t>
   </si>
@@ -76,9 +76,6 @@
     <t>Omar Sherif</t>
   </si>
   <si>
-    <t xml:space="preserve">The system should be either web-based or PC-based. </t>
-  </si>
-  <si>
     <t>LH-CRS-REGISTRATION-001</t>
   </si>
   <si>
@@ -278,6 +275,15 @@
   </si>
   <si>
     <t>Adding more CRSs for registration and ID constrains depends on last SIQ version</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The system will be web-based application based on PC-based. </t>
+  </si>
+  <si>
+    <t>v1.7</t>
+  </si>
+  <si>
+    <t>modify system constrains CRSs</t>
   </si>
 </sst>
 </file>
@@ -543,27 +549,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -848,8 +854,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -880,7 +886,7 @@
         <v>13</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C2" s="10" t="s">
         <v>2</v>
@@ -892,10 +898,10 @@
     <row r="3" spans="1:4">
       <c r="A3" s="32"/>
       <c r="B3" s="20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C3" s="21" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D3" s="11" t="s">
         <v>16</v>
@@ -904,10 +910,10 @@
     <row r="4" spans="1:4">
       <c r="A4" s="32"/>
       <c r="B4" s="19" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C4" s="22" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D4" s="10" t="s">
         <v>16</v>
@@ -916,10 +922,10 @@
     <row r="5" spans="1:4">
       <c r="A5" s="32"/>
       <c r="B5" s="20" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C5" s="21" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D5" s="11" t="s">
         <v>16</v>
@@ -928,10 +934,10 @@
     <row r="6" spans="1:4">
       <c r="A6" s="32"/>
       <c r="B6" s="19" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C6" s="22" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D6" s="10" t="s">
         <v>16</v>
@@ -940,10 +946,10 @@
     <row r="7" spans="1:4">
       <c r="A7" s="32"/>
       <c r="B7" s="20" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D7" s="11" t="s">
         <v>16</v>
@@ -952,10 +958,10 @@
     <row r="8" spans="1:4">
       <c r="A8" s="32"/>
       <c r="B8" s="19" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C8" s="22" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D8" s="10" t="s">
         <v>16</v>
@@ -964,10 +970,10 @@
     <row r="9" spans="1:4">
       <c r="A9" s="32"/>
       <c r="B9" s="20" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D9" s="11" t="s">
         <v>16</v>
@@ -976,21 +982,21 @@
     <row r="10" spans="1:4">
       <c r="A10" s="33"/>
       <c r="B10" s="19" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C10" s="22" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D10" s="10" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11" s="29" t="s">
+      <c r="A11" s="36" t="s">
         <v>7</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C11" s="10" t="s">
         <v>3</v>
@@ -1000,35 +1006,35 @@
       </c>
     </row>
     <row r="12" spans="1:4">
-      <c r="A12" s="29"/>
+      <c r="A12" s="36"/>
       <c r="B12" s="20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C12" s="21" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D12" s="11" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:4">
-      <c r="A13" s="29"/>
+      <c r="A13" s="36"/>
       <c r="B13" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="37" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" s="20" t="s">
         <v>38</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="D13" s="10" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14" s="30" t="s">
-        <v>8</v>
-      </c>
-      <c r="B14" s="20" t="s">
-        <v>39</v>
       </c>
       <c r="C14" s="11" t="s">
         <v>4</v>
@@ -1038,71 +1044,71 @@
       </c>
     </row>
     <row r="15" spans="1:4">
-      <c r="A15" s="30"/>
+      <c r="A15" s="37"/>
       <c r="B15" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="C15" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="37"/>
+      <c r="B16" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="37"/>
+      <c r="B17" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="C15" s="22" t="s">
-        <v>45</v>
-      </c>
-      <c r="D15" s="10" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16" s="30"/>
-      <c r="B16" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="C16" s="11" t="s">
+      <c r="C17" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="D16" s="11" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17" s="30"/>
-      <c r="B17" s="19" t="s">
+      <c r="D17" s="10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="37"/>
+      <c r="B18" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="C17" s="22" t="s">
+      <c r="C18" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="D17" s="10" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18" s="30"/>
-      <c r="B18" s="20" t="s">
+      <c r="D18" s="11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="37"/>
+      <c r="B19" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="C18" s="11" t="s">
+      <c r="C19" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="D18" s="11" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19" s="30"/>
-      <c r="B19" s="19" t="s">
-        <v>43</v>
-      </c>
-      <c r="C19" s="22" t="s">
-        <v>31</v>
-      </c>
       <c r="D19" s="10" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="20" spans="1:4" s="12" customFormat="1">
-      <c r="A20" s="29" t="s">
+      <c r="A20" s="36" t="s">
         <v>9</v>
       </c>
       <c r="B20" s="23" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C20" s="12" t="s">
         <v>5</v>
@@ -1112,12 +1118,12 @@
       </c>
     </row>
     <row r="21" spans="1:4" s="13" customFormat="1">
-      <c r="A21" s="29"/>
+      <c r="A21" s="36"/>
       <c r="B21" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="C21" s="13" t="s">
         <v>60</v>
-      </c>
-      <c r="C21" s="13" t="s">
-        <v>61</v>
       </c>
       <c r="D21" s="13" t="s">
         <v>17</v>
@@ -1128,21 +1134,21 @@
         <v>12</v>
       </c>
       <c r="B22" s="26" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>18</v>
+        <v>85</v>
       </c>
       <c r="D22" s="14" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="23" spans="1:4" s="13" customFormat="1">
-      <c r="A23" s="36" t="s">
+      <c r="A23" s="34" t="s">
         <v>10</v>
       </c>
       <c r="B23" s="24" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C23" s="13" t="s">
         <v>14</v>
@@ -1152,88 +1158,88 @@
       </c>
     </row>
     <row r="24" spans="1:4" s="13" customFormat="1">
-      <c r="A24" s="37"/>
-      <c r="B24" s="34" t="s">
-        <v>83</v>
-      </c>
-      <c r="C24" s="35" t="s">
-        <v>80</v>
-      </c>
-      <c r="D24" s="35" t="s">
+      <c r="A24" s="35"/>
+      <c r="B24" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="C24" s="30" t="s">
+        <v>79</v>
+      </c>
+      <c r="D24" s="30" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="25" spans="1:4" s="12" customFormat="1">
-      <c r="A25" s="30" t="s">
+      <c r="A25" s="37" t="s">
         <v>11</v>
       </c>
       <c r="B25" s="26" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D25" s="14" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="26" spans="1:4" s="13" customFormat="1">
-      <c r="A26" s="30"/>
+      <c r="A26" s="37"/>
       <c r="B26" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="C26" s="15" t="s">
         <v>63</v>
-      </c>
-      <c r="C26" s="15" t="s">
-        <v>64</v>
       </c>
       <c r="D26" s="15" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="27" spans="1:4" s="12" customFormat="1">
-      <c r="A27" s="29" t="s">
+      <c r="A27" s="36" t="s">
+        <v>64</v>
+      </c>
+      <c r="B27" s="26" t="s">
         <v>65</v>
       </c>
-      <c r="B27" s="26" t="s">
-        <v>66</v>
-      </c>
       <c r="C27" s="14" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D27" s="14" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="28" spans="1:4" s="13" customFormat="1">
-      <c r="A28" s="29"/>
+      <c r="A28" s="36"/>
       <c r="B28" s="27" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C28" s="13" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D28" s="15" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="29" spans="1:4" s="12" customFormat="1">
-      <c r="A29" s="29"/>
+      <c r="A29" s="36"/>
       <c r="B29" s="26" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C29" s="12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D29" s="14" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="30" spans="1:4" s="13" customFormat="1">
-      <c r="A30" s="29"/>
+      <c r="A30" s="36"/>
       <c r="B30" s="27" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C30" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D30" s="15" t="s">
         <v>17</v>
@@ -1241,13 +1247,13 @@
     </row>
   </sheetData>
   <mergeCells count="7">
+    <mergeCell ref="A2:A10"/>
+    <mergeCell ref="A23:A24"/>
     <mergeCell ref="A27:A30"/>
     <mergeCell ref="A11:A13"/>
     <mergeCell ref="A14:A19"/>
     <mergeCell ref="A20:A21"/>
     <mergeCell ref="A25:A26"/>
-    <mergeCell ref="A2:A10"/>
-    <mergeCell ref="A23:A24"/>
   </mergeCells>
   <phoneticPr fontId="10" type="noConversion"/>
   <dataValidations count="1">
@@ -1260,10 +1266,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1276,27 +1282,27 @@
   <sheetData>
     <row r="1" spans="1:4" s="9" customFormat="1" ht="40.5">
       <c r="A1" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="C1" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="D1" s="7" t="s">
         <v>48</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="37.5">
       <c r="A2" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D2" s="2">
         <v>45754</v>
@@ -1304,13 +1310,13 @@
     </row>
     <row r="3" spans="1:4" ht="37.5">
       <c r="A3" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D3" s="4">
         <v>45754</v>
@@ -1318,13 +1324,13 @@
     </row>
     <row r="4" spans="1:4" ht="37.5">
       <c r="A4" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D4" s="4">
         <v>45759</v>
@@ -1332,13 +1338,13 @@
     </row>
     <row r="5" spans="1:4" ht="37.5">
       <c r="A5" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D5" s="4">
         <v>45759</v>
@@ -1346,16 +1352,30 @@
     </row>
     <row r="6" spans="1:4" ht="37.5">
       <c r="A6" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>84</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>85</v>
       </c>
       <c r="D6" s="4">
         <v>45765</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="18.75">
+      <c r="A7" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D7" s="4">
+        <v>45766</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
v1.8 Modify Notification CRSs after Review
</commit_message>
<xml_diff>
--- a/LH_REQUIREMENTS/LH_CRS.xlsx
+++ b/LH_REQUIREMENTS/LH_CRS.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98444024-1314-495F-8A0F-3BDD8DC712AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12450" activeTab="1"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LH_CRS" sheetId="1" r:id="rId1"/>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="90">
   <si>
     <t>ID</t>
   </si>
@@ -202,9 +203,6 @@
     <t>LH-CRS-NOTIFICATIONS-002</t>
   </si>
   <si>
-    <t>The website must provide a notification system for users.</t>
-  </si>
-  <si>
     <t>Admin features must include the ability to remove articles, videos, and audio files.</t>
   </si>
   <si>
@@ -284,13 +282,22 @@
   </si>
   <si>
     <t>modify system constrains CRSs</t>
+  </si>
+  <si>
+    <t>The system must notify users within the website interface when new content is added to a followed category.</t>
+  </si>
+  <si>
+    <t>v1.8</t>
+  </si>
+  <si>
+    <t>modify Notification CRSs after Review</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="11">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -487,7 +494,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -516,12 +523,12 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -531,26 +538,24 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -851,23 +856,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.140625" style="28" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.28515625" style="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.109375" style="28" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.33203125" style="11" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="104" style="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.85546875" style="11"/>
+    <col min="4" max="4" width="18.109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.88671875" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="18" customFormat="1" ht="19.5">
+    <row r="1" spans="1:4" s="18" customFormat="1" ht="19.2" x14ac:dyDescent="0.35">
       <c r="A1" s="16" t="s">
         <v>6</v>
       </c>
@@ -881,8 +886,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="31" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="29" t="s">
         <v>13</v>
       </c>
       <c r="B2" s="19" t="s">
@@ -895,8 +900,8 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="32"/>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="30"/>
       <c r="B3" s="20" t="s">
         <v>31</v>
       </c>
@@ -907,8 +912,8 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="32"/>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="30"/>
       <c r="B4" s="19" t="s">
         <v>32</v>
       </c>
@@ -919,8 +924,8 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="32"/>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="30"/>
       <c r="B5" s="20" t="s">
         <v>33</v>
       </c>
@@ -931,8 +936,8 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="32"/>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="30"/>
       <c r="B6" s="19" t="s">
         <v>34</v>
       </c>
@@ -943,8 +948,8 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="32"/>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="30"/>
       <c r="B7" s="20" t="s">
         <v>35</v>
       </c>
@@ -955,44 +960,44 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
-      <c r="A8" s="32"/>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="30"/>
       <c r="B8" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="C8" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="30"/>
+      <c r="B9" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="C9" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="C8" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="D8" s="10" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" s="32"/>
-      <c r="B9" s="20" t="s">
+      <c r="D9" s="11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="31"/>
+      <c r="B10" s="19" t="s">
         <v>80</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C10" s="22" t="s">
         <v>77</v>
       </c>
-      <c r="D9" s="11" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="33"/>
-      <c r="B10" s="19" t="s">
-        <v>81</v>
-      </c>
-      <c r="C10" s="22" t="s">
-        <v>78</v>
-      </c>
       <c r="D10" s="10" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
-      <c r="A11" s="36" t="s">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="34" t="s">
         <v>7</v>
       </c>
       <c r="B11" s="19" t="s">
@@ -1005,8 +1010,8 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
-      <c r="A12" s="36"/>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="34"/>
       <c r="B12" s="20" t="s">
         <v>19</v>
       </c>
@@ -1017,8 +1022,8 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
-      <c r="A13" s="36"/>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="34"/>
       <c r="B13" s="19" t="s">
         <v>37</v>
       </c>
@@ -1029,8 +1034,8 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
-      <c r="A14" s="37" t="s">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="35" t="s">
         <v>8</v>
       </c>
       <c r="B14" s="20" t="s">
@@ -1043,8 +1048,8 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
-      <c r="A15" s="37"/>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="35"/>
       <c r="B15" s="19" t="s">
         <v>39</v>
       </c>
@@ -1055,8 +1060,8 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
-      <c r="A16" s="37"/>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="35"/>
       <c r="B16" s="20" t="s">
         <v>20</v>
       </c>
@@ -1067,8 +1072,8 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
-      <c r="A17" s="37"/>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="35"/>
       <c r="B17" s="19" t="s">
         <v>40</v>
       </c>
@@ -1079,8 +1084,8 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
-      <c r="A18" s="37"/>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="35"/>
       <c r="B18" s="20" t="s">
         <v>41</v>
       </c>
@@ -1091,8 +1096,8 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
-      <c r="A19" s="37"/>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="35"/>
       <c r="B19" s="19" t="s">
         <v>42</v>
       </c>
@@ -1103,8 +1108,8 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:4" s="12" customFormat="1">
-      <c r="A20" s="36" t="s">
+    <row r="20" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="34" t="s">
         <v>9</v>
       </c>
       <c r="B20" s="23" t="s">
@@ -1117,19 +1122,19 @@
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:4" s="13" customFormat="1">
-      <c r="A21" s="36"/>
+    <row r="21" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="34"/>
       <c r="B21" s="24" t="s">
         <v>59</v>
       </c>
       <c r="C21" s="13" t="s">
-        <v>60</v>
+        <v>87</v>
       </c>
       <c r="D21" s="13" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="1:4" s="12" customFormat="1">
+    <row r="22" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="25" t="s">
         <v>12</v>
       </c>
@@ -1137,14 +1142,14 @@
         <v>56</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D22" s="14" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="23" spans="1:4" s="13" customFormat="1">
-      <c r="A23" s="34" t="s">
+    <row r="23" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="32" t="s">
         <v>10</v>
       </c>
       <c r="B23" s="24" t="s">
@@ -1157,89 +1162,89 @@
         <v>17</v>
       </c>
     </row>
-    <row r="24" spans="1:4" s="13" customFormat="1">
-      <c r="A24" s="35"/>
-      <c r="B24" s="29" t="s">
-        <v>82</v>
-      </c>
-      <c r="C24" s="30" t="s">
-        <v>79</v>
-      </c>
-      <c r="D24" s="30" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" s="12" customFormat="1">
-      <c r="A25" s="37" t="s">
+    <row r="24" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="33"/>
+      <c r="B24" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="C24" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="D24" s="11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="35" t="s">
         <v>11</v>
       </c>
       <c r="B25" s="26" t="s">
         <v>58</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D25" s="14" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="26" spans="1:4" s="13" customFormat="1">
-      <c r="A26" s="37"/>
+    <row r="26" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="35"/>
       <c r="B26" s="27" t="s">
+        <v>61</v>
+      </c>
+      <c r="C26" s="15" t="s">
         <v>62</v>
-      </c>
-      <c r="C26" s="15" t="s">
-        <v>63</v>
       </c>
       <c r="D26" s="15" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="27" spans="1:4" s="12" customFormat="1">
-      <c r="A27" s="36" t="s">
+    <row r="27" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="34" t="s">
+        <v>63</v>
+      </c>
+      <c r="B27" s="26" t="s">
         <v>64</v>
       </c>
-      <c r="B27" s="26" t="s">
-        <v>65</v>
-      </c>
       <c r="C27" s="14" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D27" s="14" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="28" spans="1:4" s="13" customFormat="1">
-      <c r="A28" s="36"/>
+    <row r="28" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="34"/>
       <c r="B28" s="27" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C28" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D28" s="15" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="29" spans="1:4" s="12" customFormat="1">
-      <c r="A29" s="36"/>
+    <row r="29" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="34"/>
       <c r="B29" s="26" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C29" s="12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D29" s="14" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="30" spans="1:4" s="13" customFormat="1">
-      <c r="A30" s="36"/>
+    <row r="30" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="34"/>
       <c r="B30" s="27" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C30" s="15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D30" s="15" t="s">
         <v>17</v>
@@ -1257,7 +1262,7 @@
   </mergeCells>
   <phoneticPr fontId="10" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation allowBlank="1" showDropDown="1" sqref="A20 A11 D2 D11 D14 A2 D20:D30 A23 A25"/>
+    <dataValidation allowBlank="1" showDropDown="1" sqref="A20 A11 D2 D11 D14 A2 D20:D30 A23 A25" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1265,22 +1270,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" customWidth="1"/>
-    <col min="2" max="2" width="22.7109375" customWidth="1"/>
-    <col min="3" max="3" width="62.140625" customWidth="1"/>
-    <col min="4" max="4" width="18.7109375" customWidth="1"/>
+    <col min="1" max="1" width="15.44140625" customWidth="1"/>
+    <col min="2" max="2" width="22.6640625" customWidth="1"/>
+    <col min="3" max="3" width="62.109375" customWidth="1"/>
+    <col min="4" max="4" width="18.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="9" customFormat="1" ht="40.5">
+    <row r="1" spans="1:4" s="9" customFormat="1" ht="42" x14ac:dyDescent="0.4">
       <c r="A1" s="7" t="s">
         <v>45</v>
       </c>
@@ -1294,7 +1299,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="37.5">
+    <row r="2" spans="1:4" ht="37.200000000000003" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>50</v>
       </c>
@@ -1308,7 +1313,7 @@
         <v>45754</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="37.5">
+    <row r="3" spans="1:4" ht="37.200000000000003" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>51</v>
       </c>
@@ -1322,7 +1327,7 @@
         <v>45754</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="37.5">
+    <row r="4" spans="1:4" ht="37.200000000000003" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>54</v>
       </c>
@@ -1336,46 +1341,60 @@
         <v>45759</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="37.5">
+    <row r="5" spans="1:4" ht="37.200000000000003" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D5" s="4">
         <v>45759</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="37.5">
+    <row r="6" spans="1:4" ht="37.200000000000003" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>83</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>84</v>
       </c>
       <c r="D6" s="4">
         <v>45765</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="18.75">
+    <row r="7" spans="1:4" ht="18.600000000000001" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>86</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>87</v>
       </c>
       <c r="D7" s="4">
         <v>45766</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="18.600000000000001" x14ac:dyDescent="0.3">
+      <c r="A8" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D8" s="4">
+        <v>45768</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
v1.9 Updating Login CRS
</commit_message>
<xml_diff>
--- a/LH_REQUIREMENTS/LH_CRS.xlsx
+++ b/LH_REQUIREMENTS/LH_CRS.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20417"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98444024-1314-495F-8A0F-3BDD8DC712AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{183EF454-7316-4B80-8DC5-44023910FE89}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6945" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LH_CRS" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="91">
   <si>
     <t>ID</t>
   </si>
@@ -224,21 +224,6 @@
     <t>LH-CRS-LOGIN-003</t>
   </si>
   <si>
-    <t>LH-CRS-LOGIN-004</t>
-  </si>
-  <si>
-    <t>Users must log in using their email and password.</t>
-  </si>
-  <si>
-    <t>Store passwords using hashing and salting techniques.</t>
-  </si>
-  <si>
-    <t>Show a generic error message for login failures including incorrect password, empty fields, or unregistered email.</t>
-  </si>
-  <si>
-    <t>Only registered users can log in.</t>
-  </si>
-  <si>
     <t>v1.5</t>
   </si>
   <si>
@@ -291,13 +276,31 @@
   </si>
   <si>
     <t>modify Notification CRSs after Review</t>
+  </si>
+  <si>
+    <t>In the case of login failures, a generic error message must be displayed to the user. The message should not reveal whether the issue is related to an incorrect email, incorrect password, or empty fields. The goal is to prevent providing specific information that could aid in malicious attempts.</t>
+  </si>
+  <si>
+    <t>User passwords must be securely stored using modern cryptographic techniques, including hashing and salting, to protect sensitive information.</t>
+  </si>
+  <si>
+    <t>Gehad Ashry</t>
+  </si>
+  <si>
+    <t>v1.9</t>
+  </si>
+  <si>
+    <t>Updating Login CRS</t>
+  </si>
+  <si>
+    <t>Users must log in using a valid email address, which must follow the correct email format (username@domain.com), and a password as specified during the registration process. Only users who have successfully registered and are present in the system’s user database can log in.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -494,7 +497,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -576,6 +579,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -857,22 +869,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D30"/>
+  <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.109375" style="28" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.33203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.140625" style="28" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.28515625" style="11" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="104" style="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.109375" style="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.88671875" style="11"/>
+    <col min="4" max="4" width="18.140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.85546875" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="18" customFormat="1" ht="19.2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" s="18" customFormat="1" ht="19.5">
       <c r="A1" s="16" t="s">
         <v>6</v>
       </c>
@@ -886,7 +898,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4">
       <c r="A2" s="29" t="s">
         <v>13</v>
       </c>
@@ -900,7 +912,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4">
       <c r="A3" s="30"/>
       <c r="B3" s="20" t="s">
         <v>31</v>
@@ -912,7 +924,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4">
       <c r="A4" s="30"/>
       <c r="B4" s="19" t="s">
         <v>32</v>
@@ -924,7 +936,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4">
       <c r="A5" s="30"/>
       <c r="B5" s="20" t="s">
         <v>33</v>
@@ -936,7 +948,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4">
       <c r="A6" s="30"/>
       <c r="B6" s="19" t="s">
         <v>34</v>
@@ -948,7 +960,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4">
       <c r="A7" s="30"/>
       <c r="B7" s="20" t="s">
         <v>35</v>
@@ -960,43 +972,43 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4">
       <c r="A8" s="30"/>
       <c r="B8" s="19" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="C8" s="22" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="D8" s="10" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4">
       <c r="A9" s="30"/>
       <c r="B9" s="20" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="D9" s="11" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4">
       <c r="A10" s="31"/>
       <c r="B10" s="19" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="C10" s="22" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="D10" s="10" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4">
       <c r="A11" s="34" t="s">
         <v>7</v>
       </c>
@@ -1010,7 +1022,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4">
       <c r="A12" s="34"/>
       <c r="B12" s="20" t="s">
         <v>19</v>
@@ -1022,7 +1034,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4">
       <c r="A13" s="34"/>
       <c r="B13" s="19" t="s">
         <v>37</v>
@@ -1034,7 +1046,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4">
       <c r="A14" s="35" t="s">
         <v>8</v>
       </c>
@@ -1048,7 +1060,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4">
       <c r="A15" s="35"/>
       <c r="B15" s="19" t="s">
         <v>39</v>
@@ -1060,7 +1072,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4">
       <c r="A16" s="35"/>
       <c r="B16" s="20" t="s">
         <v>20</v>
@@ -1072,7 +1084,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4">
       <c r="A17" s="35"/>
       <c r="B17" s="19" t="s">
         <v>40</v>
@@ -1084,7 +1096,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4">
       <c r="A18" s="35"/>
       <c r="B18" s="20" t="s">
         <v>41</v>
@@ -1096,7 +1108,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4">
       <c r="A19" s="35"/>
       <c r="B19" s="19" t="s">
         <v>42</v>
@@ -1108,7 +1120,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" s="12" customFormat="1">
       <c r="A20" s="34" t="s">
         <v>9</v>
       </c>
@@ -1122,19 +1134,19 @@
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" s="13" customFormat="1">
       <c r="A21" s="34"/>
       <c r="B21" s="24" t="s">
         <v>59</v>
       </c>
       <c r="C21" s="13" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="D21" s="13" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" s="12" customFormat="1">
       <c r="A22" s="25" t="s">
         <v>12</v>
       </c>
@@ -1142,13 +1154,13 @@
         <v>56</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="D22" s="14" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="23" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" s="13" customFormat="1">
       <c r="A23" s="32" t="s">
         <v>10</v>
       </c>
@@ -1162,19 +1174,19 @@
         <v>17</v>
       </c>
     </row>
-    <row r="24" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" s="13" customFormat="1">
       <c r="A24" s="33"/>
       <c r="B24" s="20" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="D24" s="11" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="25" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" s="12" customFormat="1">
       <c r="A25" s="35" t="s">
         <v>11</v>
       </c>
@@ -1188,7 +1200,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="26" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" s="13" customFormat="1">
       <c r="A26" s="35"/>
       <c r="B26" s="27" t="s">
         <v>61</v>
@@ -1200,61 +1212,49 @@
         <v>17</v>
       </c>
     </row>
-    <row r="27" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" s="12" customFormat="1" ht="45">
       <c r="A27" s="34" t="s">
         <v>63</v>
       </c>
-      <c r="B27" s="26" t="s">
+      <c r="B27" s="37" t="s">
         <v>64</v>
       </c>
-      <c r="C27" s="14" t="s">
-        <v>68</v>
+      <c r="C27" s="36" t="s">
+        <v>90</v>
       </c>
       <c r="D27" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.3">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" s="13" customFormat="1" ht="45">
       <c r="A28" s="34"/>
       <c r="B28" s="27" t="s">
         <v>65</v>
       </c>
-      <c r="C28" s="13" t="s">
-        <v>71</v>
+      <c r="C28" s="38" t="s">
+        <v>85</v>
       </c>
       <c r="D28" s="15" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.3">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" s="13" customFormat="1" ht="30">
       <c r="A29" s="34"/>
-      <c r="B29" s="26" t="s">
+      <c r="B29" s="37" t="s">
         <v>66</v>
       </c>
-      <c r="C29" s="12" t="s">
-        <v>70</v>
+      <c r="C29" s="36" t="s">
+        <v>86</v>
       </c>
       <c r="D29" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="34"/>
-      <c r="B30" s="27" t="s">
-        <v>67</v>
-      </c>
-      <c r="C30" s="15" t="s">
-        <v>69</v>
-      </c>
-      <c r="D30" s="15" t="s">
-        <v>17</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="7">
     <mergeCell ref="A2:A10"/>
     <mergeCell ref="A23:A24"/>
-    <mergeCell ref="A27:A30"/>
+    <mergeCell ref="A27:A29"/>
     <mergeCell ref="A11:A13"/>
     <mergeCell ref="A14:A19"/>
     <mergeCell ref="A20:A21"/>
@@ -1262,7 +1262,7 @@
   </mergeCells>
   <phoneticPr fontId="10" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation allowBlank="1" showDropDown="1" sqref="A20 A11 D2 D11 D14 A2 D20:D30 A23 A25" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
+    <dataValidation allowBlank="1" showDropDown="1" sqref="A20 A11 D2 D11 D14 A2 A23 A25 D20:D29" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1271,21 +1271,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15.44140625" customWidth="1"/>
-    <col min="2" max="2" width="22.6640625" customWidth="1"/>
-    <col min="3" max="3" width="62.109375" customWidth="1"/>
-    <col min="4" max="4" width="18.6640625" customWidth="1"/>
+    <col min="1" max="1" width="15.42578125" customWidth="1"/>
+    <col min="2" max="2" width="22.7109375" customWidth="1"/>
+    <col min="3" max="3" width="62.140625" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="9" customFormat="1" ht="42" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4" s="9" customFormat="1" ht="40.5">
       <c r="A1" s="7" t="s">
         <v>45</v>
       </c>
@@ -1299,7 +1299,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="37.200000000000003" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="37.5">
       <c r="A2" s="5" t="s">
         <v>50</v>
       </c>
@@ -1313,7 +1313,7 @@
         <v>45754</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="37.200000000000003" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="37.5">
       <c r="A3" s="6" t="s">
         <v>51</v>
       </c>
@@ -1327,7 +1327,7 @@
         <v>45754</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="37.200000000000003" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="37.5">
       <c r="A4" s="5" t="s">
         <v>54</v>
       </c>
@@ -1341,60 +1341,74 @@
         <v>45759</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="37.200000000000003" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="37.5">
       <c r="A5" s="5" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="D5" s="4">
         <v>45759</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="37.200000000000003" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" ht="37.5">
       <c r="A6" s="5" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="D6" s="4">
         <v>45765</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="18.600000000000001" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="18.75">
       <c r="A7" s="5" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="D7" s="4">
         <v>45766</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="18.600000000000001" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" ht="18.75">
       <c r="A8" s="5" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="D8" s="4">
         <v>45768</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="18.75">
+      <c r="A9" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D9" s="4">
+        <v>45776</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
v1.10 Updating ADMINHOME CRS and USERHOME
</commit_message>
<xml_diff>
--- a/LH_REQUIREMENTS/LH_CRS.xlsx
+++ b/LH_REQUIREMENTS/LH_CRS.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20417"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{183EF454-7316-4B80-8DC5-44023910FE89}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6945" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6945"/>
   </bookViews>
   <sheets>
     <sheet name="LH_CRS" sheetId="1" r:id="rId1"/>
@@ -21,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="110">
   <si>
     <t>ID</t>
   </si>
@@ -236,9 +235,6 @@
     <t>LH-CRS-REGISTRATION-007</t>
   </si>
   <si>
-    <t xml:space="preserve"> the username have specific constraints</t>
-  </si>
-  <si>
     <t>m prevent multiple registrations using the same email or username</t>
   </si>
   <si>
@@ -294,13 +290,81 @@
   </si>
   <si>
     <t>Users must log in using a valid email address, which must follow the correct email format (username@domain.com), and a password as specified during the registration process. Only users who have successfully registered and are present in the system’s user database can log in.</t>
+  </si>
+  <si>
+    <t>v1.10</t>
+  </si>
+  <si>
+    <t>Hala Eldaly</t>
+  </si>
+  <si>
+    <t>ADMINHOME</t>
+  </si>
+  <si>
+    <t>LH-CRS-ADMINHOME-001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Administrators must have access to a dedicated homepage to manage all posts and actions related to their administrative tasks. This page should display posts from all categories, each with its title and a short preview. Additionally, a dropdown menu labeled "Admin Tools" must provide options for different administrative actions. The page should include a personalized welcome message for the administrator at the top right corner and a logo at the top left corner.
+</t>
+  </si>
+  <si>
+    <t>LH-CRS-ADMINHOME-002</t>
+  </si>
+  <si>
+    <t>LH-CRS-ADMINHOME-003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Posts listed on the Admin Home Page must be fetched dynamically to reflect the latest updates across all categories. Any errors in fetching posts.
+</t>
+  </si>
+  <si>
+    <t>the username have specific constraints</t>
+  </si>
+  <si>
+    <t>Updating ADMINHOME CRS and USERHOME</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LH-CRS-USERHOME-001
+</t>
+  </si>
+  <si>
+    <t>LH-CRS-USERHOME-002</t>
+  </si>
+  <si>
+    <t>LH-CRS-USERHOME-003</t>
+  </si>
+  <si>
+    <t>USERHOME</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The home page must dynamically fetch and display notifications for new articles in categories the user follows, ensuring that users are kept updated with the latest content. Notifications should include the category name and a brief description of the new update.
+</t>
+  </si>
+  <si>
+    <t>LH-CRS-USERHOME-004</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Users must have access to a personalized home page displaying a welcome message and their username prominently at the top. A button labeled "Go to Categories" should allow users to navigate to the categories page effortlessly.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Posts from followed categories must be listed on the user home page. Each post should include a title and post content. The system must ensure real-time synchronization to reflect the latest updates accurately.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A notification bell icon must be displayed on the user home page, showing the number of new notifications. 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The dropdown menu labeled "Admin Tools" must provide clearly defined actions like "Delete Post" and "Delete User" in a drop-down menu Each action must be intuitively accessible and function securely.
+</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -376,8 +440,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -432,8 +503,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -456,48 +533,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -526,12 +567,9 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -541,56 +579,84 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="20% - Accent5" xfId="1" builtinId="46"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -868,390 +934,660 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D29"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:X36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView tabSelected="1" topLeftCell="C30" zoomScale="142" zoomScaleNormal="76" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.140625" style="28" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.28515625" style="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="104" style="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.85546875" style="11"/>
+    <col min="1" max="1" width="18.140625" style="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.5703125" style="10" customWidth="1"/>
+    <col min="3" max="3" width="104" style="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" style="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.85546875" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="18" customFormat="1" ht="19.5">
-      <c r="A1" s="16" t="s">
+    <row r="1" spans="1:4" s="15" customFormat="1" ht="19.5">
+      <c r="A1" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="D1" s="14" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="18" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="30"/>
-      <c r="B3" s="20" t="s">
+      <c r="A3" s="39"/>
+      <c r="B3" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="C3" s="21" t="s">
+      <c r="C3" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="20" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="30"/>
-      <c r="B4" s="19" t="s">
+      <c r="A4" s="39"/>
+      <c r="B4" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="C4" s="22" t="s">
+      <c r="C4" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="18" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="30"/>
-      <c r="B5" s="20" t="s">
+      <c r="A5" s="39"/>
+      <c r="B5" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="C5" s="21" t="s">
+      <c r="C5" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="11" t="s">
+      <c r="D5" s="20" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="30"/>
-      <c r="B6" s="19" t="s">
+      <c r="A6" s="39"/>
+      <c r="B6" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="22" t="s">
+      <c r="C6" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="D6" s="18" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" s="30"/>
-      <c r="B7" s="20" t="s">
+      <c r="A7" s="39"/>
+      <c r="B7" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="11" t="s">
+      <c r="D7" s="20" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" s="30"/>
-      <c r="B8" s="19" t="s">
+      <c r="A8" s="39"/>
+      <c r="B8" s="17" t="s">
         <v>70</v>
       </c>
-      <c r="C8" s="22" t="s">
+      <c r="C8" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="D8" s="18" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" s="30"/>
-      <c r="B9" s="20" t="s">
+      <c r="A9" s="39"/>
+      <c r="B9" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="C9" s="20" t="s">
+        <v>98</v>
+      </c>
+      <c r="D9" s="20" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="39"/>
+      <c r="B10" s="17" t="s">
         <v>74</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C10" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="D9" s="11" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="31"/>
-      <c r="B10" s="19" t="s">
-        <v>75</v>
-      </c>
-      <c r="C10" s="22" t="s">
-        <v>72</v>
-      </c>
-      <c r="D10" s="10" t="s">
+      <c r="D10" s="18" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11" s="34" t="s">
+      <c r="A11" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="19" t="s">
+      <c r="B11" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="C11" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="D11" s="10" t="s">
+      <c r="D11" s="18" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:4">
-      <c r="A12" s="34"/>
-      <c r="B12" s="20" t="s">
+      <c r="A12" s="38"/>
+      <c r="B12" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="21" t="s">
+      <c r="C12" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="D12" s="11" t="s">
+      <c r="D12" s="20" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:4">
-      <c r="A13" s="34"/>
-      <c r="B13" s="19" t="s">
+      <c r="A13" s="38"/>
+      <c r="B13" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="C13" s="10" t="s">
+      <c r="C13" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="D13" s="10" t="s">
+      <c r="D13" s="18" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:4">
-      <c r="A14" s="35" t="s">
+      <c r="A14" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="B14" s="20" t="s">
+      <c r="B14" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="C14" s="11" t="s">
+      <c r="C14" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="D14" s="11" t="s">
+      <c r="D14" s="20" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:4">
-      <c r="A15" s="35"/>
-      <c r="B15" s="19" t="s">
+      <c r="A15" s="39"/>
+      <c r="B15" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="C15" s="22" t="s">
+      <c r="C15" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="D15" s="10" t="s">
+      <c r="D15" s="18" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:4">
-      <c r="A16" s="35"/>
-      <c r="B16" s="20" t="s">
+      <c r="A16" s="39"/>
+      <c r="B16" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="11" t="s">
+      <c r="C16" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="D16" s="11" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17" s="35"/>
-      <c r="B17" s="19" t="s">
+      <c r="D16" s="20" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:24">
+      <c r="A17" s="39"/>
+      <c r="B17" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="C17" s="22" t="s">
+      <c r="C17" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="D17" s="10" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18" s="35"/>
-      <c r="B18" s="20" t="s">
+      <c r="D17" s="18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:24">
+      <c r="A18" s="39"/>
+      <c r="B18" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="C18" s="11" t="s">
+      <c r="C18" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="D18" s="11" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19" s="35"/>
-      <c r="B19" s="19" t="s">
+      <c r="D18" s="20" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:24">
+      <c r="A19" s="39"/>
+      <c r="B19" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="C19" s="22" t="s">
+      <c r="C19" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="D19" s="10" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" s="12" customFormat="1">
-      <c r="A20" s="34" t="s">
+      <c r="D19" s="18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:24" s="11" customFormat="1">
+      <c r="A20" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="B20" s="23" t="s">
+      <c r="B20" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="C20" s="12" t="s">
+      <c r="C20" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="D20" s="12" t="s">
+      <c r="D20" s="22" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:4" s="13" customFormat="1">
-      <c r="A21" s="34"/>
-      <c r="B21" s="24" t="s">
+    <row r="21" spans="1:24" s="12" customFormat="1">
+      <c r="A21" s="38"/>
+      <c r="B21" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="C21" s="13" t="s">
-        <v>82</v>
-      </c>
-      <c r="D21" s="13" t="s">
+      <c r="C21" s="24" t="s">
+        <v>81</v>
+      </c>
+      <c r="D21" s="24" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" s="12" customFormat="1">
+      <c r="E21" s="10"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="10"/>
+      <c r="H21" s="10"/>
+      <c r="I21" s="10"/>
+      <c r="J21" s="10"/>
+      <c r="K21" s="10"/>
+      <c r="L21" s="10"/>
+      <c r="M21" s="10"/>
+      <c r="N21" s="10"/>
+      <c r="O21" s="10"/>
+      <c r="P21" s="10"/>
+      <c r="Q21" s="10"/>
+      <c r="R21" s="10"/>
+      <c r="S21" s="10"/>
+      <c r="T21" s="10"/>
+      <c r="U21" s="10"/>
+      <c r="V21" s="10"/>
+      <c r="W21" s="10"/>
+      <c r="X21" s="10"/>
+    </row>
+    <row r="22" spans="1:24" s="11" customFormat="1">
       <c r="A22" s="25" t="s">
         <v>12</v>
       </c>
       <c r="B22" s="26" t="s">
         <v>56</v>
       </c>
-      <c r="C22" s="14" t="s">
-        <v>79</v>
-      </c>
-      <c r="D22" s="14" t="s">
+      <c r="C22" s="27" t="s">
+        <v>78</v>
+      </c>
+      <c r="D22" s="27" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" s="13" customFormat="1">
-      <c r="A23" s="32" t="s">
+      <c r="E22" s="10"/>
+      <c r="F22" s="10"/>
+      <c r="G22" s="10"/>
+      <c r="H22" s="10"/>
+      <c r="I22" s="10"/>
+      <c r="J22" s="10"/>
+      <c r="K22" s="10"/>
+      <c r="L22" s="10"/>
+      <c r="M22" s="10"/>
+      <c r="N22" s="10"/>
+      <c r="O22" s="10"/>
+      <c r="P22" s="10"/>
+      <c r="Q22" s="10"/>
+      <c r="R22" s="10"/>
+      <c r="S22" s="10"/>
+      <c r="T22" s="10"/>
+      <c r="U22" s="10"/>
+      <c r="V22" s="10"/>
+      <c r="W22" s="10"/>
+      <c r="X22" s="10"/>
+    </row>
+    <row r="23" spans="1:24" s="12" customFormat="1">
+      <c r="A23" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="B23" s="24" t="s">
+      <c r="B23" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="C23" s="13" t="s">
+      <c r="C23" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="D23" s="13" t="s">
+      <c r="D23" s="24" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" s="13" customFormat="1">
-      <c r="A24" s="33"/>
-      <c r="B24" s="20" t="s">
-        <v>76</v>
-      </c>
-      <c r="C24" s="11" t="s">
-        <v>73</v>
-      </c>
-      <c r="D24" s="11" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" s="12" customFormat="1">
-      <c r="A25" s="35" t="s">
+      <c r="E23" s="10"/>
+      <c r="F23" s="10"/>
+      <c r="G23" s="10"/>
+      <c r="H23" s="10"/>
+      <c r="I23" s="10"/>
+      <c r="J23" s="10"/>
+      <c r="K23" s="10"/>
+      <c r="L23" s="10"/>
+      <c r="M23" s="10"/>
+      <c r="N23" s="10"/>
+      <c r="O23" s="10"/>
+      <c r="P23" s="10"/>
+      <c r="Q23" s="10"/>
+      <c r="R23" s="10"/>
+      <c r="S23" s="10"/>
+      <c r="T23" s="10"/>
+      <c r="U23" s="10"/>
+      <c r="V23" s="10"/>
+      <c r="W23" s="10"/>
+      <c r="X23" s="10"/>
+    </row>
+    <row r="24" spans="1:24" s="12" customFormat="1">
+      <c r="A24" s="40"/>
+      <c r="B24" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="C24" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="D24" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="E24" s="10"/>
+      <c r="F24" s="10"/>
+      <c r="G24" s="10"/>
+      <c r="H24" s="10"/>
+      <c r="I24" s="10"/>
+      <c r="J24" s="10"/>
+      <c r="K24" s="10"/>
+      <c r="L24" s="10"/>
+      <c r="M24" s="10"/>
+      <c r="N24" s="10"/>
+      <c r="O24" s="10"/>
+      <c r="P24" s="10"/>
+      <c r="Q24" s="10"/>
+      <c r="R24" s="10"/>
+      <c r="S24" s="10"/>
+      <c r="T24" s="10"/>
+      <c r="U24" s="10"/>
+      <c r="V24" s="10"/>
+      <c r="W24" s="10"/>
+      <c r="X24" s="10"/>
+    </row>
+    <row r="25" spans="1:24" s="11" customFormat="1">
+      <c r="A25" s="39" t="s">
         <v>11</v>
       </c>
       <c r="B25" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="C25" s="14" t="s">
+      <c r="C25" s="27" t="s">
         <v>60</v>
       </c>
-      <c r="D25" s="14" t="s">
+      <c r="D25" s="27" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" s="13" customFormat="1">
-      <c r="A26" s="35"/>
-      <c r="B26" s="27" t="s">
+      <c r="E25" s="10"/>
+      <c r="F25" s="10"/>
+      <c r="G25" s="10"/>
+      <c r="H25" s="10"/>
+      <c r="I25" s="10"/>
+      <c r="J25" s="10"/>
+      <c r="K25" s="10"/>
+      <c r="L25" s="10"/>
+      <c r="M25" s="10"/>
+      <c r="N25" s="10"/>
+      <c r="O25" s="10"/>
+      <c r="P25" s="10"/>
+      <c r="Q25" s="10"/>
+      <c r="R25" s="10"/>
+      <c r="S25" s="10"/>
+      <c r="T25" s="10"/>
+      <c r="U25" s="10"/>
+      <c r="V25" s="10"/>
+      <c r="W25" s="10"/>
+      <c r="X25" s="10"/>
+    </row>
+    <row r="26" spans="1:24" s="12" customFormat="1">
+      <c r="A26" s="39"/>
+      <c r="B26" s="28" t="s">
         <v>61</v>
       </c>
-      <c r="C26" s="15" t="s">
+      <c r="C26" s="29" t="s">
         <v>62</v>
       </c>
-      <c r="D26" s="15" t="s">
+      <c r="D26" s="29" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" s="12" customFormat="1" ht="45">
-      <c r="A27" s="34" t="s">
+      <c r="E26" s="10"/>
+      <c r="F26" s="10"/>
+      <c r="G26" s="10"/>
+      <c r="H26" s="10"/>
+      <c r="I26" s="10"/>
+      <c r="J26" s="10"/>
+      <c r="K26" s="10"/>
+      <c r="L26" s="10"/>
+      <c r="M26" s="10"/>
+      <c r="N26" s="10"/>
+      <c r="O26" s="10"/>
+      <c r="P26" s="10"/>
+      <c r="Q26" s="10"/>
+      <c r="R26" s="10"/>
+      <c r="S26" s="10"/>
+      <c r="T26" s="10"/>
+      <c r="U26" s="10"/>
+      <c r="V26" s="10"/>
+      <c r="W26" s="10"/>
+      <c r="X26" s="10"/>
+    </row>
+    <row r="27" spans="1:24" s="11" customFormat="1" ht="45">
+      <c r="A27" s="38" t="s">
         <v>63</v>
       </c>
-      <c r="B27" s="37" t="s">
+      <c r="B27" s="26" t="s">
         <v>64</v>
       </c>
-      <c r="C27" s="36" t="s">
-        <v>90</v>
-      </c>
-      <c r="D27" s="14" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" s="13" customFormat="1" ht="45">
-      <c r="A28" s="34"/>
-      <c r="B28" s="27" t="s">
+      <c r="C27" s="31" t="s">
+        <v>89</v>
+      </c>
+      <c r="D27" s="27" t="s">
+        <v>86</v>
+      </c>
+      <c r="E27" s="10"/>
+      <c r="F27" s="10"/>
+      <c r="G27" s="10"/>
+      <c r="H27" s="10"/>
+      <c r="I27" s="10"/>
+      <c r="J27" s="10"/>
+      <c r="K27" s="10"/>
+      <c r="L27" s="10"/>
+      <c r="M27" s="10"/>
+      <c r="N27" s="10"/>
+      <c r="O27" s="10"/>
+      <c r="P27" s="10"/>
+      <c r="Q27" s="10"/>
+      <c r="R27" s="10"/>
+      <c r="S27" s="10"/>
+      <c r="T27" s="10"/>
+      <c r="U27" s="10"/>
+      <c r="V27" s="10"/>
+      <c r="W27" s="10"/>
+      <c r="X27" s="10"/>
+    </row>
+    <row r="28" spans="1:24" s="12" customFormat="1" ht="45">
+      <c r="A28" s="38"/>
+      <c r="B28" s="28" t="s">
         <v>65</v>
       </c>
-      <c r="C28" s="38" t="s">
+      <c r="C28" s="30" t="s">
+        <v>84</v>
+      </c>
+      <c r="D28" s="29" t="s">
+        <v>86</v>
+      </c>
+      <c r="E28" s="10"/>
+      <c r="F28" s="10"/>
+      <c r="G28" s="10"/>
+      <c r="H28" s="10"/>
+      <c r="I28" s="10"/>
+      <c r="J28" s="10"/>
+      <c r="K28" s="10"/>
+      <c r="L28" s="10"/>
+      <c r="M28" s="10"/>
+      <c r="N28" s="10"/>
+      <c r="O28" s="10"/>
+      <c r="P28" s="10"/>
+      <c r="Q28" s="10"/>
+      <c r="R28" s="10"/>
+      <c r="S28" s="10"/>
+      <c r="T28" s="10"/>
+      <c r="U28" s="10"/>
+      <c r="V28" s="10"/>
+      <c r="W28" s="10"/>
+      <c r="X28" s="10"/>
+    </row>
+    <row r="29" spans="1:24" s="12" customFormat="1" ht="30">
+      <c r="A29" s="38"/>
+      <c r="B29" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="C29" s="31" t="s">
         <v>85</v>
       </c>
-      <c r="D28" s="15" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" s="13" customFormat="1" ht="30">
-      <c r="A29" s="34"/>
-      <c r="B29" s="37" t="s">
-        <v>66</v>
-      </c>
-      <c r="C29" s="36" t="s">
+      <c r="D29" s="27" t="s">
         <v>86</v>
       </c>
-      <c r="D29" s="14" t="s">
-        <v>87</v>
+      <c r="E29" s="10"/>
+      <c r="F29" s="10"/>
+      <c r="G29" s="10"/>
+      <c r="H29" s="10"/>
+      <c r="I29" s="10"/>
+      <c r="J29" s="10"/>
+      <c r="K29" s="10"/>
+      <c r="L29" s="10"/>
+      <c r="M29" s="10"/>
+      <c r="N29" s="10"/>
+      <c r="O29" s="10"/>
+      <c r="P29" s="10"/>
+      <c r="Q29" s="10"/>
+      <c r="R29" s="10"/>
+      <c r="S29" s="10"/>
+      <c r="T29" s="10"/>
+      <c r="U29" s="10"/>
+      <c r="V29" s="10"/>
+      <c r="W29" s="10"/>
+      <c r="X29" s="10"/>
+    </row>
+    <row r="30" spans="1:24" ht="105">
+      <c r="A30" s="37" t="s">
+        <v>92</v>
+      </c>
+      <c r="B30" s="32" t="s">
+        <v>93</v>
+      </c>
+      <c r="C30" s="33" t="s">
+        <v>94</v>
+      </c>
+      <c r="D30" s="32" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="31" spans="1:24" ht="45">
+      <c r="A31" s="37"/>
+      <c r="B31" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="C31" s="31" t="s">
+        <v>97</v>
+      </c>
+      <c r="D31" s="20" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="32" spans="1:24" ht="75">
+      <c r="A32" s="37"/>
+      <c r="B32" s="34" t="s">
+        <v>96</v>
+      </c>
+      <c r="C32" s="36" t="s">
+        <v>109</v>
+      </c>
+      <c r="D32" s="32" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="75">
+      <c r="A33" s="38" t="s">
+        <v>103</v>
+      </c>
+      <c r="B33" s="35" t="s">
+        <v>100</v>
+      </c>
+      <c r="C33" s="31" t="s">
+        <v>106</v>
+      </c>
+      <c r="D33" s="20" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="90">
+      <c r="A34" s="38"/>
+      <c r="B34" s="34" t="s">
+        <v>101</v>
+      </c>
+      <c r="C34" s="36" t="s">
+        <v>104</v>
+      </c>
+      <c r="D34" s="32" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="75">
+      <c r="A35" s="38"/>
+      <c r="B35" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="C35" s="31" t="s">
+        <v>107</v>
+      </c>
+      <c r="D35" s="20" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="60">
+      <c r="A36" s="38"/>
+      <c r="B36" s="34" t="s">
+        <v>105</v>
+      </c>
+      <c r="C36" s="36" t="s">
+        <v>108</v>
+      </c>
+      <c r="D36" s="32" t="s">
+        <v>91</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="9">
+    <mergeCell ref="A30:A32"/>
+    <mergeCell ref="A33:A36"/>
     <mergeCell ref="A2:A10"/>
     <mergeCell ref="A23:A24"/>
     <mergeCell ref="A27:A29"/>
@@ -1262,7 +1598,7 @@
   </mergeCells>
   <phoneticPr fontId="10" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation allowBlank="1" showDropDown="1" sqref="A20 A11 D2 D11 D14 A2 A23 A25 D20:D29" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
+    <dataValidation allowBlank="1" showDropDown="1" sqref="A20 A11 D2 D11 D14 A2 A23 A25 D20:D29"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1270,11 +1606,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1357,13 +1693,13 @@
     </row>
     <row r="6" spans="1:4" ht="37.5">
       <c r="A6" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>77</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>78</v>
       </c>
       <c r="D6" s="4">
         <v>45765</v>
@@ -1371,13 +1707,13 @@
     </row>
     <row r="7" spans="1:4" ht="18.75">
       <c r="A7" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>80</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>81</v>
       </c>
       <c r="D7" s="4">
         <v>45766</v>
@@ -1385,13 +1721,13 @@
     </row>
     <row r="8" spans="1:4" ht="18.75">
       <c r="A8" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D8" s="4">
         <v>45768</v>
@@ -1399,15 +1735,29 @@
     </row>
     <row r="9" spans="1:4" ht="18.75">
       <c r="A9" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>89</v>
-      </c>
       <c r="D9" s="4">
+        <v>45776</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="18.75">
+      <c r="A10" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D10" s="4">
         <v>45776</v>
       </c>
     </row>

</xml_diff>

<commit_message>
v2.1 Updating delete posts feature
</commit_message>
<xml_diff>
--- a/LH_REQUIREMENTS/LH_CRS.xlsx
+++ b/LH_REQUIREMENTS/LH_CRS.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6945" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16815" windowHeight="7650"/>
   </bookViews>
   <sheets>
     <sheet name="LH_CRS" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="131">
   <si>
     <t>ID</t>
   </si>
@@ -196,13 +196,7 @@
     <t>LH-CRS-ID-CONSTRAINS-001</t>
   </si>
   <si>
-    <t>LH-CRS-ADMIN-CONSTRAINS-001</t>
-  </si>
-  <si>
     <t>LH-CRS-NOTIFICATIONS-002</t>
-  </si>
-  <si>
-    <t>Admin features must include the ability to remove articles, videos, and audio files.</t>
   </si>
   <si>
     <t>LH-CRS-ADMIN-CONSTRAINS-002</t>
@@ -400,6 +394,39 @@
   </si>
   <si>
     <t>Updating PUBLISHVIDEO</t>
+  </si>
+  <si>
+    <t>publish video</t>
+  </si>
+  <si>
+    <t>Admin can delete a post by searching about posts of any user by its username</t>
+  </si>
+  <si>
+    <t>LH-CRS-DELETEPOST-001</t>
+  </si>
+  <si>
+    <t>LH-CRS-DELETEPOST-002</t>
+  </si>
+  <si>
+    <t>an informative message will appear if there is no posts of username that you search by it</t>
+  </si>
+  <si>
+    <t>an informative message will appear if username that you search by it not found</t>
+  </si>
+  <si>
+    <t>LH-CRS-DELETEPOST-003</t>
+  </si>
+  <si>
+    <t>LH-CRS-DELETEPOST-004</t>
+  </si>
+  <si>
+    <t>Admin have the ability to delete any post ( "articles" ," videos", "audio") throw delete post page</t>
+  </si>
+  <si>
+    <t>LH-CRS-DELETEPOST-005</t>
+  </si>
+  <si>
+    <t>Admin can go back to admin home page by clicking the logo pf the website</t>
   </si>
 </sst>
 </file>
@@ -617,7 +644,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -661,24 +688,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -691,18 +712,12 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -719,9 +734,6 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="10" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -733,14 +745,35 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1023,10 +1056,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X41"/>
+  <dimension ref="A1:W45"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" zoomScale="96" zoomScaleNormal="76" workbookViewId="0">
-      <selection activeCell="C48" sqref="C48"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="96" zoomScaleNormal="76" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -1053,250 +1086,250 @@
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="38" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="C2" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="19" t="s">
+      <c r="D2" s="18" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="17"/>
-      <c r="B3" s="20" t="s">
+      <c r="A3" s="38"/>
+      <c r="B3" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="C3" s="21" t="s">
+      <c r="C3" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="21" t="s">
+      <c r="D3" s="20" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="17"/>
-      <c r="B4" s="18" t="s">
+      <c r="A4" s="38"/>
+      <c r="B4" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="C4" s="19" t="s">
+      <c r="C4" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="19" t="s">
+      <c r="D4" s="18" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="17"/>
-      <c r="B5" s="20" t="s">
+      <c r="A5" s="38"/>
+      <c r="B5" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="C5" s="21" t="s">
+      <c r="C5" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="21" t="s">
+      <c r="D5" s="20" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="17"/>
-      <c r="B6" s="18" t="s">
+      <c r="A6" s="38"/>
+      <c r="B6" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="19" t="s">
+      <c r="C6" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="19" t="s">
+      <c r="D6" s="18" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" s="17"/>
-      <c r="B7" s="20" t="s">
+      <c r="A7" s="38"/>
+      <c r="B7" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="C7" s="21" t="s">
+      <c r="C7" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="21" t="s">
+      <c r="D7" s="20" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" s="17"/>
-      <c r="B8" s="18" t="s">
+      <c r="A8" s="38"/>
+      <c r="B8" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="C8" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="D8" s="18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="38"/>
+      <c r="B9" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="C8" s="19" t="s">
-        <v>69</v>
-      </c>
-      <c r="D8" s="19" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" s="17"/>
-      <c r="B9" s="20" t="s">
-        <v>72</v>
-      </c>
-      <c r="C9" s="21" t="s">
-        <v>97</v>
-      </c>
-      <c r="D9" s="21" t="s">
+      <c r="C9" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="D9" s="20" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:4">
-      <c r="A10" s="17"/>
-      <c r="B10" s="18" t="s">
-        <v>73</v>
-      </c>
-      <c r="C10" s="19" t="s">
-        <v>118</v>
-      </c>
-      <c r="D10" s="19" t="s">
+      <c r="A10" s="38"/>
+      <c r="B10" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="C10" s="18" t="s">
+        <v>116</v>
+      </c>
+      <c r="D10" s="18" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11" s="22" t="s">
+      <c r="A11" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="18" t="s">
+      <c r="B11" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="C11" s="19" t="s">
+      <c r="C11" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="D11" s="19" t="s">
+      <c r="D11" s="18" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:4">
-      <c r="A12" s="22"/>
-      <c r="B12" s="20" t="s">
+      <c r="A12" s="39"/>
+      <c r="B12" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="21" t="s">
+      <c r="C12" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="D12" s="21" t="s">
+      <c r="D12" s="20" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:4">
-      <c r="A13" s="22"/>
-      <c r="B13" s="18" t="s">
+      <c r="A13" s="39"/>
+      <c r="B13" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="C13" s="19" t="s">
+      <c r="C13" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="D13" s="19" t="s">
+      <c r="D13" s="18" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:4">
-      <c r="A14" s="17" t="s">
+      <c r="A14" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="B14" s="20" t="s">
+      <c r="B14" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="C14" s="21" t="s">
+      <c r="C14" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="D14" s="21" t="s">
+      <c r="D14" s="20" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:4">
-      <c r="A15" s="17"/>
-      <c r="B15" s="18" t="s">
+      <c r="A15" s="38"/>
+      <c r="B15" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="C15" s="19" t="s">
+      <c r="C15" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="D15" s="19" t="s">
+      <c r="D15" s="18" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:4">
-      <c r="A16" s="17"/>
-      <c r="B16" s="20" t="s">
+      <c r="A16" s="38"/>
+      <c r="B16" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="21" t="s">
+      <c r="C16" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="D16" s="21" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="17" spans="1:24">
-      <c r="A17" s="17"/>
-      <c r="B17" s="18" t="s">
+      <c r="D16" s="20" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23">
+      <c r="A17" s="38"/>
+      <c r="B17" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="C17" s="19" t="s">
+      <c r="C17" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="D17" s="19" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="1:24">
-      <c r="A18" s="17"/>
-      <c r="B18" s="20" t="s">
+      <c r="D17" s="18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:23">
+      <c r="A18" s="38"/>
+      <c r="B18" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="C18" s="21" t="s">
+      <c r="C18" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="D18" s="21" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="19" spans="1:24">
-      <c r="A19" s="17"/>
-      <c r="B19" s="18" t="s">
+      <c r="D18" s="20" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:23">
+      <c r="A19" s="38"/>
+      <c r="B19" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="C19" s="19" t="s">
+      <c r="C19" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="D19" s="19" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="20" spans="1:24" s="11" customFormat="1">
-      <c r="A20" s="22" t="s">
+      <c r="D19" s="18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23" s="11" customFormat="1">
+      <c r="A20" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="B20" s="23" t="s">
+      <c r="B20" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="C20" s="24" t="s">
+      <c r="C20" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="D20" s="24" t="s">
+      <c r="D20" s="22" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:24" s="12" customFormat="1">
-      <c r="A21" s="22"/>
-      <c r="B21" s="25" t="s">
-        <v>59</v>
-      </c>
-      <c r="C21" s="26" t="s">
-        <v>80</v>
-      </c>
-      <c r="D21" s="26" t="s">
+    <row r="21" spans="1:23" s="12" customFormat="1">
+      <c r="A21" s="39"/>
+      <c r="B21" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="C21" s="24" t="s">
+        <v>78</v>
+      </c>
+      <c r="D21" s="24" t="s">
         <v>17</v>
       </c>
       <c r="E21" s="10"/>
@@ -1318,19 +1351,18 @@
       <c r="U21" s="10"/>
       <c r="V21" s="10"/>
       <c r="W21" s="10"/>
-      <c r="X21" s="10"/>
-    </row>
-    <row r="22" spans="1:24" s="11" customFormat="1">
-      <c r="A22" s="27" t="s">
+    </row>
+    <row r="22" spans="1:23" s="11" customFormat="1">
+      <c r="A22" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="B22" s="28" t="s">
+      <c r="B22" s="25" t="s">
         <v>56</v>
       </c>
-      <c r="C22" s="29" t="s">
-        <v>77</v>
-      </c>
-      <c r="D22" s="29" t="s">
+      <c r="C22" s="26" t="s">
+        <v>75</v>
+      </c>
+      <c r="D22" s="26" t="s">
         <v>17</v>
       </c>
       <c r="E22" s="10"/>
@@ -1352,19 +1384,18 @@
       <c r="U22" s="10"/>
       <c r="V22" s="10"/>
       <c r="W22" s="10"/>
-      <c r="X22" s="10"/>
-    </row>
-    <row r="23" spans="1:24" s="12" customFormat="1">
-      <c r="A23" s="30" t="s">
+    </row>
+    <row r="23" spans="1:23" s="12" customFormat="1">
+      <c r="A23" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="B23" s="25" t="s">
+      <c r="B23" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="C23" s="26" t="s">
+      <c r="C23" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="D23" s="26" t="s">
+      <c r="D23" s="24" t="s">
         <v>17</v>
       </c>
       <c r="E23" s="10"/>
@@ -1386,17 +1417,16 @@
       <c r="U23" s="10"/>
       <c r="V23" s="10"/>
       <c r="W23" s="10"/>
-      <c r="X23" s="10"/>
-    </row>
-    <row r="24" spans="1:24" s="12" customFormat="1">
-      <c r="A24" s="30"/>
-      <c r="B24" s="20" t="s">
-        <v>74</v>
-      </c>
-      <c r="C24" s="21" t="s">
-        <v>71</v>
-      </c>
-      <c r="D24" s="21" t="s">
+    </row>
+    <row r="24" spans="1:23" s="12" customFormat="1">
+      <c r="A24" s="41"/>
+      <c r="B24" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="C24" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="D24" s="20" t="s">
         <v>16</v>
       </c>
       <c r="E24" s="10"/>
@@ -1418,20 +1448,19 @@
       <c r="U24" s="10"/>
       <c r="V24" s="10"/>
       <c r="W24" s="10"/>
-      <c r="X24" s="10"/>
-    </row>
-    <row r="25" spans="1:24" s="11" customFormat="1">
-      <c r="A25" s="17" t="s">
+    </row>
+    <row r="25" spans="1:23" s="11" customFormat="1">
+      <c r="A25" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="B25" s="28" t="s">
-        <v>58</v>
-      </c>
-      <c r="C25" s="29" t="s">
-        <v>60</v>
-      </c>
-      <c r="D25" s="29" t="s">
-        <v>17</v>
+      <c r="B25" s="23" t="s">
+        <v>122</v>
+      </c>
+      <c r="C25" s="24" t="s">
+        <v>128</v>
+      </c>
+      <c r="D25" s="24" t="s">
+        <v>16</v>
       </c>
       <c r="E25" s="10"/>
       <c r="F25" s="10"/>
@@ -1452,18 +1481,17 @@
       <c r="U25" s="10"/>
       <c r="V25" s="10"/>
       <c r="W25" s="10"/>
-      <c r="X25" s="10"/>
-    </row>
-    <row r="26" spans="1:24" s="12" customFormat="1">
-      <c r="A26" s="17"/>
-      <c r="B26" s="31" t="s">
-        <v>61</v>
-      </c>
-      <c r="C26" s="32" t="s">
-        <v>62</v>
-      </c>
-      <c r="D26" s="32" t="s">
-        <v>17</v>
+    </row>
+    <row r="26" spans="1:23" s="11" customFormat="1">
+      <c r="A26" s="38"/>
+      <c r="B26" s="25" t="s">
+        <v>123</v>
+      </c>
+      <c r="C26" s="26" t="s">
+        <v>121</v>
+      </c>
+      <c r="D26" s="26" t="s">
+        <v>16</v>
       </c>
       <c r="E26" s="10"/>
       <c r="F26" s="10"/>
@@ -1484,20 +1512,17 @@
       <c r="U26" s="10"/>
       <c r="V26" s="10"/>
       <c r="W26" s="10"/>
-      <c r="X26" s="10"/>
-    </row>
-    <row r="27" spans="1:24" s="11" customFormat="1" ht="45">
-      <c r="A27" s="22" t="s">
-        <v>63</v>
-      </c>
-      <c r="B27" s="28" t="s">
-        <v>64</v>
-      </c>
-      <c r="C27" s="33" t="s">
-        <v>88</v>
-      </c>
-      <c r="D27" s="29" t="s">
-        <v>85</v>
+    </row>
+    <row r="27" spans="1:23" s="11" customFormat="1">
+      <c r="A27" s="38"/>
+      <c r="B27" s="23" t="s">
+        <v>126</v>
+      </c>
+      <c r="C27" s="24" t="s">
+        <v>124</v>
+      </c>
+      <c r="D27" s="24" t="s">
+        <v>16</v>
       </c>
       <c r="E27" s="10"/>
       <c r="F27" s="10"/>
@@ -1518,18 +1543,17 @@
       <c r="U27" s="10"/>
       <c r="V27" s="10"/>
       <c r="W27" s="10"/>
-      <c r="X27" s="10"/>
-    </row>
-    <row r="28" spans="1:24" s="12" customFormat="1" ht="45">
-      <c r="A28" s="22"/>
-      <c r="B28" s="31" t="s">
-        <v>65</v>
-      </c>
-      <c r="C28" s="34" t="s">
-        <v>83</v>
-      </c>
-      <c r="D28" s="32" t="s">
-        <v>85</v>
+    </row>
+    <row r="28" spans="1:23" s="11" customFormat="1">
+      <c r="A28" s="38"/>
+      <c r="B28" s="25" t="s">
+        <v>127</v>
+      </c>
+      <c r="C28" s="26" t="s">
+        <v>125</v>
+      </c>
+      <c r="D28" s="26" t="s">
+        <v>16</v>
       </c>
       <c r="E28" s="10"/>
       <c r="F28" s="10"/>
@@ -1550,18 +1574,17 @@
       <c r="U28" s="10"/>
       <c r="V28" s="10"/>
       <c r="W28" s="10"/>
-      <c r="X28" s="10"/>
-    </row>
-    <row r="29" spans="1:24" s="12" customFormat="1" ht="30">
-      <c r="A29" s="22"/>
-      <c r="B29" s="28" t="s">
-        <v>66</v>
-      </c>
-      <c r="C29" s="33" t="s">
-        <v>84</v>
-      </c>
-      <c r="D29" s="29" t="s">
-        <v>85</v>
+    </row>
+    <row r="29" spans="1:23" s="11" customFormat="1">
+      <c r="A29" s="38"/>
+      <c r="B29" s="23" t="s">
+        <v>129</v>
+      </c>
+      <c r="C29" s="24" t="s">
+        <v>130</v>
+      </c>
+      <c r="D29" s="24" t="s">
+        <v>16</v>
       </c>
       <c r="E29" s="10"/>
       <c r="F29" s="10"/>
@@ -1582,174 +1605,299 @@
       <c r="U29" s="10"/>
       <c r="V29" s="10"/>
       <c r="W29" s="10"/>
-      <c r="X29" s="10"/>
-    </row>
-    <row r="30" spans="1:24" ht="105">
-      <c r="A30" s="35" t="s">
+    </row>
+    <row r="30" spans="1:23" s="12" customFormat="1">
+      <c r="A30" s="38"/>
+      <c r="B30" s="36" t="s">
+        <v>59</v>
+      </c>
+      <c r="C30" s="37" t="s">
+        <v>60</v>
+      </c>
+      <c r="D30" s="37" t="s">
+        <v>17</v>
+      </c>
+      <c r="E30" s="10"/>
+      <c r="F30" s="10"/>
+      <c r="G30" s="10"/>
+      <c r="H30" s="10"/>
+      <c r="I30" s="10"/>
+      <c r="J30" s="10"/>
+      <c r="K30" s="10"/>
+      <c r="L30" s="10"/>
+      <c r="M30" s="10"/>
+      <c r="N30" s="10"/>
+      <c r="O30" s="10"/>
+      <c r="P30" s="10"/>
+      <c r="Q30" s="10"/>
+      <c r="R30" s="10"/>
+      <c r="S30" s="10"/>
+      <c r="T30" s="10"/>
+      <c r="U30" s="10"/>
+      <c r="V30" s="10"/>
+      <c r="W30" s="10"/>
+    </row>
+    <row r="31" spans="1:23" s="11" customFormat="1" ht="45">
+      <c r="A31" s="39" t="s">
+        <v>61</v>
+      </c>
+      <c r="B31" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="C31" s="29" t="s">
+        <v>86</v>
+      </c>
+      <c r="D31" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="E31" s="10"/>
+      <c r="F31" s="10"/>
+      <c r="G31" s="10"/>
+      <c r="H31" s="10"/>
+      <c r="I31" s="10"/>
+      <c r="J31" s="10"/>
+      <c r="K31" s="10"/>
+      <c r="L31" s="10"/>
+      <c r="M31" s="10"/>
+      <c r="N31" s="10"/>
+      <c r="O31" s="10"/>
+      <c r="P31" s="10"/>
+      <c r="Q31" s="10"/>
+      <c r="R31" s="10"/>
+      <c r="S31" s="10"/>
+      <c r="T31" s="10"/>
+      <c r="U31" s="10"/>
+      <c r="V31" s="10"/>
+      <c r="W31" s="10"/>
+    </row>
+    <row r="32" spans="1:23" s="12" customFormat="1" ht="45">
+      <c r="A32" s="39"/>
+      <c r="B32" s="27" t="s">
+        <v>63</v>
+      </c>
+      <c r="C32" s="30" t="s">
+        <v>81</v>
+      </c>
+      <c r="D32" s="28" t="s">
+        <v>83</v>
+      </c>
+      <c r="E32" s="10"/>
+      <c r="F32" s="10"/>
+      <c r="G32" s="10"/>
+      <c r="H32" s="10"/>
+      <c r="I32" s="10"/>
+      <c r="J32" s="10"/>
+      <c r="K32" s="10"/>
+      <c r="L32" s="10"/>
+      <c r="M32" s="10"/>
+      <c r="N32" s="10"/>
+      <c r="O32" s="10"/>
+      <c r="P32" s="10"/>
+      <c r="Q32" s="10"/>
+      <c r="R32" s="10"/>
+      <c r="S32" s="10"/>
+      <c r="T32" s="10"/>
+      <c r="U32" s="10"/>
+      <c r="V32" s="10"/>
+      <c r="W32" s="10"/>
+    </row>
+    <row r="33" spans="1:23" s="12" customFormat="1" ht="30">
+      <c r="A33" s="39"/>
+      <c r="B33" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="C33" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="D33" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="E33" s="10"/>
+      <c r="F33" s="10"/>
+      <c r="G33" s="10"/>
+      <c r="H33" s="10"/>
+      <c r="I33" s="10"/>
+      <c r="J33" s="10"/>
+      <c r="K33" s="10"/>
+      <c r="L33" s="10"/>
+      <c r="M33" s="10"/>
+      <c r="N33" s="10"/>
+      <c r="O33" s="10"/>
+      <c r="P33" s="10"/>
+      <c r="Q33" s="10"/>
+      <c r="R33" s="10"/>
+      <c r="S33" s="10"/>
+      <c r="T33" s="10"/>
+      <c r="U33" s="10"/>
+      <c r="V33" s="10"/>
+      <c r="W33" s="10"/>
+    </row>
+    <row r="34" spans="1:23" ht="105">
+      <c r="A34" s="42" t="s">
+        <v>89</v>
+      </c>
+      <c r="B34" s="31" t="s">
+        <v>90</v>
+      </c>
+      <c r="C34" s="32" t="s">
         <v>91</v>
       </c>
-      <c r="B30" s="36" t="s">
+      <c r="D34" s="31" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="35" spans="1:23" ht="45">
+      <c r="A35" s="42"/>
+      <c r="B35" s="19" t="s">
         <v>92</v>
       </c>
-      <c r="C30" s="37" t="s">
+      <c r="C35" s="29" t="s">
+        <v>94</v>
+      </c>
+      <c r="D35" s="20" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="36" spans="1:23" ht="75">
+      <c r="A36" s="42"/>
+      <c r="B36" s="33" t="s">
         <v>93</v>
       </c>
-      <c r="D30" s="36" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="31" spans="1:24" ht="45">
-      <c r="A31" s="35"/>
-      <c r="B31" s="20" t="s">
-        <v>94</v>
-      </c>
-      <c r="C31" s="33" t="s">
-        <v>96</v>
-      </c>
-      <c r="D31" s="21" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="32" spans="1:24" ht="75">
-      <c r="A32" s="35"/>
-      <c r="B32" s="38" t="s">
-        <v>95</v>
-      </c>
-      <c r="C32" s="39" t="s">
+      <c r="C36" s="34" t="s">
+        <v>106</v>
+      </c>
+      <c r="D36" s="31" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="37" spans="1:23" ht="75">
+      <c r="A37" s="39" t="s">
+        <v>100</v>
+      </c>
+      <c r="B37" s="35" t="s">
+        <v>97</v>
+      </c>
+      <c r="C37" s="29" t="s">
+        <v>103</v>
+      </c>
+      <c r="D37" s="20" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="38" spans="1:23" ht="90">
+      <c r="A38" s="39"/>
+      <c r="B38" s="33" t="s">
+        <v>98</v>
+      </c>
+      <c r="C38" s="34" t="s">
+        <v>101</v>
+      </c>
+      <c r="D38" s="31" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="39" spans="1:23" ht="75">
+      <c r="A39" s="39"/>
+      <c r="B39" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="C39" s="29" t="s">
+        <v>104</v>
+      </c>
+      <c r="D39" s="20" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="40" spans="1:23" ht="60">
+      <c r="A40" s="39"/>
+      <c r="B40" s="33" t="s">
+        <v>102</v>
+      </c>
+      <c r="C40" s="34" t="s">
+        <v>105</v>
+      </c>
+      <c r="D40" s="31" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="41" spans="1:23" ht="45">
+      <c r="A41" s="43" t="s">
+        <v>120</v>
+      </c>
+      <c r="B41" s="35" t="s">
+        <v>107</v>
+      </c>
+      <c r="C41" s="29" t="s">
+        <v>117</v>
+      </c>
+      <c r="D41" s="20" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="42" spans="1:23" ht="75">
+      <c r="A42" s="44"/>
+      <c r="B42" s="33" t="s">
         <v>108</v>
       </c>
-      <c r="D32" s="36" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="75">
-      <c r="A33" s="22" t="s">
-        <v>102</v>
-      </c>
-      <c r="B33" s="40" t="s">
-        <v>99</v>
-      </c>
-      <c r="C33" s="33" t="s">
-        <v>105</v>
-      </c>
-      <c r="D33" s="21" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" ht="90">
-      <c r="A34" s="22"/>
-      <c r="B34" s="38" t="s">
-        <v>100</v>
-      </c>
-      <c r="C34" s="39" t="s">
-        <v>103</v>
-      </c>
-      <c r="D34" s="36" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" ht="75">
-      <c r="A35" s="22"/>
-      <c r="B35" s="20" t="s">
-        <v>101</v>
-      </c>
-      <c r="C35" s="33" t="s">
-        <v>106</v>
-      </c>
-      <c r="D35" s="21" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="60">
-      <c r="A36" s="22"/>
-      <c r="B36" s="38" t="s">
-        <v>104</v>
-      </c>
-      <c r="C36" s="39" t="s">
-        <v>107</v>
-      </c>
-      <c r="D36" s="36" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" ht="45">
-      <c r="A37" s="41" t="s">
-        <v>102</v>
-      </c>
-      <c r="B37" s="40" t="s">
+      <c r="C42" s="34" t="s">
+        <v>111</v>
+      </c>
+      <c r="D42" s="31" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="43" spans="1:23" ht="75">
+      <c r="A43" s="44"/>
+      <c r="B43" s="19" t="s">
         <v>109</v>
       </c>
-      <c r="C37" s="33" t="s">
-        <v>119</v>
-      </c>
-      <c r="D37" s="21" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" ht="75">
-      <c r="A38" s="42"/>
-      <c r="B38" s="38" t="s">
+      <c r="C43" s="29" t="s">
+        <v>112</v>
+      </c>
+      <c r="D43" s="20" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="44" spans="1:23" ht="120">
+      <c r="A44" s="44"/>
+      <c r="B44" s="33" t="s">
         <v>110</v>
       </c>
-      <c r="C38" s="39" t="s">
+      <c r="C44" s="34" t="s">
         <v>113</v>
       </c>
-      <c r="D38" s="36" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" ht="75">
-      <c r="A39" s="42"/>
-      <c r="B39" s="20" t="s">
-        <v>111</v>
-      </c>
-      <c r="C39" s="33" t="s">
+      <c r="D44" s="31" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="45" spans="1:23" ht="75">
+      <c r="A45" s="45"/>
+      <c r="B45" s="19" t="s">
         <v>114</v>
       </c>
-      <c r="D39" s="21" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" ht="120">
-      <c r="A40" s="42"/>
-      <c r="B40" s="38" t="s">
-        <v>112</v>
-      </c>
-      <c r="C40" s="39" t="s">
+      <c r="C45" s="29" t="s">
         <v>115</v>
       </c>
-      <c r="D40" s="36" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" ht="75">
-      <c r="A41" s="43"/>
-      <c r="B41" s="20" t="s">
-        <v>116</v>
-      </c>
-      <c r="C41" s="33" t="s">
-        <v>117</v>
-      </c>
-      <c r="D41" s="21" t="s">
-        <v>90</v>
+      <c r="D45" s="20" t="s">
+        <v>88</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="10">
-    <mergeCell ref="A37:A41"/>
-    <mergeCell ref="A30:A32"/>
-    <mergeCell ref="A33:A36"/>
+    <mergeCell ref="A41:A45"/>
+    <mergeCell ref="A34:A36"/>
+    <mergeCell ref="A37:A40"/>
     <mergeCell ref="A2:A10"/>
     <mergeCell ref="A23:A24"/>
-    <mergeCell ref="A27:A29"/>
+    <mergeCell ref="A31:A33"/>
     <mergeCell ref="A11:A13"/>
     <mergeCell ref="A14:A19"/>
     <mergeCell ref="A20:A21"/>
-    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="A25:A30"/>
   </mergeCells>
   <phoneticPr fontId="10" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation allowBlank="1" showDropDown="1" sqref="A20 A11 D2 D11 D14 A2 A23 A25 D20:D29"/>
+    <dataValidation allowBlank="1" showDropDown="1" sqref="A20 A11 D2 D11 D14 A2 A23 A25:A29 D20:D33"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1760,8 +1908,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1830,13 +1978,13 @@
     </row>
     <row r="5" spans="1:4" ht="37.5">
       <c r="A5" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D5" s="4">
         <v>45759</v>
@@ -1844,13 +1992,13 @@
     </row>
     <row r="6" spans="1:4" ht="37.5">
       <c r="A6" s="5" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D6" s="4">
         <v>45765</v>
@@ -1858,13 +2006,13 @@
     </row>
     <row r="7" spans="1:4" ht="18.75">
       <c r="A7" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D7" s="4">
         <v>45766</v>
@@ -1872,13 +2020,13 @@
     </row>
     <row r="8" spans="1:4" ht="18.75">
       <c r="A8" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D8" s="4">
         <v>45768</v>
@@ -1886,13 +2034,13 @@
     </row>
     <row r="9" spans="1:4" ht="18.75">
       <c r="A9" s="5" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>85</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>87</v>
       </c>
       <c r="D9" s="4">
         <v>45776</v>
@@ -1900,13 +2048,13 @@
     </row>
     <row r="10" spans="1:4" ht="18.75">
       <c r="A10" s="5" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D10" s="4">
         <v>45776</v>
@@ -1914,13 +2062,13 @@
     </row>
     <row r="11" spans="1:4" ht="18.75">
       <c r="A11" s="5" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D11" s="4">
         <v>45777</v>

</xml_diff>

<commit_message>
v2.3 Updating Deleting post according to review
Updating Admin Constraints "Delete post feature" according review comments
</commit_message>
<xml_diff>
--- a/LH_REQUIREMENTS/LH_CRS.xlsx
+++ b/LH_REQUIREMENTS/LH_CRS.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20417"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F96D4A0C-CB2C-43F4-9C31-6212E56686F8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="3870" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="LH_CRS" sheetId="1" r:id="rId1"/>
@@ -21,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="142">
   <si>
     <t>ID</t>
   </si>
@@ -417,33 +416,18 @@
     <t>LH-CRS-DELETEPOST-001</t>
   </si>
   <si>
-    <t>Admin have the ability to delete any post ( "articles" ," videos", "audio") throw delete post page</t>
-  </si>
-  <si>
     <t>LH-CRS-DELETEPOST-002</t>
   </si>
   <si>
-    <t>Admin can delete a post by searching about posts of any user by its username</t>
-  </si>
-  <si>
     <t>LH-CRS-DELETEPOST-003</t>
   </si>
   <si>
-    <t>an informative message will appear if there is no posts of username that you search by it</t>
-  </si>
-  <si>
     <t>LH-CRS-DELETEPOST-004</t>
   </si>
   <si>
-    <t>an informative message will appear if username that you search by it not found</t>
-  </si>
-  <si>
     <t>LH-CRS-DELETEPOST-005</t>
   </si>
   <si>
-    <t>Admin can go back to admin home page by clicking the logo pf the website</t>
-  </si>
-  <si>
     <t>v2.0</t>
   </si>
   <si>
@@ -453,16 +437,37 @@
     <t>Updating ADMINHOME CRS, USERHOME and PUBLISHVIDEO</t>
   </si>
   <si>
-    <t>Upadting Admin Constraints adding Deleting post feature</t>
-  </si>
-  <si>
     <t>v2.2</t>
+  </si>
+  <si>
+    <t>The admin has the ability to delete any post (articles, videos, or audio recordings) through the 'Delete Post' page."</t>
+  </si>
+  <si>
+    <t>The admin can delete a post by searching for a user's posts using their username.</t>
+  </si>
+  <si>
+    <t>If no posts are found for the entered username, an informative message must be displayed.</t>
+  </si>
+  <si>
+    <t>If the entered username does not exist in the system, an informative message must be displayed.</t>
+  </si>
+  <si>
+    <t>The admin can return to the admin home page by clicking the website logo.</t>
+  </si>
+  <si>
+    <t>v2.3</t>
+  </si>
+  <si>
+    <t>Updating Admin Constraints adding "Delete post feature"</t>
+  </si>
+  <si>
+    <t>Updating Admin Constraints "Delete post feature" according review comments</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="10">
     <font>
       <sz val="11"/>
@@ -751,6 +756,33 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -760,38 +792,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1072,11 +1077,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X48"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="83" zoomScaleNormal="76" workbookViewId="0">
-      <selection activeCell="C45" sqref="C45"/>
+    <sheetView topLeftCell="A40" zoomScale="83" zoomScaleNormal="76" workbookViewId="0">
+      <selection activeCell="C51" sqref="C51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -1103,7 +1108,7 @@
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="39" t="s">
         <v>114</v>
       </c>
       <c r="B2" s="26" t="s">
@@ -1117,7 +1122,7 @@
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="45"/>
+      <c r="A3" s="39"/>
       <c r="B3" s="27" t="s">
         <v>19</v>
       </c>
@@ -1129,7 +1134,7 @@
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="45"/>
+      <c r="A4" s="39"/>
       <c r="B4" s="26" t="s">
         <v>20</v>
       </c>
@@ -1141,7 +1146,7 @@
       </c>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="45"/>
+      <c r="A5" s="39"/>
       <c r="B5" s="27" t="s">
         <v>21</v>
       </c>
@@ -1153,7 +1158,7 @@
       </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="45"/>
+      <c r="A6" s="39"/>
       <c r="B6" s="26" t="s">
         <v>22</v>
       </c>
@@ -1165,7 +1170,7 @@
       </c>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" s="45"/>
+      <c r="A7" s="39"/>
       <c r="B7" s="27" t="s">
         <v>23</v>
       </c>
@@ -1177,7 +1182,7 @@
       </c>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" s="45"/>
+      <c r="A8" s="39"/>
       <c r="B8" s="26" t="s">
         <v>49</v>
       </c>
@@ -1189,7 +1194,7 @@
       </c>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" s="45"/>
+      <c r="A9" s="39"/>
       <c r="B9" s="27" t="s">
         <v>51</v>
       </c>
@@ -1201,7 +1206,7 @@
       </c>
     </row>
     <row r="10" spans="1:4">
-      <c r="A10" s="45"/>
+      <c r="A10" s="39"/>
       <c r="B10" s="26" t="s">
         <v>52</v>
       </c>
@@ -1213,7 +1218,7 @@
       </c>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11" s="44" t="s">
+      <c r="A11" s="40" t="s">
         <v>115</v>
       </c>
       <c r="B11" s="26" t="s">
@@ -1227,7 +1232,7 @@
       </c>
     </row>
     <row r="12" spans="1:4">
-      <c r="A12" s="44"/>
+      <c r="A12" s="40"/>
       <c r="B12" s="27" t="s">
         <v>12</v>
       </c>
@@ -1239,7 +1244,7 @@
       </c>
     </row>
     <row r="13" spans="1:4">
-      <c r="A13" s="44"/>
+      <c r="A13" s="40"/>
       <c r="B13" s="26" t="s">
         <v>25</v>
       </c>
@@ -1251,7 +1256,7 @@
       </c>
     </row>
     <row r="14" spans="1:4">
-      <c r="A14" s="40" t="s">
+      <c r="A14" s="41" t="s">
         <v>116</v>
       </c>
       <c r="B14" s="30" t="s">
@@ -1277,7 +1282,7 @@
       </c>
     </row>
     <row r="16" spans="1:4">
-      <c r="A16" s="43" t="s">
+      <c r="A16" s="50" t="s">
         <v>117</v>
       </c>
       <c r="B16" s="29" t="s">
@@ -1291,7 +1296,7 @@
       </c>
     </row>
     <row r="17" spans="1:24">
-      <c r="A17" s="43" t="s">
+      <c r="A17" s="50" t="s">
         <v>6</v>
       </c>
       <c r="B17" s="26" t="s">
@@ -1305,7 +1310,7 @@
       </c>
     </row>
     <row r="18" spans="1:24">
-      <c r="A18" s="43"/>
+      <c r="A18" s="50"/>
       <c r="B18" s="27" t="s">
         <v>53</v>
       </c>
@@ -1316,82 +1321,82 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:24">
-      <c r="A19" s="46" t="s">
+    <row r="19" spans="1:24" ht="30">
+      <c r="A19" s="43" t="s">
         <v>118</v>
       </c>
       <c r="B19" s="26" t="s">
         <v>125</v>
       </c>
       <c r="C19" s="22" t="s">
+        <v>134</v>
+      </c>
+      <c r="D19" s="23" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:24">
+      <c r="A20" s="44"/>
+      <c r="B20" s="37" t="s">
         <v>126</v>
       </c>
-      <c r="D19" s="23" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="20" spans="1:24">
-      <c r="A20" s="47"/>
-      <c r="B20" s="49" t="s">
+      <c r="C20" s="20" t="s">
+        <v>135</v>
+      </c>
+      <c r="D20" s="38" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:24">
+      <c r="A21" s="44"/>
+      <c r="B21" s="26" t="s">
         <v>127</v>
       </c>
-      <c r="C20" s="20" t="s">
+      <c r="C21" s="22" t="s">
+        <v>136</v>
+      </c>
+      <c r="D21" s="23" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:24">
+      <c r="A22" s="44"/>
+      <c r="B22" s="37" t="s">
         <v>128</v>
       </c>
-      <c r="D20" s="50" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="21" spans="1:24">
-      <c r="A21" s="47"/>
-      <c r="B21" s="26" t="s">
+      <c r="C22" s="20" t="s">
+        <v>137</v>
+      </c>
+      <c r="D22" s="38" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:24" ht="15" customHeight="1">
+      <c r="A23" s="44"/>
+      <c r="B23" s="26" t="s">
         <v>129</v>
       </c>
-      <c r="C21" s="22" t="s">
-        <v>130</v>
-      </c>
-      <c r="D21" s="23" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="22" spans="1:24">
-      <c r="A22" s="47"/>
-      <c r="B22" s="49" t="s">
-        <v>131</v>
-      </c>
-      <c r="C22" s="20" t="s">
-        <v>132</v>
-      </c>
-      <c r="D22" s="50" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="23" spans="1:24" ht="15" customHeight="1">
-      <c r="A23" s="47"/>
-      <c r="B23" s="26" t="s">
-        <v>133</v>
-      </c>
       <c r="C23" s="22" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="D23" s="23" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="24" spans="1:24" s="11" customFormat="1">
-      <c r="A24" s="48"/>
-      <c r="B24" s="49" t="s">
+      <c r="A24" s="45"/>
+      <c r="B24" s="37" t="s">
         <v>40</v>
       </c>
       <c r="C24" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="D24" s="50" t="s">
+      <c r="D24" s="38" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="25" spans="1:24" s="12" customFormat="1" ht="45">
-      <c r="A25" s="44" t="s">
+      <c r="A25" s="40" t="s">
         <v>119</v>
       </c>
       <c r="B25" s="26" t="s">
@@ -1425,7 +1430,7 @@
       <c r="X25" s="10"/>
     </row>
     <row r="26" spans="1:24" s="11" customFormat="1" ht="45">
-      <c r="A26" s="44"/>
+      <c r="A26" s="40"/>
       <c r="B26" s="29" t="s">
         <v>44</v>
       </c>
@@ -1457,7 +1462,7 @@
       <c r="X26" s="10"/>
     </row>
     <row r="27" spans="1:24" s="12" customFormat="1" ht="30">
-      <c r="A27" s="44"/>
+      <c r="A27" s="40"/>
       <c r="B27" s="26" t="s">
         <v>45</v>
       </c>
@@ -1489,7 +1494,7 @@
       <c r="X27" s="10"/>
     </row>
     <row r="28" spans="1:24" s="12" customFormat="1" ht="78.75" customHeight="1">
-      <c r="A28" s="40" t="s">
+      <c r="A28" s="41" t="s">
         <v>120</v>
       </c>
       <c r="B28" s="27" t="s">
@@ -1523,7 +1528,7 @@
       <c r="X28" s="10"/>
     </row>
     <row r="29" spans="1:24" s="11" customFormat="1" ht="34.5" customHeight="1">
-      <c r="A29" s="41"/>
+      <c r="A29" s="49"/>
       <c r="B29" s="26" t="s">
         <v>71</v>
       </c>
@@ -1587,7 +1592,7 @@
       <c r="X30" s="10"/>
     </row>
     <row r="31" spans="1:24" s="11" customFormat="1" ht="45" customHeight="1">
-      <c r="A31" s="44" t="s">
+      <c r="A31" s="40" t="s">
         <v>121</v>
       </c>
       <c r="B31" s="26" t="s">
@@ -1621,7 +1626,7 @@
       <c r="X31" s="10"/>
     </row>
     <row r="32" spans="1:24" s="12" customFormat="1" ht="48.75" customHeight="1">
-      <c r="A32" s="44"/>
+      <c r="A32" s="40"/>
       <c r="B32" s="27" t="s">
         <v>76</v>
       </c>
@@ -1653,7 +1658,7 @@
       <c r="X32" s="10"/>
     </row>
     <row r="33" spans="1:24" s="12" customFormat="1" ht="35.25" customHeight="1">
-      <c r="A33" s="44"/>
+      <c r="A33" s="40"/>
       <c r="B33" s="26" t="s">
         <v>77</v>
       </c>
@@ -1685,7 +1690,7 @@
       <c r="X33" s="10"/>
     </row>
     <row r="34" spans="1:24" ht="21" customHeight="1">
-      <c r="A34" s="44"/>
+      <c r="A34" s="40"/>
       <c r="B34" s="31" t="s">
         <v>79</v>
       </c>
@@ -1697,7 +1702,7 @@
       </c>
     </row>
     <row r="35" spans="1:24" ht="45">
-      <c r="A35" s="40" t="s">
+      <c r="A35" s="41" t="s">
         <v>122</v>
       </c>
       <c r="B35" s="26" t="s">
@@ -1711,7 +1716,7 @@
       </c>
     </row>
     <row r="36" spans="1:24" ht="38.25" customHeight="1">
-      <c r="A36" s="41"/>
+      <c r="A36" s="49"/>
       <c r="B36" s="27" t="s">
         <v>85</v>
       </c>
@@ -1723,7 +1728,7 @@
       </c>
     </row>
     <row r="37" spans="1:24" ht="48.75" customHeight="1">
-      <c r="A37" s="41"/>
+      <c r="A37" s="49"/>
       <c r="B37" s="26" t="s">
         <v>86</v>
       </c>
@@ -1735,7 +1740,7 @@
       </c>
     </row>
     <row r="38" spans="1:24" ht="50.25" customHeight="1">
-      <c r="A38" s="41"/>
+      <c r="A38" s="49"/>
       <c r="B38" s="27" t="s">
         <v>87</v>
       </c>
@@ -1759,7 +1764,7 @@
       </c>
     </row>
     <row r="40" spans="1:24" ht="30">
-      <c r="A40" s="37" t="s">
+      <c r="A40" s="46" t="s">
         <v>123</v>
       </c>
       <c r="B40" s="27" t="s">
@@ -1773,7 +1778,7 @@
       </c>
     </row>
     <row r="41" spans="1:24" ht="30">
-      <c r="A41" s="38"/>
+      <c r="A41" s="47"/>
       <c r="B41" s="26" t="s">
         <v>96</v>
       </c>
@@ -1785,7 +1790,7 @@
       </c>
     </row>
     <row r="42" spans="1:24">
-      <c r="A42" s="38"/>
+      <c r="A42" s="47"/>
       <c r="B42" s="27" t="s">
         <v>97</v>
       </c>
@@ -1797,7 +1802,7 @@
       </c>
     </row>
     <row r="43" spans="1:24" ht="45">
-      <c r="A43" s="38"/>
+      <c r="A43" s="47"/>
       <c r="B43" s="26" t="s">
         <v>98</v>
       </c>
@@ -1809,7 +1814,7 @@
       </c>
     </row>
     <row r="44" spans="1:24" ht="30">
-      <c r="A44" s="39"/>
+      <c r="A44" s="48"/>
       <c r="B44" s="27" t="s">
         <v>99</v>
       </c>
@@ -1821,7 +1826,7 @@
       </c>
     </row>
     <row r="45" spans="1:24" ht="45">
-      <c r="A45" s="40" t="s">
+      <c r="A45" s="41" t="s">
         <v>124</v>
       </c>
       <c r="B45" s="26" t="s">
@@ -1835,7 +1840,7 @@
       </c>
     </row>
     <row r="46" spans="1:24" ht="30">
-      <c r="A46" s="41"/>
+      <c r="A46" s="49"/>
       <c r="B46" s="27" t="s">
         <v>104</v>
       </c>
@@ -1847,7 +1852,7 @@
       </c>
     </row>
     <row r="47" spans="1:24" ht="45">
-      <c r="A47" s="41"/>
+      <c r="A47" s="49"/>
       <c r="B47" s="26" t="s">
         <v>105</v>
       </c>
@@ -1872,21 +1877,21 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A2:A10"/>
-    <mergeCell ref="A25:A27"/>
-    <mergeCell ref="A11:A13"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="A19:A24"/>
     <mergeCell ref="A40:A44"/>
     <mergeCell ref="A45:A48"/>
     <mergeCell ref="A16:A18"/>
     <mergeCell ref="A35:A39"/>
     <mergeCell ref="A28:A30"/>
     <mergeCell ref="A31:A34"/>
+    <mergeCell ref="A2:A10"/>
+    <mergeCell ref="A25:A27"/>
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="A19:A24"/>
   </mergeCells>
   <phoneticPr fontId="9" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation allowBlank="1" showDropDown="1" sqref="A14 A11 D2 D11 A2 A17 A19 D45 D41 D43 D14:D27" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
+    <dataValidation allowBlank="1" showDropDown="1" sqref="A14 A11 D2 D11 A2 A17 A19 D45 D41 D43 D14:D27"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1894,11 +1899,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2037,13 +2042,13 @@
     </row>
     <row r="10" spans="1:4" ht="37.5">
       <c r="A10" s="5" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>68</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="D10" s="2">
         <v>45776</v>
@@ -2051,13 +2056,13 @@
     </row>
     <row r="11" spans="1:4" ht="37.5">
       <c r="A11" s="6" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="D11" s="4">
         <v>45777</v>
@@ -2065,7 +2070,7 @@
     </row>
     <row r="12" spans="1:4" ht="56.25">
       <c r="A12" s="5" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>64</v>
@@ -2074,6 +2079,20 @@
         <v>113</v>
       </c>
       <c r="D12" s="2">
+        <v>45777</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="37.5">
+      <c r="A13" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="D13" s="2">
         <v>45777</v>
       </c>
     </row>

</xml_diff>

<commit_message>
V2.4 update the admin constrains by modifying the delete user constrains
</commit_message>
<xml_diff>
--- a/LH_REQUIREMENTS/LH_CRS.xlsx
+++ b/LH_REQUIREMENTS/LH_CRS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650"/>
   </bookViews>
   <sheets>
     <sheet name="LH_CRS" sheetId="1" r:id="rId1"/>
     <sheet name="LH_CRS_VERSION_HISTORY" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="154">
   <si>
     <t>ID</t>
   </si>
@@ -142,13 +142,7 @@
     <t>LH-CRS-ID-CONSTRAINS-001</t>
   </si>
   <si>
-    <t>LH-CRS-ADMIN-CONSTRAINS-001</t>
-  </si>
-  <si>
     <t>LH-CRS-NOTIFICATIONS-002</t>
-  </si>
-  <si>
-    <t>Admin features must include the ability to delete users.</t>
   </si>
   <si>
     <t>LH-CRS-LOGIN-001</t>
@@ -462,12 +456,54 @@
   </si>
   <si>
     <t>Updating Admin Constraints "Delete post feature" according review comments</t>
+  </si>
+  <si>
+    <t>LH-CRS-DELETEUSER_001</t>
+  </si>
+  <si>
+    <t>LH-CRS-DELETEUSER_002</t>
+  </si>
+  <si>
+    <t>LH-CRS-DELETEUSER_003</t>
+  </si>
+  <si>
+    <t>LH-CRS-DELETEUSER_004</t>
+  </si>
+  <si>
+    <t>LH-CRS-DELETEUSER_005</t>
+  </si>
+  <si>
+    <t>The admin has the ability to delete any user from the delete post page</t>
+  </si>
+  <si>
+    <t>The admin can search about the user by their username</t>
+  </si>
+  <si>
+    <t>the username ind the id of the user should apear after the admin search</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the system should show message if the user is not exist </t>
+  </si>
+  <si>
+    <t>the system should delete the user posts related to this user name</t>
+  </si>
+  <si>
+    <t>LH-CRS-DELETEUSER_006</t>
+  </si>
+  <si>
+    <t>the system should still an the same page after deleting a user</t>
+  </si>
+  <si>
+    <t>LH-CRS-DELETEUSER_007</t>
+  </si>
+  <si>
+    <t>the admin can take sure the user is already deleted by refresh and search by the same username</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="10">
     <font>
       <sz val="11"/>
@@ -652,7 +688,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -762,40 +798,37 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -858,7 +891,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -893,7 +926,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1070,7 +1103,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1078,10 +1111,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X48"/>
+  <dimension ref="A1:X54"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" zoomScale="83" zoomScaleNormal="76" workbookViewId="0">
-      <selection activeCell="C51" sqref="C51"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="83" zoomScaleNormal="76" workbookViewId="0">
+      <selection activeCell="B31" sqref="A31:XFD31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -1108,8 +1141,8 @@
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="39" t="s">
-        <v>114</v>
+      <c r="A2" s="47" t="s">
+        <v>112</v>
       </c>
       <c r="B2" s="26" t="s">
         <v>11</v>
@@ -1122,7 +1155,7 @@
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="39"/>
+      <c r="A3" s="47"/>
       <c r="B3" s="27" t="s">
         <v>19</v>
       </c>
@@ -1134,7 +1167,7 @@
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="39"/>
+      <c r="A4" s="47"/>
       <c r="B4" s="26" t="s">
         <v>20</v>
       </c>
@@ -1146,7 +1179,7 @@
       </c>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="39"/>
+      <c r="A5" s="47"/>
       <c r="B5" s="27" t="s">
         <v>21</v>
       </c>
@@ -1158,7 +1191,7 @@
       </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="39"/>
+      <c r="A6" s="47"/>
       <c r="B6" s="26" t="s">
         <v>22</v>
       </c>
@@ -1170,7 +1203,7 @@
       </c>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" s="39"/>
+      <c r="A7" s="47"/>
       <c r="B7" s="27" t="s">
         <v>23</v>
       </c>
@@ -1182,44 +1215,44 @@
       </c>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" s="39"/>
+      <c r="A8" s="47"/>
       <c r="B8" s="26" t="s">
+        <v>47</v>
+      </c>
+      <c r="C8" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="D8" s="34" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="47"/>
+      <c r="B9" s="27" t="s">
         <v>49</v>
       </c>
-      <c r="C8" s="17" t="s">
-        <v>48</v>
-      </c>
-      <c r="D8" s="34" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" s="39"/>
-      <c r="B9" s="27" t="s">
-        <v>51</v>
-      </c>
       <c r="C9" s="18" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D9" s="16" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:4">
-      <c r="A10" s="39"/>
+      <c r="A10" s="47"/>
       <c r="B10" s="26" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C10" s="17" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D10" s="34" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11" s="40" t="s">
-        <v>115</v>
+      <c r="A11" s="46" t="s">
+        <v>113</v>
       </c>
       <c r="B11" s="26" t="s">
         <v>24</v>
@@ -1232,7 +1265,7 @@
       </c>
     </row>
     <row r="12" spans="1:4">
-      <c r="A12" s="40"/>
+      <c r="A12" s="46"/>
       <c r="B12" s="27" t="s">
         <v>12</v>
       </c>
@@ -1244,7 +1277,7 @@
       </c>
     </row>
     <row r="13" spans="1:4">
-      <c r="A13" s="40"/>
+      <c r="A13" s="46"/>
       <c r="B13" s="26" t="s">
         <v>25</v>
       </c>
@@ -1256,8 +1289,8 @@
       </c>
     </row>
     <row r="14" spans="1:4">
-      <c r="A14" s="41" t="s">
-        <v>116</v>
+      <c r="A14" s="42" t="s">
+        <v>114</v>
       </c>
       <c r="B14" s="30" t="s">
         <v>37</v>
@@ -1270,33 +1303,33 @@
       </c>
     </row>
     <row r="15" spans="1:4">
-      <c r="A15" s="42"/>
+      <c r="A15" s="44"/>
       <c r="B15" s="26" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C15" s="22" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D15" s="23" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:4">
-      <c r="A16" s="50" t="s">
-        <v>117</v>
+      <c r="A16" s="45" t="s">
+        <v>115</v>
       </c>
       <c r="B16" s="29" t="s">
         <v>38</v>
       </c>
       <c r="C16" s="20" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D16" s="36" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:24">
-      <c r="A17" s="50" t="s">
+      <c r="A17" s="45" t="s">
         <v>6</v>
       </c>
       <c r="B17" s="26" t="s">
@@ -1310,299 +1343,161 @@
       </c>
     </row>
     <row r="18" spans="1:24">
-      <c r="A18" s="50"/>
+      <c r="A18" s="45"/>
       <c r="B18" s="27" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C18" s="18" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D18" s="16" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="19" spans="1:24" ht="30">
-      <c r="A19" s="43" t="s">
-        <v>118</v>
+      <c r="A19" s="48" t="s">
+        <v>116</v>
       </c>
       <c r="B19" s="26" t="s">
+        <v>123</v>
+      </c>
+      <c r="C19" s="22" t="s">
+        <v>132</v>
+      </c>
+      <c r="D19" s="23" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:24">
+      <c r="A20" s="49"/>
+      <c r="B20" s="37" t="s">
+        <v>124</v>
+      </c>
+      <c r="C20" s="20" t="s">
+        <v>133</v>
+      </c>
+      <c r="D20" s="38" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:24">
+      <c r="A21" s="49"/>
+      <c r="B21" s="26" t="s">
         <v>125</v>
       </c>
-      <c r="C19" s="22" t="s">
+      <c r="C21" s="22" t="s">
         <v>134</v>
       </c>
-      <c r="D19" s="23" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="20" spans="1:24">
-      <c r="A20" s="44"/>
-      <c r="B20" s="37" t="s">
+      <c r="D21" s="23" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:24">
+      <c r="A22" s="49"/>
+      <c r="B22" s="37" t="s">
         <v>126</v>
       </c>
-      <c r="C20" s="20" t="s">
+      <c r="C22" s="20" t="s">
         <v>135</v>
       </c>
-      <c r="D20" s="38" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="21" spans="1:24">
-      <c r="A21" s="44"/>
-      <c r="B21" s="26" t="s">
+      <c r="D22" s="38" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:24" ht="15" customHeight="1">
+      <c r="A23" s="49"/>
+      <c r="B23" s="26" t="s">
         <v>127</v>
       </c>
-      <c r="C21" s="22" t="s">
+      <c r="C23" s="22" t="s">
         <v>136</v>
       </c>
-      <c r="D21" s="23" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="22" spans="1:24">
-      <c r="A22" s="44"/>
-      <c r="B22" s="37" t="s">
-        <v>128</v>
-      </c>
-      <c r="C22" s="20" t="s">
-        <v>137</v>
-      </c>
-      <c r="D22" s="38" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="23" spans="1:24" ht="15" customHeight="1">
-      <c r="A23" s="44"/>
-      <c r="B23" s="26" t="s">
-        <v>129</v>
-      </c>
-      <c r="C23" s="22" t="s">
-        <v>138</v>
-      </c>
       <c r="D23" s="23" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:24" s="11" customFormat="1">
-      <c r="A24" s="45"/>
-      <c r="B24" s="37" t="s">
-        <v>40</v>
-      </c>
-      <c r="C24" s="20" t="s">
-        <v>42</v>
-      </c>
-      <c r="D24" s="38" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="25" spans="1:24" s="12" customFormat="1" ht="45">
-      <c r="A25" s="40" t="s">
-        <v>119</v>
-      </c>
+    <row r="24" spans="1:24" ht="15" customHeight="1">
+      <c r="A24" s="49"/>
+      <c r="B24" s="26" t="s">
+        <v>140</v>
+      </c>
+      <c r="C24" s="22" t="s">
+        <v>145</v>
+      </c>
+      <c r="D24" s="23"/>
+    </row>
+    <row r="25" spans="1:24" ht="15" customHeight="1">
+      <c r="A25" s="49"/>
       <c r="B25" s="26" t="s">
-        <v>43</v>
+        <v>141</v>
       </c>
       <c r="C25" s="22" t="s">
-        <v>67</v>
-      </c>
-      <c r="D25" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="E25" s="10"/>
-      <c r="F25" s="10"/>
-      <c r="G25" s="10"/>
-      <c r="H25" s="10"/>
-      <c r="I25" s="10"/>
-      <c r="J25" s="10"/>
-      <c r="K25" s="10"/>
-      <c r="L25" s="10"/>
-      <c r="M25" s="10"/>
-      <c r="N25" s="10"/>
-      <c r="O25" s="10"/>
-      <c r="P25" s="10"/>
-      <c r="Q25" s="10"/>
-      <c r="R25" s="10"/>
-      <c r="S25" s="10"/>
-      <c r="T25" s="10"/>
-      <c r="U25" s="10"/>
-      <c r="V25" s="10"/>
-      <c r="W25" s="10"/>
-      <c r="X25" s="10"/>
-    </row>
-    <row r="26" spans="1:24" s="11" customFormat="1" ht="45">
-      <c r="A26" s="40"/>
-      <c r="B26" s="29" t="s">
-        <v>44</v>
-      </c>
-      <c r="C26" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="D26" s="36" t="s">
-        <v>64</v>
-      </c>
-      <c r="E26" s="10"/>
-      <c r="F26" s="10"/>
-      <c r="G26" s="10"/>
-      <c r="H26" s="10"/>
-      <c r="I26" s="10"/>
-      <c r="J26" s="10"/>
-      <c r="K26" s="10"/>
-      <c r="L26" s="10"/>
-      <c r="M26" s="10"/>
-      <c r="N26" s="10"/>
-      <c r="O26" s="10"/>
-      <c r="P26" s="10"/>
-      <c r="Q26" s="10"/>
-      <c r="R26" s="10"/>
-      <c r="S26" s="10"/>
-      <c r="T26" s="10"/>
-      <c r="U26" s="10"/>
-      <c r="V26" s="10"/>
-      <c r="W26" s="10"/>
-      <c r="X26" s="10"/>
-    </row>
-    <row r="27" spans="1:24" s="12" customFormat="1" ht="30">
-      <c r="A27" s="40"/>
+        <v>146</v>
+      </c>
+      <c r="D25" s="23"/>
+    </row>
+    <row r="26" spans="1:24" ht="15" customHeight="1">
+      <c r="A26" s="49"/>
+      <c r="B26" s="26" t="s">
+        <v>142</v>
+      </c>
+      <c r="C26" s="22" t="s">
+        <v>147</v>
+      </c>
+      <c r="D26" s="23"/>
+    </row>
+    <row r="27" spans="1:24" ht="15" customHeight="1">
+      <c r="A27" s="49"/>
       <c r="B27" s="26" t="s">
-        <v>45</v>
+        <v>143</v>
       </c>
       <c r="C27" s="22" t="s">
-        <v>63</v>
-      </c>
-      <c r="D27" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="E27" s="10"/>
-      <c r="F27" s="10"/>
-      <c r="G27" s="10"/>
-      <c r="H27" s="10"/>
-      <c r="I27" s="10"/>
-      <c r="J27" s="10"/>
-      <c r="K27" s="10"/>
-      <c r="L27" s="10"/>
-      <c r="M27" s="10"/>
-      <c r="N27" s="10"/>
-      <c r="O27" s="10"/>
-      <c r="P27" s="10"/>
-      <c r="Q27" s="10"/>
-      <c r="R27" s="10"/>
-      <c r="S27" s="10"/>
-      <c r="T27" s="10"/>
-      <c r="U27" s="10"/>
-      <c r="V27" s="10"/>
-      <c r="W27" s="10"/>
-      <c r="X27" s="10"/>
-    </row>
-    <row r="28" spans="1:24" s="12" customFormat="1" ht="78.75" customHeight="1">
-      <c r="A28" s="41" t="s">
-        <v>120</v>
-      </c>
-      <c r="B28" s="27" t="s">
-        <v>69</v>
-      </c>
-      <c r="C28" s="21" t="s">
-        <v>70</v>
-      </c>
-      <c r="D28" s="16" t="s">
-        <v>68</v>
-      </c>
-      <c r="E28" s="10"/>
-      <c r="F28" s="10"/>
-      <c r="G28" s="10"/>
-      <c r="H28" s="10"/>
-      <c r="I28" s="10"/>
-      <c r="J28" s="10"/>
-      <c r="K28" s="10"/>
-      <c r="L28" s="10"/>
-      <c r="M28" s="10"/>
-      <c r="N28" s="10"/>
-      <c r="O28" s="10"/>
-      <c r="P28" s="10"/>
-      <c r="Q28" s="10"/>
-      <c r="R28" s="10"/>
-      <c r="S28" s="10"/>
-      <c r="T28" s="10"/>
-      <c r="U28" s="10"/>
-      <c r="V28" s="10"/>
-      <c r="W28" s="10"/>
-      <c r="X28" s="10"/>
-    </row>
-    <row r="29" spans="1:24" s="11" customFormat="1" ht="34.5" customHeight="1">
+        <v>148</v>
+      </c>
+      <c r="D27" s="23"/>
+    </row>
+    <row r="28" spans="1:24" ht="15" customHeight="1">
+      <c r="A28" s="49"/>
+      <c r="B28" s="26" t="s">
+        <v>144</v>
+      </c>
+      <c r="C28" s="22" t="s">
+        <v>149</v>
+      </c>
+      <c r="D28" s="23"/>
+    </row>
+    <row r="29" spans="1:24" ht="15" customHeight="1">
       <c r="A29" s="49"/>
       <c r="B29" s="26" t="s">
-        <v>71</v>
+        <v>150</v>
       </c>
       <c r="C29" s="22" t="s">
-        <v>73</v>
-      </c>
-      <c r="D29" s="23" t="s">
-        <v>68</v>
-      </c>
-      <c r="E29" s="10"/>
-      <c r="F29" s="10"/>
-      <c r="G29" s="10"/>
-      <c r="H29" s="10"/>
-      <c r="I29" s="10"/>
-      <c r="J29" s="10"/>
-      <c r="K29" s="10"/>
-      <c r="L29" s="10"/>
-      <c r="M29" s="10"/>
-      <c r="N29" s="10"/>
-      <c r="O29" s="10"/>
-      <c r="P29" s="10"/>
-      <c r="Q29" s="10"/>
-      <c r="R29" s="10"/>
-      <c r="S29" s="10"/>
-      <c r="T29" s="10"/>
-      <c r="U29" s="10"/>
-      <c r="V29" s="10"/>
-      <c r="W29" s="10"/>
-      <c r="X29" s="10"/>
-    </row>
-    <row r="30" spans="1:24" s="12" customFormat="1" ht="34.5" customHeight="1">
-      <c r="A30" s="42"/>
-      <c r="B30" s="27" t="s">
-        <v>72</v>
-      </c>
-      <c r="C30" s="21" t="s">
-        <v>83</v>
-      </c>
-      <c r="D30" s="16" t="s">
-        <v>68</v>
-      </c>
-      <c r="E30" s="10"/>
-      <c r="F30" s="10"/>
-      <c r="G30" s="10"/>
-      <c r="H30" s="10"/>
-      <c r="I30" s="10"/>
-      <c r="J30" s="10"/>
-      <c r="K30" s="10"/>
-      <c r="L30" s="10"/>
-      <c r="M30" s="10"/>
-      <c r="N30" s="10"/>
-      <c r="O30" s="10"/>
-      <c r="P30" s="10"/>
-      <c r="Q30" s="10"/>
-      <c r="R30" s="10"/>
-      <c r="S30" s="10"/>
-      <c r="T30" s="10"/>
-      <c r="U30" s="10"/>
-      <c r="V30" s="10"/>
-      <c r="W30" s="10"/>
-      <c r="X30" s="10"/>
-    </row>
-    <row r="31" spans="1:24" s="11" customFormat="1" ht="45" customHeight="1">
-      <c r="A31" s="40" t="s">
-        <v>121</v>
+        <v>151</v>
+      </c>
+      <c r="D29" s="23"/>
+    </row>
+    <row r="30" spans="1:24" ht="15" customHeight="1">
+      <c r="A30" s="49"/>
+      <c r="B30" s="26" t="s">
+        <v>152</v>
+      </c>
+      <c r="C30" s="22" t="s">
+        <v>153</v>
+      </c>
+      <c r="D30" s="23"/>
+    </row>
+    <row r="31" spans="1:24" s="12" customFormat="1" ht="45">
+      <c r="A31" s="46" t="s">
+        <v>117</v>
       </c>
       <c r="B31" s="26" t="s">
-        <v>75</v>
+        <v>41</v>
       </c>
       <c r="C31" s="22" t="s">
-        <v>80</v>
+        <v>65</v>
       </c>
       <c r="D31" s="23" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="E31" s="10"/>
       <c r="F31" s="10"/>
@@ -1625,16 +1520,16 @@
       <c r="W31" s="10"/>
       <c r="X31" s="10"/>
     </row>
-    <row r="32" spans="1:24" s="12" customFormat="1" ht="48.75" customHeight="1">
-      <c r="A32" s="40"/>
-      <c r="B32" s="27" t="s">
-        <v>76</v>
+    <row r="32" spans="1:24" s="11" customFormat="1" ht="45">
+      <c r="A32" s="46"/>
+      <c r="B32" s="29" t="s">
+        <v>42</v>
       </c>
       <c r="C32" s="21" t="s">
-        <v>78</v>
-      </c>
-      <c r="D32" s="16" t="s">
-        <v>68</v>
+        <v>60</v>
+      </c>
+      <c r="D32" s="36" t="s">
+        <v>62</v>
       </c>
       <c r="E32" s="10"/>
       <c r="F32" s="10"/>
@@ -1657,16 +1552,16 @@
       <c r="W32" s="10"/>
       <c r="X32" s="10"/>
     </row>
-    <row r="33" spans="1:24" s="12" customFormat="1" ht="35.25" customHeight="1">
-      <c r="A33" s="40"/>
+    <row r="33" spans="1:24" s="12" customFormat="1" ht="30">
+      <c r="A33" s="46"/>
       <c r="B33" s="26" t="s">
-        <v>77</v>
+        <v>43</v>
       </c>
       <c r="C33" s="22" t="s">
-        <v>81</v>
+        <v>61</v>
       </c>
       <c r="D33" s="23" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="E33" s="10"/>
       <c r="F33" s="10"/>
@@ -1689,209 +1584,405 @@
       <c r="W33" s="10"/>
       <c r="X33" s="10"/>
     </row>
-    <row r="34" spans="1:24" ht="21" customHeight="1">
-      <c r="A34" s="40"/>
-      <c r="B34" s="31" t="s">
+    <row r="34" spans="1:24" s="12" customFormat="1" ht="78.75" customHeight="1">
+      <c r="A34" s="42" t="s">
+        <v>118</v>
+      </c>
+      <c r="B34" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="C34" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="D34" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="E34" s="10"/>
+      <c r="F34" s="10"/>
+      <c r="G34" s="10"/>
+      <c r="H34" s="10"/>
+      <c r="I34" s="10"/>
+      <c r="J34" s="10"/>
+      <c r="K34" s="10"/>
+      <c r="L34" s="10"/>
+      <c r="M34" s="10"/>
+      <c r="N34" s="10"/>
+      <c r="O34" s="10"/>
+      <c r="P34" s="10"/>
+      <c r="Q34" s="10"/>
+      <c r="R34" s="10"/>
+      <c r="S34" s="10"/>
+      <c r="T34" s="10"/>
+      <c r="U34" s="10"/>
+      <c r="V34" s="10"/>
+      <c r="W34" s="10"/>
+      <c r="X34" s="10"/>
+    </row>
+    <row r="35" spans="1:24" s="11" customFormat="1" ht="34.5" customHeight="1">
+      <c r="A35" s="43"/>
+      <c r="B35" s="26" t="s">
+        <v>69</v>
+      </c>
+      <c r="C35" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="D35" s="23" t="s">
+        <v>66</v>
+      </c>
+      <c r="E35" s="10"/>
+      <c r="F35" s="10"/>
+      <c r="G35" s="10"/>
+      <c r="H35" s="10"/>
+      <c r="I35" s="10"/>
+      <c r="J35" s="10"/>
+      <c r="K35" s="10"/>
+      <c r="L35" s="10"/>
+      <c r="M35" s="10"/>
+      <c r="N35" s="10"/>
+      <c r="O35" s="10"/>
+      <c r="P35" s="10"/>
+      <c r="Q35" s="10"/>
+      <c r="R35" s="10"/>
+      <c r="S35" s="10"/>
+      <c r="T35" s="10"/>
+      <c r="U35" s="10"/>
+      <c r="V35" s="10"/>
+      <c r="W35" s="10"/>
+      <c r="X35" s="10"/>
+    </row>
+    <row r="36" spans="1:24" s="12" customFormat="1" ht="34.5" customHeight="1">
+      <c r="A36" s="44"/>
+      <c r="B36" s="27" t="s">
+        <v>70</v>
+      </c>
+      <c r="C36" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="D36" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="E36" s="10"/>
+      <c r="F36" s="10"/>
+      <c r="G36" s="10"/>
+      <c r="H36" s="10"/>
+      <c r="I36" s="10"/>
+      <c r="J36" s="10"/>
+      <c r="K36" s="10"/>
+      <c r="L36" s="10"/>
+      <c r="M36" s="10"/>
+      <c r="N36" s="10"/>
+      <c r="O36" s="10"/>
+      <c r="P36" s="10"/>
+      <c r="Q36" s="10"/>
+      <c r="R36" s="10"/>
+      <c r="S36" s="10"/>
+      <c r="T36" s="10"/>
+      <c r="U36" s="10"/>
+      <c r="V36" s="10"/>
+      <c r="W36" s="10"/>
+      <c r="X36" s="10"/>
+    </row>
+    <row r="37" spans="1:24" s="11" customFormat="1" ht="45" customHeight="1">
+      <c r="A37" s="46" t="s">
+        <v>119</v>
+      </c>
+      <c r="B37" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="C37" s="22" t="s">
+        <v>78</v>
+      </c>
+      <c r="D37" s="23" t="s">
+        <v>66</v>
+      </c>
+      <c r="E37" s="10"/>
+      <c r="F37" s="10"/>
+      <c r="G37" s="10"/>
+      <c r="H37" s="10"/>
+      <c r="I37" s="10"/>
+      <c r="J37" s="10"/>
+      <c r="K37" s="10"/>
+      <c r="L37" s="10"/>
+      <c r="M37" s="10"/>
+      <c r="N37" s="10"/>
+      <c r="O37" s="10"/>
+      <c r="P37" s="10"/>
+      <c r="Q37" s="10"/>
+      <c r="R37" s="10"/>
+      <c r="S37" s="10"/>
+      <c r="T37" s="10"/>
+      <c r="U37" s="10"/>
+      <c r="V37" s="10"/>
+      <c r="W37" s="10"/>
+      <c r="X37" s="10"/>
+    </row>
+    <row r="38" spans="1:24" s="12" customFormat="1" ht="48.75" customHeight="1">
+      <c r="A38" s="46"/>
+      <c r="B38" s="27" t="s">
+        <v>74</v>
+      </c>
+      <c r="C38" s="21" t="s">
+        <v>76</v>
+      </c>
+      <c r="D38" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="E38" s="10"/>
+      <c r="F38" s="10"/>
+      <c r="G38" s="10"/>
+      <c r="H38" s="10"/>
+      <c r="I38" s="10"/>
+      <c r="J38" s="10"/>
+      <c r="K38" s="10"/>
+      <c r="L38" s="10"/>
+      <c r="M38" s="10"/>
+      <c r="N38" s="10"/>
+      <c r="O38" s="10"/>
+      <c r="P38" s="10"/>
+      <c r="Q38" s="10"/>
+      <c r="R38" s="10"/>
+      <c r="S38" s="10"/>
+      <c r="T38" s="10"/>
+      <c r="U38" s="10"/>
+      <c r="V38" s="10"/>
+      <c r="W38" s="10"/>
+      <c r="X38" s="10"/>
+    </row>
+    <row r="39" spans="1:24" s="12" customFormat="1" ht="35.25" customHeight="1">
+      <c r="A39" s="46"/>
+      <c r="B39" s="26" t="s">
+        <v>75</v>
+      </c>
+      <c r="C39" s="22" t="s">
         <v>79</v>
       </c>
-      <c r="C34" s="21" t="s">
+      <c r="D39" s="23" t="s">
+        <v>66</v>
+      </c>
+      <c r="E39" s="10"/>
+      <c r="F39" s="10"/>
+      <c r="G39" s="10"/>
+      <c r="H39" s="10"/>
+      <c r="I39" s="10"/>
+      <c r="J39" s="10"/>
+      <c r="K39" s="10"/>
+      <c r="L39" s="10"/>
+      <c r="M39" s="10"/>
+      <c r="N39" s="10"/>
+      <c r="O39" s="10"/>
+      <c r="P39" s="10"/>
+      <c r="Q39" s="10"/>
+      <c r="R39" s="10"/>
+      <c r="S39" s="10"/>
+      <c r="T39" s="10"/>
+      <c r="U39" s="10"/>
+      <c r="V39" s="10"/>
+      <c r="W39" s="10"/>
+      <c r="X39" s="10"/>
+    </row>
+    <row r="40" spans="1:24" ht="21" customHeight="1">
+      <c r="A40" s="46"/>
+      <c r="B40" s="31" t="s">
+        <v>77</v>
+      </c>
+      <c r="C40" s="21" t="s">
+        <v>80</v>
+      </c>
+      <c r="D40" s="16" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="41" spans="1:24" ht="45">
+      <c r="A41" s="42" t="s">
+        <v>120</v>
+      </c>
+      <c r="B41" s="26" t="s">
         <v>82</v>
       </c>
-      <c r="D34" s="16" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="35" spans="1:24" ht="45">
-      <c r="A35" s="41" t="s">
+      <c r="C41" s="22" t="s">
+        <v>92</v>
+      </c>
+      <c r="D41" s="34" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="42" spans="1:24" ht="38.25" customHeight="1">
+      <c r="A42" s="43"/>
+      <c r="B42" s="27" t="s">
+        <v>83</v>
+      </c>
+      <c r="C42" s="21" t="s">
+        <v>86</v>
+      </c>
+      <c r="D42" s="16" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="43" spans="1:24" ht="48.75" customHeight="1">
+      <c r="A43" s="43"/>
+      <c r="B43" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="C43" s="22" t="s">
+        <v>87</v>
+      </c>
+      <c r="D43" s="34" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="44" spans="1:24" ht="50.25" customHeight="1">
+      <c r="A44" s="43"/>
+      <c r="B44" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="C44" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="D44" s="16" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="45" spans="1:24" ht="36" customHeight="1">
+      <c r="A45" s="44"/>
+      <c r="B45" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="C45" s="22" t="s">
+        <v>90</v>
+      </c>
+      <c r="D45" s="34" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="46" spans="1:24" ht="30">
+      <c r="A46" s="39" t="s">
+        <v>121</v>
+      </c>
+      <c r="B46" s="27" t="s">
+        <v>93</v>
+      </c>
+      <c r="C46" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="D46" s="16" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="47" spans="1:24" ht="30">
+      <c r="A47" s="40"/>
+      <c r="B47" s="26" t="s">
+        <v>94</v>
+      </c>
+      <c r="C47" s="22" t="s">
+        <v>107</v>
+      </c>
+      <c r="D47" s="34" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="48" spans="1:24">
+      <c r="A48" s="40"/>
+      <c r="B48" s="27" t="s">
+        <v>95</v>
+      </c>
+      <c r="C48" s="25" t="s">
+        <v>99</v>
+      </c>
+      <c r="D48" s="16" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="45">
+      <c r="A49" s="40"/>
+      <c r="B49" s="26" t="s">
+        <v>96</v>
+      </c>
+      <c r="C49" s="22" t="s">
+        <v>100</v>
+      </c>
+      <c r="D49" s="34" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="30">
+      <c r="A50" s="41"/>
+      <c r="B50" s="27" t="s">
+        <v>97</v>
+      </c>
+      <c r="C50" s="21" t="s">
+        <v>98</v>
+      </c>
+      <c r="D50" s="16" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="45">
+      <c r="A51" s="42" t="s">
         <v>122</v>
       </c>
-      <c r="B35" s="26" t="s">
-        <v>84</v>
-      </c>
-      <c r="C35" s="22" t="s">
-        <v>94</v>
-      </c>
-      <c r="D35" s="34" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="36" spans="1:24" ht="38.25" customHeight="1">
-      <c r="A36" s="49"/>
-      <c r="B36" s="27" t="s">
-        <v>85</v>
-      </c>
-      <c r="C36" s="21" t="s">
-        <v>88</v>
-      </c>
-      <c r="D36" s="16" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="37" spans="1:24" ht="48.75" customHeight="1">
-      <c r="A37" s="49"/>
-      <c r="B37" s="26" t="s">
-        <v>86</v>
-      </c>
-      <c r="C37" s="22" t="s">
-        <v>89</v>
-      </c>
-      <c r="D37" s="34" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="38" spans="1:24" ht="50.25" customHeight="1">
-      <c r="A38" s="49"/>
-      <c r="B38" s="27" t="s">
-        <v>87</v>
-      </c>
-      <c r="C38" s="21" t="s">
-        <v>90</v>
-      </c>
-      <c r="D38" s="16" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="39" spans="1:24" ht="36" customHeight="1">
-      <c r="A39" s="42"/>
-      <c r="B39" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="C39" s="22" t="s">
-        <v>92</v>
-      </c>
-      <c r="D39" s="34" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="40" spans="1:24" ht="30">
-      <c r="A40" s="46" t="s">
-        <v>123</v>
-      </c>
-      <c r="B40" s="27" t="s">
-        <v>95</v>
-      </c>
-      <c r="C40" s="24" t="s">
+      <c r="B51" s="26" t="s">
+        <v>101</v>
+      </c>
+      <c r="C51" s="22" t="s">
+        <v>105</v>
+      </c>
+      <c r="D51" s="34" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="30">
+      <c r="A52" s="43"/>
+      <c r="B52" s="27" t="s">
+        <v>102</v>
+      </c>
+      <c r="C52" s="21" t="s">
         <v>108</v>
       </c>
-      <c r="D40" s="16" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="41" spans="1:24" ht="30">
-      <c r="A41" s="47"/>
-      <c r="B41" s="26" t="s">
-        <v>96</v>
-      </c>
-      <c r="C41" s="22" t="s">
+      <c r="D52" s="16" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" ht="45">
+      <c r="A53" s="43"/>
+      <c r="B53" s="26" t="s">
+        <v>103</v>
+      </c>
+      <c r="C53" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="D41" s="34" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="42" spans="1:24">
-      <c r="A42" s="47"/>
-      <c r="B42" s="27" t="s">
-        <v>97</v>
-      </c>
-      <c r="C42" s="25" t="s">
-        <v>101</v>
-      </c>
-      <c r="D42" s="16" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="43" spans="1:24" ht="45">
-      <c r="A43" s="47"/>
-      <c r="B43" s="26" t="s">
-        <v>98</v>
-      </c>
-      <c r="C43" s="22" t="s">
-        <v>102</v>
-      </c>
-      <c r="D43" s="34" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="44" spans="1:24" ht="30">
-      <c r="A44" s="48"/>
-      <c r="B44" s="27" t="s">
-        <v>99</v>
-      </c>
-      <c r="C44" s="21" t="s">
-        <v>100</v>
-      </c>
-      <c r="D44" s="16" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="45" spans="1:24" ht="45">
-      <c r="A45" s="41" t="s">
-        <v>124</v>
-      </c>
-      <c r="B45" s="26" t="s">
-        <v>103</v>
-      </c>
-      <c r="C45" s="22" t="s">
-        <v>107</v>
-      </c>
-      <c r="D45" s="34" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="46" spans="1:24" ht="30">
-      <c r="A46" s="49"/>
-      <c r="B46" s="27" t="s">
+      <c r="D53" s="34" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" ht="34.5" customHeight="1">
+      <c r="A54" s="44"/>
+      <c r="B54" s="27" t="s">
         <v>104</v>
       </c>
-      <c r="C46" s="21" t="s">
+      <c r="C54" s="21" t="s">
         <v>110</v>
       </c>
-      <c r="D46" s="16" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="47" spans="1:24" ht="45">
-      <c r="A47" s="49"/>
-      <c r="B47" s="26" t="s">
-        <v>105</v>
-      </c>
-      <c r="C47" s="22" t="s">
-        <v>111</v>
-      </c>
-      <c r="D47" s="34" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="48" spans="1:24" ht="34.5" customHeight="1">
-      <c r="A48" s="42"/>
-      <c r="B48" s="27" t="s">
-        <v>106</v>
-      </c>
-      <c r="C48" s="21" t="s">
-        <v>112</v>
-      </c>
-      <c r="D48" s="16" t="s">
-        <v>64</v>
+      <c r="D54" s="16" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A40:A44"/>
-    <mergeCell ref="A45:A48"/>
-    <mergeCell ref="A16:A18"/>
-    <mergeCell ref="A35:A39"/>
-    <mergeCell ref="A28:A30"/>
-    <mergeCell ref="A31:A34"/>
     <mergeCell ref="A2:A10"/>
-    <mergeCell ref="A25:A27"/>
+    <mergeCell ref="A31:A33"/>
     <mergeCell ref="A11:A13"/>
     <mergeCell ref="A14:A15"/>
-    <mergeCell ref="A19:A24"/>
+    <mergeCell ref="A19:A30"/>
+    <mergeCell ref="A46:A50"/>
+    <mergeCell ref="A51:A54"/>
+    <mergeCell ref="A16:A18"/>
+    <mergeCell ref="A41:A45"/>
+    <mergeCell ref="A34:A36"/>
+    <mergeCell ref="A37:A40"/>
   </mergeCells>
   <phoneticPr fontId="9" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation allowBlank="1" showDropDown="1" sqref="A14 A11 D2 D11 A2 A17 A19 D45 D41 D43 D14:D27"/>
+    <dataValidation allowBlank="1" showDropDown="1" sqref="A14 A11 D2 D11 A2 A17 A19 D51 D47 D49 D14:D33"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1902,7 +1993,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+    <sheetView topLeftCell="A6" workbookViewId="0">
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
@@ -1972,13 +2063,13 @@
     </row>
     <row r="5" spans="1:4" ht="37.5">
       <c r="A5" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D5" s="4">
         <v>45759</v>
@@ -1986,13 +2077,13 @@
     </row>
     <row r="6" spans="1:4" ht="37.5">
       <c r="A6" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D6" s="2">
         <v>45765</v>
@@ -2000,13 +2091,13 @@
     </row>
     <row r="7" spans="1:4" ht="18.75">
       <c r="A7" s="6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D7" s="4">
         <v>45766</v>
@@ -2014,13 +2105,13 @@
     </row>
     <row r="8" spans="1:4" ht="18.75">
       <c r="A8" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D8" s="2">
         <v>45768</v>
@@ -2028,13 +2119,13 @@
     </row>
     <row r="9" spans="1:4" ht="18.75">
       <c r="A9" s="6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B9" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>64</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>66</v>
       </c>
       <c r="D9" s="4">
         <v>45776</v>
@@ -2042,13 +2133,13 @@
     </row>
     <row r="10" spans="1:4" ht="37.5">
       <c r="A10" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>130</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>132</v>
       </c>
       <c r="D10" s="2">
         <v>45776</v>
@@ -2056,13 +2147,13 @@
     </row>
     <row r="11" spans="1:4" ht="37.5">
       <c r="A11" s="6" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D11" s="4">
         <v>45777</v>
@@ -2070,13 +2161,13 @@
     </row>
     <row r="12" spans="1:4" ht="56.25">
       <c r="A12" s="5" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D12" s="2">
         <v>45777</v>
@@ -2084,13 +2175,13 @@
     </row>
     <row r="13" spans="1:4" ht="37.5">
       <c r="A13" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>139</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>141</v>
       </c>
       <c r="D13" s="2">
         <v>45777</v>

</xml_diff>

<commit_message>
v2.4 Updating USERHOME  after review comments
</commit_message>
<xml_diff>
--- a/LH_REQUIREMENTS/LH_CRS.xlsx
+++ b/LH_REQUIREMENTS/LH_CRS.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
-  <workbookPr filterPrivacy="1"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="LH_CRS" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="156">
   <si>
     <t>ID</t>
   </si>
@@ -253,10 +253,6 @@
     <t>LH-CRS-USERHOME-003</t>
   </si>
   <si>
-    <t xml:space="preserve">The home page must dynamically fetch and display notifications for new articles in categories the user follows, ensuring that users are kept updated with the latest content. Notifications should include the category name and a brief description of the new update.
-</t>
-  </si>
-  <si>
     <t>LH-CRS-USERHOME-004</t>
   </si>
   <si>
@@ -264,10 +260,6 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Posts from followed categories must be listed on the user home page. Each post should include a title and post content. The system must ensure real-time synchronization to reflect the latest updates accurately.
-</t>
-  </si>
-  <si>
     <t xml:space="preserve">A notification bell icon must be displayed on the user home page, showing the number of new notifications. 
 </t>
   </si>
@@ -498,12 +490,26 @@
   </si>
   <si>
     <t>the admin can take sure the user is already deleted by refresh and search by the same username</t>
+  </si>
+  <si>
+    <t>v2.4</t>
+  </si>
+  <si>
+    <t>Updating USERHOME  after review comments</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The home page must dynamically fetch and display notifications for new articles in categories the user follows
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Posts from followed categories must be listed on the user home page
+</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="10">
     <font>
       <sz val="11"/>
@@ -798,6 +804,24 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -807,28 +831,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1103,7 +1109,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1113,8 +1119,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="83" zoomScaleNormal="76" workbookViewId="0">
-      <selection activeCell="B31" sqref="A31:XFD31"/>
+    <sheetView topLeftCell="A37" zoomScaleNormal="76" workbookViewId="0">
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -1141,8 +1147,8 @@
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="47" t="s">
-        <v>112</v>
+      <c r="A2" s="39" t="s">
+        <v>110</v>
       </c>
       <c r="B2" s="26" t="s">
         <v>11</v>
@@ -1155,7 +1161,7 @@
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="47"/>
+      <c r="A3" s="39"/>
       <c r="B3" s="27" t="s">
         <v>19</v>
       </c>
@@ -1167,7 +1173,7 @@
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="47"/>
+      <c r="A4" s="39"/>
       <c r="B4" s="26" t="s">
         <v>20</v>
       </c>
@@ -1179,7 +1185,7 @@
       </c>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="47"/>
+      <c r="A5" s="39"/>
       <c r="B5" s="27" t="s">
         <v>21</v>
       </c>
@@ -1191,7 +1197,7 @@
       </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="47"/>
+      <c r="A6" s="39"/>
       <c r="B6" s="26" t="s">
         <v>22</v>
       </c>
@@ -1203,7 +1209,7 @@
       </c>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" s="47"/>
+      <c r="A7" s="39"/>
       <c r="B7" s="27" t="s">
         <v>23</v>
       </c>
@@ -1215,7 +1221,7 @@
       </c>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" s="47"/>
+      <c r="A8" s="39"/>
       <c r="B8" s="26" t="s">
         <v>47</v>
       </c>
@@ -1227,7 +1233,7 @@
       </c>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" s="47"/>
+      <c r="A9" s="39"/>
       <c r="B9" s="27" t="s">
         <v>49</v>
       </c>
@@ -1239,20 +1245,20 @@
       </c>
     </row>
     <row r="10" spans="1:4">
-      <c r="A10" s="47"/>
+      <c r="A10" s="39"/>
       <c r="B10" s="26" t="s">
         <v>50</v>
       </c>
       <c r="C10" s="17" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D10" s="34" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11" s="46" t="s">
-        <v>113</v>
+      <c r="A11" s="40" t="s">
+        <v>111</v>
       </c>
       <c r="B11" s="26" t="s">
         <v>24</v>
@@ -1265,7 +1271,7 @@
       </c>
     </row>
     <row r="12" spans="1:4">
-      <c r="A12" s="46"/>
+      <c r="A12" s="40"/>
       <c r="B12" s="27" t="s">
         <v>12</v>
       </c>
@@ -1277,7 +1283,7 @@
       </c>
     </row>
     <row r="13" spans="1:4">
-      <c r="A13" s="46"/>
+      <c r="A13" s="40"/>
       <c r="B13" s="26" t="s">
         <v>25</v>
       </c>
@@ -1289,8 +1295,8 @@
       </c>
     </row>
     <row r="14" spans="1:4">
-      <c r="A14" s="42" t="s">
-        <v>114</v>
+      <c r="A14" s="41" t="s">
+        <v>112</v>
       </c>
       <c r="B14" s="30" t="s">
         <v>37</v>
@@ -1303,7 +1309,7 @@
       </c>
     </row>
     <row r="15" spans="1:4">
-      <c r="A15" s="44"/>
+      <c r="A15" s="42"/>
       <c r="B15" s="26" t="s">
         <v>40</v>
       </c>
@@ -1315,8 +1321,8 @@
       </c>
     </row>
     <row r="16" spans="1:4">
-      <c r="A16" s="45" t="s">
-        <v>115</v>
+      <c r="A16" s="49" t="s">
+        <v>113</v>
       </c>
       <c r="B16" s="29" t="s">
         <v>38</v>
@@ -1329,7 +1335,7 @@
       </c>
     </row>
     <row r="17" spans="1:24">
-      <c r="A17" s="45" t="s">
+      <c r="A17" s="49" t="s">
         <v>6</v>
       </c>
       <c r="B17" s="26" t="s">
@@ -1343,7 +1349,7 @@
       </c>
     </row>
     <row r="18" spans="1:24">
-      <c r="A18" s="45"/>
+      <c r="A18" s="49"/>
       <c r="B18" s="27" t="s">
         <v>51</v>
       </c>
@@ -1355,140 +1361,140 @@
       </c>
     </row>
     <row r="19" spans="1:24" ht="30">
-      <c r="A19" s="48" t="s">
-        <v>116</v>
+      <c r="A19" s="43" t="s">
+        <v>114</v>
       </c>
       <c r="B19" s="26" t="s">
+        <v>121</v>
+      </c>
+      <c r="C19" s="22" t="s">
+        <v>130</v>
+      </c>
+      <c r="D19" s="23" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:24">
+      <c r="A20" s="44"/>
+      <c r="B20" s="37" t="s">
+        <v>122</v>
+      </c>
+      <c r="C20" s="20" t="s">
+        <v>131</v>
+      </c>
+      <c r="D20" s="38" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:24">
+      <c r="A21" s="44"/>
+      <c r="B21" s="26" t="s">
         <v>123</v>
       </c>
-      <c r="C19" s="22" t="s">
+      <c r="C21" s="22" t="s">
         <v>132</v>
       </c>
-      <c r="D19" s="23" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="20" spans="1:24">
-      <c r="A20" s="49"/>
-      <c r="B20" s="37" t="s">
+      <c r="D21" s="23" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:24">
+      <c r="A22" s="44"/>
+      <c r="B22" s="37" t="s">
         <v>124</v>
       </c>
-      <c r="C20" s="20" t="s">
+      <c r="C22" s="20" t="s">
         <v>133</v>
       </c>
-      <c r="D20" s="38" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="21" spans="1:24">
-      <c r="A21" s="49"/>
-      <c r="B21" s="26" t="s">
+      <c r="D22" s="38" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:24" ht="15" customHeight="1">
+      <c r="A23" s="44"/>
+      <c r="B23" s="26" t="s">
         <v>125</v>
       </c>
-      <c r="C21" s="22" t="s">
+      <c r="C23" s="22" t="s">
         <v>134</v>
       </c>
-      <c r="D21" s="23" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="22" spans="1:24">
-      <c r="A22" s="49"/>
-      <c r="B22" s="37" t="s">
-        <v>126</v>
-      </c>
-      <c r="C22" s="20" t="s">
-        <v>135</v>
-      </c>
-      <c r="D22" s="38" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="23" spans="1:24" ht="15" customHeight="1">
-      <c r="A23" s="49"/>
-      <c r="B23" s="26" t="s">
-        <v>127</v>
-      </c>
-      <c r="C23" s="22" t="s">
-        <v>136</v>
-      </c>
       <c r="D23" s="23" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="24" spans="1:24" ht="15" customHeight="1">
-      <c r="A24" s="49"/>
+      <c r="A24" s="44"/>
       <c r="B24" s="26" t="s">
+        <v>138</v>
+      </c>
+      <c r="C24" s="22" t="s">
+        <v>143</v>
+      </c>
+      <c r="D24" s="23"/>
+    </row>
+    <row r="25" spans="1:24" ht="15" customHeight="1">
+      <c r="A25" s="44"/>
+      <c r="B25" s="26" t="s">
+        <v>139</v>
+      </c>
+      <c r="C25" s="22" t="s">
+        <v>144</v>
+      </c>
+      <c r="D25" s="23"/>
+    </row>
+    <row r="26" spans="1:24" ht="15" customHeight="1">
+      <c r="A26" s="44"/>
+      <c r="B26" s="26" t="s">
         <v>140</v>
       </c>
-      <c r="C24" s="22" t="s">
+      <c r="C26" s="22" t="s">
         <v>145</v>
       </c>
-      <c r="D24" s="23"/>
-    </row>
-    <row r="25" spans="1:24" ht="15" customHeight="1">
-      <c r="A25" s="49"/>
-      <c r="B25" s="26" t="s">
+      <c r="D26" s="23"/>
+    </row>
+    <row r="27" spans="1:24" ht="15" customHeight="1">
+      <c r="A27" s="44"/>
+      <c r="B27" s="26" t="s">
         <v>141</v>
       </c>
-      <c r="C25" s="22" t="s">
+      <c r="C27" s="22" t="s">
         <v>146</v>
       </c>
-      <c r="D25" s="23"/>
-    </row>
-    <row r="26" spans="1:24" ht="15" customHeight="1">
-      <c r="A26" s="49"/>
-      <c r="B26" s="26" t="s">
+      <c r="D27" s="23"/>
+    </row>
+    <row r="28" spans="1:24" ht="15" customHeight="1">
+      <c r="A28" s="44"/>
+      <c r="B28" s="26" t="s">
         <v>142</v>
       </c>
-      <c r="C26" s="22" t="s">
+      <c r="C28" s="22" t="s">
         <v>147</v>
       </c>
-      <c r="D26" s="23"/>
-    </row>
-    <row r="27" spans="1:24" ht="15" customHeight="1">
-      <c r="A27" s="49"/>
-      <c r="B27" s="26" t="s">
-        <v>143</v>
-      </c>
-      <c r="C27" s="22" t="s">
+      <c r="D28" s="23"/>
+    </row>
+    <row r="29" spans="1:24" ht="15" customHeight="1">
+      <c r="A29" s="44"/>
+      <c r="B29" s="26" t="s">
         <v>148</v>
       </c>
-      <c r="D27" s="23"/>
-    </row>
-    <row r="28" spans="1:24" ht="15" customHeight="1">
-      <c r="A28" s="49"/>
-      <c r="B28" s="26" t="s">
-        <v>144</v>
-      </c>
-      <c r="C28" s="22" t="s">
+      <c r="C29" s="22" t="s">
         <v>149</v>
       </c>
-      <c r="D28" s="23"/>
-    </row>
-    <row r="29" spans="1:24" ht="15" customHeight="1">
-      <c r="A29" s="49"/>
-      <c r="B29" s="26" t="s">
+      <c r="D29" s="23"/>
+    </row>
+    <row r="30" spans="1:24" ht="15" customHeight="1">
+      <c r="A30" s="44"/>
+      <c r="B30" s="26" t="s">
         <v>150</v>
       </c>
-      <c r="C29" s="22" t="s">
+      <c r="C30" s="22" t="s">
         <v>151</v>
       </c>
-      <c r="D29" s="23"/>
-    </row>
-    <row r="30" spans="1:24" ht="15" customHeight="1">
-      <c r="A30" s="49"/>
-      <c r="B30" s="26" t="s">
-        <v>152</v>
-      </c>
-      <c r="C30" s="22" t="s">
-        <v>153</v>
-      </c>
       <c r="D30" s="23"/>
     </row>
     <row r="31" spans="1:24" s="12" customFormat="1" ht="45">
-      <c r="A31" s="46" t="s">
-        <v>117</v>
+      <c r="A31" s="40" t="s">
+        <v>115</v>
       </c>
       <c r="B31" s="26" t="s">
         <v>41</v>
@@ -1521,7 +1527,7 @@
       <c r="X31" s="10"/>
     </row>
     <row r="32" spans="1:24" s="11" customFormat="1" ht="45">
-      <c r="A32" s="46"/>
+      <c r="A32" s="40"/>
       <c r="B32" s="29" t="s">
         <v>42</v>
       </c>
@@ -1553,7 +1559,7 @@
       <c r="X32" s="10"/>
     </row>
     <row r="33" spans="1:24" s="12" customFormat="1" ht="30">
-      <c r="A33" s="46"/>
+      <c r="A33" s="40"/>
       <c r="B33" s="26" t="s">
         <v>43</v>
       </c>
@@ -1585,8 +1591,8 @@
       <c r="X33" s="10"/>
     </row>
     <row r="34" spans="1:24" s="12" customFormat="1" ht="78.75" customHeight="1">
-      <c r="A34" s="42" t="s">
-        <v>118</v>
+      <c r="A34" s="41" t="s">
+        <v>116</v>
       </c>
       <c r="B34" s="27" t="s">
         <v>67</v>
@@ -1619,7 +1625,7 @@
       <c r="X34" s="10"/>
     </row>
     <row r="35" spans="1:24" s="11" customFormat="1" ht="34.5" customHeight="1">
-      <c r="A35" s="43"/>
+      <c r="A35" s="48"/>
       <c r="B35" s="26" t="s">
         <v>69</v>
       </c>
@@ -1651,12 +1657,12 @@
       <c r="X35" s="10"/>
     </row>
     <row r="36" spans="1:24" s="12" customFormat="1" ht="34.5" customHeight="1">
-      <c r="A36" s="44"/>
+      <c r="A36" s="42"/>
       <c r="B36" s="27" t="s">
         <v>70</v>
       </c>
       <c r="C36" s="21" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D36" s="16" t="s">
         <v>66</v>
@@ -1683,14 +1689,14 @@
       <c r="X36" s="10"/>
     </row>
     <row r="37" spans="1:24" s="11" customFormat="1" ht="45" customHeight="1">
-      <c r="A37" s="46" t="s">
-        <v>119</v>
+      <c r="A37" s="40" t="s">
+        <v>117</v>
       </c>
       <c r="B37" s="26" t="s">
         <v>73</v>
       </c>
       <c r="C37" s="22" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D37" s="23" t="s">
         <v>66</v>
@@ -1717,12 +1723,12 @@
       <c r="X37" s="10"/>
     </row>
     <row r="38" spans="1:24" s="12" customFormat="1" ht="48.75" customHeight="1">
-      <c r="A38" s="46"/>
+      <c r="A38" s="40"/>
       <c r="B38" s="27" t="s">
         <v>74</v>
       </c>
       <c r="C38" s="21" t="s">
-        <v>76</v>
+        <v>154</v>
       </c>
       <c r="D38" s="16" t="s">
         <v>66</v>
@@ -1749,12 +1755,12 @@
       <c r="X38" s="10"/>
     </row>
     <row r="39" spans="1:24" s="12" customFormat="1" ht="35.25" customHeight="1">
-      <c r="A39" s="46"/>
+      <c r="A39" s="40"/>
       <c r="B39" s="26" t="s">
         <v>75</v>
       </c>
       <c r="C39" s="22" t="s">
-        <v>79</v>
+        <v>155</v>
       </c>
       <c r="D39" s="23" t="s">
         <v>66</v>
@@ -1781,186 +1787,186 @@
       <c r="X39" s="10"/>
     </row>
     <row r="40" spans="1:24" ht="21" customHeight="1">
-      <c r="A40" s="46"/>
+      <c r="A40" s="40"/>
       <c r="B40" s="31" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C40" s="21" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D40" s="16" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="41" spans="1:24" ht="45">
-      <c r="A41" s="42" t="s">
-        <v>120</v>
+      <c r="A41" s="41" t="s">
+        <v>118</v>
       </c>
       <c r="B41" s="26" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C41" s="22" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D41" s="34" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="42" spans="1:24" ht="38.25" customHeight="1">
-      <c r="A42" s="43"/>
+      <c r="A42" s="48"/>
       <c r="B42" s="27" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C42" s="21" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D42" s="16" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="43" spans="1:24" ht="48.75" customHeight="1">
-      <c r="A43" s="43"/>
+      <c r="A43" s="48"/>
       <c r="B43" s="26" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C43" s="22" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D43" s="34" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="44" spans="1:24" ht="50.25" customHeight="1">
-      <c r="A44" s="43"/>
+      <c r="A44" s="48"/>
       <c r="B44" s="27" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C44" s="21" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D44" s="16" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="45" spans="1:24" ht="36" customHeight="1">
-      <c r="A45" s="44"/>
+      <c r="A45" s="42"/>
       <c r="B45" s="26" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C45" s="22" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D45" s="34" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="46" spans="1:24" ht="30">
-      <c r="A46" s="39" t="s">
-        <v>121</v>
+      <c r="A46" s="45" t="s">
+        <v>119</v>
       </c>
       <c r="B46" s="27" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C46" s="24" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D46" s="16" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="47" spans="1:24" ht="30">
-      <c r="A47" s="40"/>
+      <c r="A47" s="46"/>
       <c r="B47" s="26" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C47" s="22" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D47" s="34" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="48" spans="1:24">
-      <c r="A48" s="40"/>
+      <c r="A48" s="46"/>
       <c r="B48" s="27" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C48" s="25" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D48" s="16" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="45">
-      <c r="A49" s="40"/>
+      <c r="A49" s="46"/>
       <c r="B49" s="26" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C49" s="22" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D49" s="34" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="30">
-      <c r="A50" s="41"/>
+      <c r="A50" s="47"/>
       <c r="B50" s="27" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C50" s="21" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D50" s="16" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="45">
-      <c r="A51" s="42" t="s">
-        <v>122</v>
+      <c r="A51" s="41" t="s">
+        <v>120</v>
       </c>
       <c r="B51" s="26" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C51" s="22" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D51" s="34" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="30">
-      <c r="A52" s="43"/>
+      <c r="A52" s="48"/>
       <c r="B52" s="27" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C52" s="21" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D52" s="16" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="45">
-      <c r="A53" s="43"/>
+      <c r="A53" s="48"/>
       <c r="B53" s="26" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C53" s="22" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D53" s="34" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="34.5" customHeight="1">
-      <c r="A54" s="44"/>
+      <c r="A54" s="42"/>
       <c r="B54" s="27" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C54" s="21" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D54" s="16" t="s">
         <v>62</v>
@@ -1968,17 +1974,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A2:A10"/>
-    <mergeCell ref="A31:A33"/>
-    <mergeCell ref="A11:A13"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="A19:A30"/>
     <mergeCell ref="A46:A50"/>
     <mergeCell ref="A51:A54"/>
     <mergeCell ref="A16:A18"/>
     <mergeCell ref="A41:A45"/>
     <mergeCell ref="A34:A36"/>
     <mergeCell ref="A37:A40"/>
+    <mergeCell ref="A2:A10"/>
+    <mergeCell ref="A31:A33"/>
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="A19:A30"/>
   </mergeCells>
   <phoneticPr fontId="9" type="noConversion"/>
   <dataValidations count="1">
@@ -1991,10 +1997,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2133,13 +2139,13 @@
     </row>
     <row r="10" spans="1:4" ht="37.5">
       <c r="A10" s="5" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>66</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D10" s="2">
         <v>45776</v>
@@ -2147,13 +2153,13 @@
     </row>
     <row r="11" spans="1:4" ht="37.5">
       <c r="A11" s="6" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D11" s="4">
         <v>45777</v>
@@ -2161,13 +2167,13 @@
     </row>
     <row r="12" spans="1:4" ht="56.25">
       <c r="A12" s="5" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>62</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D12" s="2">
         <v>45777</v>
@@ -2175,16 +2181,30 @@
     </row>
     <row r="13" spans="1:4" ht="37.5">
       <c r="A13" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>137</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>139</v>
       </c>
       <c r="D13" s="2">
         <v>45777</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="18.75">
+      <c r="A14" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D14" s="2">
+        <v>45778</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
V2.5 updating the crs of delete user page after review
</commit_message>
<xml_diff>
--- a/LH_REQUIREMENTS/LH_CRS.xlsx
+++ b/LH_REQUIREMENTS/LH_CRS.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650"/>
   </bookViews>
   <sheets>
     <sheet name="LH_CRS" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="160">
   <si>
     <t>ID</t>
   </si>
@@ -465,9 +465,6 @@
     <t>LH-CRS-DELETEUSER_005</t>
   </si>
   <si>
-    <t>The admin has the ability to delete any user from the delete post page</t>
-  </si>
-  <si>
     <t>The admin can search about the user by their username</t>
   </si>
   <si>
@@ -504,12 +501,27 @@
   <si>
     <t xml:space="preserve">Posts from followed categories must be listed on the user home page
 </t>
+  </si>
+  <si>
+    <t>V2.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eman </t>
+  </si>
+  <si>
+    <t>updating  admin constrains by adding crs for delete user after review</t>
+  </si>
+  <si>
+    <t>Eman</t>
+  </si>
+  <si>
+    <t>The admin has the ability to delete any user from the delete user page</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="10">
     <font>
       <sz val="11"/>
@@ -694,7 +706,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -804,38 +816,44 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1109,7 +1127,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1119,8 +1137,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X54"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" zoomScaleNormal="76" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScaleNormal="76" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -1147,7 +1165,7 @@
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="47" t="s">
         <v>110</v>
       </c>
       <c r="B2" s="26" t="s">
@@ -1161,7 +1179,7 @@
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="39"/>
+      <c r="A3" s="47"/>
       <c r="B3" s="27" t="s">
         <v>19</v>
       </c>
@@ -1173,7 +1191,7 @@
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="39"/>
+      <c r="A4" s="47"/>
       <c r="B4" s="26" t="s">
         <v>20</v>
       </c>
@@ -1185,7 +1203,7 @@
       </c>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="39"/>
+      <c r="A5" s="47"/>
       <c r="B5" s="27" t="s">
         <v>21</v>
       </c>
@@ -1197,7 +1215,7 @@
       </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="39"/>
+      <c r="A6" s="47"/>
       <c r="B6" s="26" t="s">
         <v>22</v>
       </c>
@@ -1209,7 +1227,7 @@
       </c>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" s="39"/>
+      <c r="A7" s="47"/>
       <c r="B7" s="27" t="s">
         <v>23</v>
       </c>
@@ -1221,7 +1239,7 @@
       </c>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" s="39"/>
+      <c r="A8" s="47"/>
       <c r="B8" s="26" t="s">
         <v>47</v>
       </c>
@@ -1233,7 +1251,7 @@
       </c>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" s="39"/>
+      <c r="A9" s="47"/>
       <c r="B9" s="27" t="s">
         <v>49</v>
       </c>
@@ -1245,7 +1263,7 @@
       </c>
     </row>
     <row r="10" spans="1:4">
-      <c r="A10" s="39"/>
+      <c r="A10" s="47"/>
       <c r="B10" s="26" t="s">
         <v>50</v>
       </c>
@@ -1257,7 +1275,7 @@
       </c>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11" s="40" t="s">
+      <c r="A11" s="46" t="s">
         <v>111</v>
       </c>
       <c r="B11" s="26" t="s">
@@ -1271,7 +1289,7 @@
       </c>
     </row>
     <row r="12" spans="1:4">
-      <c r="A12" s="40"/>
+      <c r="A12" s="46"/>
       <c r="B12" s="27" t="s">
         <v>12</v>
       </c>
@@ -1283,7 +1301,7 @@
       </c>
     </row>
     <row r="13" spans="1:4">
-      <c r="A13" s="40"/>
+      <c r="A13" s="46"/>
       <c r="B13" s="26" t="s">
         <v>25</v>
       </c>
@@ -1295,7 +1313,7 @@
       </c>
     </row>
     <row r="14" spans="1:4">
-      <c r="A14" s="41" t="s">
+      <c r="A14" s="42" t="s">
         <v>112</v>
       </c>
       <c r="B14" s="30" t="s">
@@ -1309,7 +1327,7 @@
       </c>
     </row>
     <row r="15" spans="1:4">
-      <c r="A15" s="42"/>
+      <c r="A15" s="44"/>
       <c r="B15" s="26" t="s">
         <v>40</v>
       </c>
@@ -1321,7 +1339,7 @@
       </c>
     </row>
     <row r="16" spans="1:4">
-      <c r="A16" s="49" t="s">
+      <c r="A16" s="45" t="s">
         <v>113</v>
       </c>
       <c r="B16" s="29" t="s">
@@ -1335,7 +1353,7 @@
       </c>
     </row>
     <row r="17" spans="1:24">
-      <c r="A17" s="49" t="s">
+      <c r="A17" s="45" t="s">
         <v>6</v>
       </c>
       <c r="B17" s="26" t="s">
@@ -1349,7 +1367,7 @@
       </c>
     </row>
     <row r="18" spans="1:24">
-      <c r="A18" s="49"/>
+      <c r="A18" s="45"/>
       <c r="B18" s="27" t="s">
         <v>51</v>
       </c>
@@ -1361,7 +1379,7 @@
       </c>
     </row>
     <row r="19" spans="1:24" ht="30">
-      <c r="A19" s="43" t="s">
+      <c r="A19" s="48" t="s">
         <v>114</v>
       </c>
       <c r="B19" s="26" t="s">
@@ -1375,7 +1393,7 @@
       </c>
     </row>
     <row r="20" spans="1:24">
-      <c r="A20" s="44"/>
+      <c r="A20" s="49"/>
       <c r="B20" s="37" t="s">
         <v>122</v>
       </c>
@@ -1387,7 +1405,7 @@
       </c>
     </row>
     <row r="21" spans="1:24">
-      <c r="A21" s="44"/>
+      <c r="A21" s="49"/>
       <c r="B21" s="26" t="s">
         <v>123</v>
       </c>
@@ -1399,7 +1417,7 @@
       </c>
     </row>
     <row r="22" spans="1:24">
-      <c r="A22" s="44"/>
+      <c r="A22" s="49"/>
       <c r="B22" s="37" t="s">
         <v>124</v>
       </c>
@@ -1411,7 +1429,7 @@
       </c>
     </row>
     <row r="23" spans="1:24" ht="15" customHeight="1">
-      <c r="A23" s="44"/>
+      <c r="A23" s="49"/>
       <c r="B23" s="26" t="s">
         <v>125</v>
       </c>
@@ -1423,77 +1441,91 @@
       </c>
     </row>
     <row r="24" spans="1:24" ht="15" customHeight="1">
-      <c r="A24" s="44"/>
+      <c r="A24" s="49"/>
       <c r="B24" s="26" t="s">
         <v>138</v>
       </c>
       <c r="C24" s="22" t="s">
-        <v>143</v>
-      </c>
-      <c r="D24" s="23"/>
+        <v>159</v>
+      </c>
+      <c r="D24" s="23" t="s">
+        <v>158</v>
+      </c>
     </row>
     <row r="25" spans="1:24" ht="15" customHeight="1">
-      <c r="A25" s="44"/>
+      <c r="A25" s="49"/>
       <c r="B25" s="26" t="s">
         <v>139</v>
       </c>
       <c r="C25" s="22" t="s">
-        <v>144</v>
-      </c>
-      <c r="D25" s="23"/>
+        <v>143</v>
+      </c>
+      <c r="D25" s="23" t="s">
+        <v>158</v>
+      </c>
     </row>
     <row r="26" spans="1:24" ht="15" customHeight="1">
-      <c r="A26" s="44"/>
+      <c r="A26" s="49"/>
       <c r="B26" s="26" t="s">
         <v>140</v>
       </c>
       <c r="C26" s="22" t="s">
-        <v>145</v>
-      </c>
-      <c r="D26" s="23"/>
+        <v>144</v>
+      </c>
+      <c r="D26" s="23" t="s">
+        <v>158</v>
+      </c>
     </row>
     <row r="27" spans="1:24" ht="15" customHeight="1">
-      <c r="A27" s="44"/>
+      <c r="A27" s="49"/>
       <c r="B27" s="26" t="s">
         <v>141</v>
       </c>
       <c r="C27" s="22" t="s">
-        <v>146</v>
-      </c>
-      <c r="D27" s="23"/>
+        <v>145</v>
+      </c>
+      <c r="D27" s="23" t="s">
+        <v>158</v>
+      </c>
     </row>
     <row r="28" spans="1:24" ht="15" customHeight="1">
-      <c r="A28" s="44"/>
+      <c r="A28" s="49"/>
       <c r="B28" s="26" t="s">
         <v>142</v>
       </c>
       <c r="C28" s="22" t="s">
+        <v>146</v>
+      </c>
+      <c r="D28" s="23" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="29" spans="1:24" ht="15" customHeight="1">
+      <c r="A29" s="49"/>
+      <c r="B29" s="26" t="s">
         <v>147</v>
       </c>
-      <c r="D28" s="23"/>
-    </row>
-    <row r="29" spans="1:24" ht="15" customHeight="1">
-      <c r="A29" s="44"/>
-      <c r="B29" s="26" t="s">
+      <c r="C29" s="22" t="s">
         <v>148</v>
       </c>
-      <c r="C29" s="22" t="s">
+      <c r="D29" s="23" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="30" spans="1:24" ht="15" customHeight="1">
+      <c r="A30" s="49"/>
+      <c r="B30" s="26" t="s">
         <v>149</v>
       </c>
-      <c r="D29" s="23"/>
-    </row>
-    <row r="30" spans="1:24" ht="15" customHeight="1">
-      <c r="A30" s="44"/>
-      <c r="B30" s="26" t="s">
+      <c r="C30" s="22" t="s">
         <v>150</v>
       </c>
-      <c r="C30" s="22" t="s">
-        <v>151</v>
-      </c>
-      <c r="D30" s="23"/>
+      <c r="D30" s="23" t="s">
+        <v>158</v>
+      </c>
     </row>
     <row r="31" spans="1:24" s="12" customFormat="1" ht="45">
-      <c r="A31" s="40" t="s">
+      <c r="A31" s="46" t="s">
         <v>115</v>
       </c>
       <c r="B31" s="26" t="s">
@@ -1527,7 +1559,7 @@
       <c r="X31" s="10"/>
     </row>
     <row r="32" spans="1:24" s="11" customFormat="1" ht="45">
-      <c r="A32" s="40"/>
+      <c r="A32" s="46"/>
       <c r="B32" s="29" t="s">
         <v>42</v>
       </c>
@@ -1559,7 +1591,7 @@
       <c r="X32" s="10"/>
     </row>
     <row r="33" spans="1:24" s="12" customFormat="1" ht="30">
-      <c r="A33" s="40"/>
+      <c r="A33" s="46"/>
       <c r="B33" s="26" t="s">
         <v>43</v>
       </c>
@@ -1591,7 +1623,7 @@
       <c r="X33" s="10"/>
     </row>
     <row r="34" spans="1:24" s="12" customFormat="1" ht="78.75" customHeight="1">
-      <c r="A34" s="41" t="s">
+      <c r="A34" s="42" t="s">
         <v>116</v>
       </c>
       <c r="B34" s="27" t="s">
@@ -1625,7 +1657,7 @@
       <c r="X34" s="10"/>
     </row>
     <row r="35" spans="1:24" s="11" customFormat="1" ht="34.5" customHeight="1">
-      <c r="A35" s="48"/>
+      <c r="A35" s="43"/>
       <c r="B35" s="26" t="s">
         <v>69</v>
       </c>
@@ -1657,7 +1689,7 @@
       <c r="X35" s="10"/>
     </row>
     <row r="36" spans="1:24" s="12" customFormat="1" ht="34.5" customHeight="1">
-      <c r="A36" s="42"/>
+      <c r="A36" s="44"/>
       <c r="B36" s="27" t="s">
         <v>70</v>
       </c>
@@ -1689,7 +1721,7 @@
       <c r="X36" s="10"/>
     </row>
     <row r="37" spans="1:24" s="11" customFormat="1" ht="45" customHeight="1">
-      <c r="A37" s="40" t="s">
+      <c r="A37" s="46" t="s">
         <v>117</v>
       </c>
       <c r="B37" s="26" t="s">
@@ -1723,12 +1755,12 @@
       <c r="X37" s="10"/>
     </row>
     <row r="38" spans="1:24" s="12" customFormat="1" ht="48.75" customHeight="1">
-      <c r="A38" s="40"/>
+      <c r="A38" s="46"/>
       <c r="B38" s="27" t="s">
         <v>74</v>
       </c>
       <c r="C38" s="21" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D38" s="16" t="s">
         <v>66</v>
@@ -1755,12 +1787,12 @@
       <c r="X38" s="10"/>
     </row>
     <row r="39" spans="1:24" s="12" customFormat="1" ht="35.25" customHeight="1">
-      <c r="A39" s="40"/>
+      <c r="A39" s="46"/>
       <c r="B39" s="26" t="s">
         <v>75</v>
       </c>
       <c r="C39" s="22" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D39" s="23" t="s">
         <v>66</v>
@@ -1787,7 +1819,7 @@
       <c r="X39" s="10"/>
     </row>
     <row r="40" spans="1:24" ht="21" customHeight="1">
-      <c r="A40" s="40"/>
+      <c r="A40" s="46"/>
       <c r="B40" s="31" t="s">
         <v>76</v>
       </c>
@@ -1799,7 +1831,7 @@
       </c>
     </row>
     <row r="41" spans="1:24" ht="45">
-      <c r="A41" s="41" t="s">
+      <c r="A41" s="42" t="s">
         <v>118</v>
       </c>
       <c r="B41" s="26" t="s">
@@ -1813,7 +1845,7 @@
       </c>
     </row>
     <row r="42" spans="1:24" ht="38.25" customHeight="1">
-      <c r="A42" s="48"/>
+      <c r="A42" s="43"/>
       <c r="B42" s="27" t="s">
         <v>81</v>
       </c>
@@ -1825,7 +1857,7 @@
       </c>
     </row>
     <row r="43" spans="1:24" ht="48.75" customHeight="1">
-      <c r="A43" s="48"/>
+      <c r="A43" s="43"/>
       <c r="B43" s="26" t="s">
         <v>82</v>
       </c>
@@ -1837,7 +1869,7 @@
       </c>
     </row>
     <row r="44" spans="1:24" ht="50.25" customHeight="1">
-      <c r="A44" s="48"/>
+      <c r="A44" s="43"/>
       <c r="B44" s="27" t="s">
         <v>83</v>
       </c>
@@ -1849,7 +1881,7 @@
       </c>
     </row>
     <row r="45" spans="1:24" ht="36" customHeight="1">
-      <c r="A45" s="42"/>
+      <c r="A45" s="44"/>
       <c r="B45" s="26" t="s">
         <v>87</v>
       </c>
@@ -1861,7 +1893,7 @@
       </c>
     </row>
     <row r="46" spans="1:24" ht="30">
-      <c r="A46" s="45" t="s">
+      <c r="A46" s="39" t="s">
         <v>119</v>
       </c>
       <c r="B46" s="27" t="s">
@@ -1875,7 +1907,7 @@
       </c>
     </row>
     <row r="47" spans="1:24" ht="30">
-      <c r="A47" s="46"/>
+      <c r="A47" s="40"/>
       <c r="B47" s="26" t="s">
         <v>92</v>
       </c>
@@ -1887,7 +1919,7 @@
       </c>
     </row>
     <row r="48" spans="1:24">
-      <c r="A48" s="46"/>
+      <c r="A48" s="40"/>
       <c r="B48" s="27" t="s">
         <v>93</v>
       </c>
@@ -1899,7 +1931,7 @@
       </c>
     </row>
     <row r="49" spans="1:4" ht="45">
-      <c r="A49" s="46"/>
+      <c r="A49" s="40"/>
       <c r="B49" s="26" t="s">
         <v>94</v>
       </c>
@@ -1911,7 +1943,7 @@
       </c>
     </row>
     <row r="50" spans="1:4" ht="30">
-      <c r="A50" s="47"/>
+      <c r="A50" s="41"/>
       <c r="B50" s="27" t="s">
         <v>95</v>
       </c>
@@ -1923,7 +1955,7 @@
       </c>
     </row>
     <row r="51" spans="1:4" ht="45">
-      <c r="A51" s="41" t="s">
+      <c r="A51" s="42" t="s">
         <v>120</v>
       </c>
       <c r="B51" s="26" t="s">
@@ -1937,7 +1969,7 @@
       </c>
     </row>
     <row r="52" spans="1:4" ht="30">
-      <c r="A52" s="48"/>
+      <c r="A52" s="43"/>
       <c r="B52" s="27" t="s">
         <v>100</v>
       </c>
@@ -1949,7 +1981,7 @@
       </c>
     </row>
     <row r="53" spans="1:4" ht="45">
-      <c r="A53" s="48"/>
+      <c r="A53" s="43"/>
       <c r="B53" s="26" t="s">
         <v>101</v>
       </c>
@@ -1961,7 +1993,7 @@
       </c>
     </row>
     <row r="54" spans="1:4" ht="34.5" customHeight="1">
-      <c r="A54" s="42"/>
+      <c r="A54" s="44"/>
       <c r="B54" s="27" t="s">
         <v>102</v>
       </c>
@@ -1974,17 +2006,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A2:A10"/>
+    <mergeCell ref="A31:A33"/>
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="A19:A30"/>
     <mergeCell ref="A46:A50"/>
     <mergeCell ref="A51:A54"/>
     <mergeCell ref="A16:A18"/>
     <mergeCell ref="A41:A45"/>
     <mergeCell ref="A34:A36"/>
     <mergeCell ref="A37:A40"/>
-    <mergeCell ref="A2:A10"/>
-    <mergeCell ref="A31:A33"/>
-    <mergeCell ref="A11:A13"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="A19:A30"/>
   </mergeCells>
   <phoneticPr fontId="9" type="noConversion"/>
   <dataValidations count="1">
@@ -1997,10 +2029,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2195,16 +2227,30 @@
     </row>
     <row r="14" spans="1:4" ht="18.75">
       <c r="A14" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>66</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D14" s="2">
         <v>45778</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="37.5">
+      <c r="A15" s="50" t="s">
+        <v>155</v>
+      </c>
+      <c r="B15" s="51" t="s">
+        <v>156</v>
+      </c>
+      <c r="C15" s="51" t="s">
+        <v>157</v>
+      </c>
+      <c r="D15" s="2">
+        <v>45779</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
v2.7 Updated the CRS to reflect the current Registration after Review
</commit_message>
<xml_diff>
--- a/LH_REQUIREMENTS/LH_CRS.xlsx
+++ b/LH_REQUIREMENTS/LH_CRS.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E0ADA91-41E0-4109-8DBE-55A66E958ED9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BF69CC4-3F6B-4C84-B25B-C5CBCF9DF413}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LH_CRS" sheetId="1" r:id="rId1"/>
@@ -483,27 +483,12 @@
     <t>The system must display password requirements to users before or during input (e.g., via a hint, tooltip, or guidance message near the password field).</t>
   </si>
   <si>
-    <t>If the entered username is already in use, the system must display the error message: "This username is already used" below or beside the username field.</t>
-  </si>
-  <si>
     <t>If the entered email is already in use, the system must display a clear message indicating that the email is already registered.</t>
   </si>
   <si>
     <t>The registration form must ensure that all required fields (username, password, and email) are filled out before submission. If any field is empty, a message such as "This field is required" must be shown beside the empty field.</t>
   </si>
   <si>
-    <t>The username must meet specific constraints, such as allowed characters and length limits. Invalid usernames must trigger a relevant error message.</t>
-  </si>
-  <si>
-    <t>The system must prevent multiple registrations using the same email or username by performing backend validation before account creation.</t>
-  </si>
-  <si>
-    <t>LH-CRS-REGISTRATION-010</t>
-  </si>
-  <si>
-    <t>All error messages must be displayed in a consistent and visible location, such as beneath the relevant input field or in a designated error message area (as seen in the wireframe: "Error Message: Any Error Message will display here").</t>
-  </si>
-  <si>
     <t xml:space="preserve">CATEGORIES </t>
   </si>
   <si>
@@ -571,6 +556,21 @@
   </si>
   <si>
     <t>Updated the CRS to reflect the current Registration and Categories pages based on the latest descriptions and wireframes.</t>
+  </si>
+  <si>
+    <t>If the entered username is already in use, the system must display the error message.</t>
+  </si>
+  <si>
+    <t>All error messages must be displayed in a consistent and visible location, such as beneath the relevant input field or in a designated error message area.</t>
+  </si>
+  <si>
+    <t>The username must meet specific constraints, such as allowed characters and length limits. Invalid usernames must trigger a error message.</t>
+  </si>
+  <si>
+    <t>V2.7</t>
+  </si>
+  <si>
+    <t>Updated the CRS to reflect the current Registration after Review</t>
   </si>
 </sst>
 </file>
@@ -817,82 +817,82 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1175,40 +1175,40 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:X62"/>
+  <dimension ref="A1:X61"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScaleNormal="76" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="76" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="18.109375" style="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.5546875" style="39" customWidth="1"/>
-    <col min="3" max="3" width="104" style="25" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.109375" style="26" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.88671875" style="25"/>
+    <col min="2" max="2" width="31.5546875" style="32" customWidth="1"/>
+    <col min="3" max="3" width="104" style="22" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.109375" style="23" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.88671875" style="22"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="23" customFormat="1" ht="19.2" x14ac:dyDescent="0.35">
-      <c r="A1" s="20" t="s">
+    <row r="1" spans="1:4" s="20" customFormat="1" ht="19.2" x14ac:dyDescent="0.35">
+      <c r="A1" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="22" t="s">
+      <c r="C1" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="22" t="s">
+      <c r="D1" s="19" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="39" t="s">
         <v>96</v>
       </c>
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="21" t="s">
         <v>9</v>
       </c>
       <c r="C2" s="11" t="s">
@@ -1219,20 +1219,20 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="18"/>
+      <c r="A3" s="40"/>
       <c r="B3" s="15" t="s">
         <v>11</v>
       </c>
       <c r="C3" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="26" t="s">
+      <c r="D3" s="23" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="18"/>
-      <c r="B4" s="24" t="s">
+      <c r="A4" s="40"/>
+      <c r="B4" s="21" t="s">
         <v>12</v>
       </c>
       <c r="C4" s="11" t="s">
@@ -1243,920 +1243,908 @@
       </c>
     </row>
     <row r="5" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="18"/>
+      <c r="A5" s="40"/>
       <c r="B5" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C5" s="10" t="s">
         <v>147</v>
       </c>
-      <c r="D5" s="26" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="18"/>
-      <c r="B6" s="24" t="s">
+      <c r="D5" s="23" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="40"/>
+      <c r="B6" s="21" t="s">
         <v>14</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>148</v>
+        <v>173</v>
       </c>
       <c r="D6" s="12" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="18"/>
+      <c r="A7" s="40"/>
       <c r="B7" s="15" t="s">
         <v>15</v>
       </c>
       <c r="C7" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="D7" s="23" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="40"/>
+      <c r="B8" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" s="11" t="s">
         <v>149</v>
       </c>
-      <c r="D7" s="26" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="18"/>
-      <c r="B8" s="24" t="s">
-        <v>35</v>
-      </c>
-      <c r="C8" s="11" t="s">
-        <v>150</v>
-      </c>
       <c r="D8" s="12" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A9" s="18"/>
+      <c r="A9" s="40"/>
       <c r="B9" s="15" t="s">
         <v>37</v>
       </c>
       <c r="C9" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="D9" s="23" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A10" s="41"/>
+      <c r="B10" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>174</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="42" t="s">
+        <v>150</v>
+      </c>
+      <c r="B11" s="21" t="s">
         <v>151</v>
       </c>
-      <c r="D9" s="26" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A10" s="18"/>
-      <c r="B10" s="24" t="s">
-        <v>38</v>
-      </c>
-      <c r="C10" s="11" t="s">
+      <c r="C11" s="11" t="s">
+        <v>161</v>
+      </c>
+      <c r="D11" s="33" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="42"/>
+      <c r="B12" s="25" t="s">
         <v>152</v>
       </c>
-      <c r="D10" s="12" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A11" s="28"/>
-      <c r="B11" s="29" t="s">
+      <c r="C12" s="10" t="s">
+        <v>162</v>
+      </c>
+      <c r="D12" s="27" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="42"/>
+      <c r="B13" s="21" t="s">
         <v>153</v>
       </c>
-      <c r="C11" s="30" t="s">
+      <c r="C13" s="11" t="s">
+        <v>163</v>
+      </c>
+      <c r="D13" s="33" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A14" s="42"/>
+      <c r="B14" s="25" t="s">
         <v>154</v>
       </c>
-      <c r="D11" s="31" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="19" t="s">
+      <c r="C14" s="10" t="s">
+        <v>164</v>
+      </c>
+      <c r="D14" s="27" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="42"/>
+      <c r="B15" s="21" t="s">
         <v>155</v>
       </c>
-      <c r="B12" s="24" t="s">
+      <c r="C15" s="34" t="s">
+        <v>165</v>
+      </c>
+      <c r="D15" s="12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="42"/>
+      <c r="B16" s="25" t="s">
         <v>156</v>
       </c>
-      <c r="C12" s="11" t="s">
+      <c r="C16" s="10" t="s">
         <v>166</v>
       </c>
-      <c r="D12" s="40" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="19"/>
-      <c r="B13" s="29" t="s">
+      <c r="D16" s="27" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="42"/>
+      <c r="B17" s="21" t="s">
         <v>157</v>
       </c>
-      <c r="C13" s="10" t="s">
+      <c r="C17" s="34" t="s">
         <v>167</v>
       </c>
-      <c r="D13" s="31" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="19"/>
-      <c r="B14" s="24" t="s">
+      <c r="D17" s="12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="42"/>
+      <c r="B18" s="25" t="s">
         <v>158</v>
       </c>
-      <c r="C14" s="11" t="s">
+      <c r="C18" s="10" t="s">
         <v>168</v>
       </c>
-      <c r="D14" s="40" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A15" s="19"/>
-      <c r="B15" s="29" t="s">
+      <c r="D18" s="27" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="42"/>
+      <c r="B19" s="21" t="s">
         <v>159</v>
       </c>
-      <c r="C15" s="10" t="s">
+      <c r="C19" s="34" t="s">
         <v>169</v>
       </c>
-      <c r="D15" s="31" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" s="19"/>
-      <c r="B16" s="24" t="s">
+      <c r="D19" s="12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="42"/>
+      <c r="B20" s="25" t="s">
         <v>160</v>
       </c>
-      <c r="C16" s="41" t="s">
+      <c r="C20" s="26" t="s">
         <v>170</v>
       </c>
-      <c r="D16" s="12" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="19"/>
-      <c r="B17" s="29" t="s">
-        <v>161</v>
-      </c>
-      <c r="C17" s="10" t="s">
-        <v>171</v>
-      </c>
-      <c r="D17" s="31" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="19"/>
-      <c r="B18" s="24" t="s">
-        <v>162</v>
-      </c>
-      <c r="C18" s="41" t="s">
-        <v>172</v>
-      </c>
-      <c r="D18" s="12" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="19"/>
-      <c r="B19" s="29" t="s">
-        <v>163</v>
-      </c>
-      <c r="C19" s="10" t="s">
-        <v>173</v>
-      </c>
-      <c r="D19" s="31" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="19"/>
-      <c r="B20" s="24" t="s">
-        <v>164</v>
-      </c>
-      <c r="C20" s="41" t="s">
-        <v>174</v>
-      </c>
-      <c r="D20" s="12" t="s">
+      <c r="D20" s="27" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="19"/>
-      <c r="B21" s="29" t="s">
-        <v>165</v>
-      </c>
-      <c r="C21" s="30" t="s">
-        <v>175</v>
-      </c>
-      <c r="D21" s="31" t="s">
+      <c r="A21" s="39" t="s">
+        <v>97</v>
+      </c>
+      <c r="B21" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="C21" s="34" t="s">
+        <v>2</v>
+      </c>
+      <c r="D21" s="35" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="17" t="s">
-        <v>97</v>
-      </c>
-      <c r="B22" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="C22" s="41" t="s">
-        <v>2</v>
-      </c>
-      <c r="D22" s="42" t="s">
+      <c r="A22" s="41"/>
+      <c r="B22" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="D22" s="12" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" s="28"/>
-      <c r="B23" s="24" t="s">
-        <v>29</v>
-      </c>
-      <c r="C23" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="D23" s="12" t="s">
+      <c r="A23" s="42" t="s">
+        <v>98</v>
+      </c>
+      <c r="B23" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="C23" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="D23" s="27" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" s="19" t="s">
-        <v>98</v>
-      </c>
-      <c r="B24" s="29" t="s">
-        <v>27</v>
-      </c>
-      <c r="C24" s="30" t="s">
-        <v>42</v>
-      </c>
-      <c r="D24" s="31" t="s">
+      <c r="A24" s="42" t="s">
+        <v>4</v>
+      </c>
+      <c r="B24" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="C24" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D24" s="12" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="B25" s="24" t="s">
-        <v>28</v>
-      </c>
-      <c r="C25" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="D25" s="12" t="s">
-        <v>8</v>
+      <c r="A25" s="42"/>
+      <c r="B25" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D25" s="23" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" s="19"/>
-      <c r="B26" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="C26" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="D26" s="26" t="s">
+      <c r="A26" s="39" t="s">
+        <v>99</v>
+      </c>
+      <c r="B26" s="21" t="s">
+        <v>106</v>
+      </c>
+      <c r="C26" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="D26" s="12" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" s="17" t="s">
-        <v>99</v>
-      </c>
-      <c r="B27" s="24" t="s">
-        <v>106</v>
-      </c>
-      <c r="C27" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="D27" s="12" t="s">
+      <c r="A27" s="40"/>
+      <c r="B27" s="28" t="s">
+        <v>107</v>
+      </c>
+      <c r="C27" s="26" t="s">
+        <v>116</v>
+      </c>
+      <c r="D27" s="29" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A28" s="18"/>
-      <c r="B28" s="32" t="s">
-        <v>107</v>
-      </c>
-      <c r="C28" s="30" t="s">
-        <v>116</v>
-      </c>
-      <c r="D28" s="33" t="s">
+      <c r="A28" s="40"/>
+      <c r="B28" s="21" t="s">
+        <v>108</v>
+      </c>
+      <c r="C28" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="D28" s="12" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A29" s="18"/>
-      <c r="B29" s="24" t="s">
-        <v>108</v>
-      </c>
-      <c r="C29" s="11" t="s">
-        <v>117</v>
-      </c>
-      <c r="D29" s="12" t="s">
+      <c r="A29" s="40"/>
+      <c r="B29" s="28" t="s">
+        <v>109</v>
+      </c>
+      <c r="C29" s="26" t="s">
+        <v>118</v>
+      </c>
+      <c r="D29" s="29" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" s="18"/>
-      <c r="B30" s="32" t="s">
-        <v>109</v>
-      </c>
-      <c r="C30" s="30" t="s">
-        <v>118</v>
-      </c>
-      <c r="D30" s="33" t="s">
+    <row r="30" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="40"/>
+      <c r="B30" s="21" t="s">
+        <v>110</v>
+      </c>
+      <c r="C30" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="D30" s="12" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="18"/>
-      <c r="B31" s="24" t="s">
-        <v>110</v>
+      <c r="A31" s="40"/>
+      <c r="B31" s="21" t="s">
+        <v>123</v>
       </c>
       <c r="C31" s="11" t="s">
-        <v>119</v>
+        <v>144</v>
       </c>
       <c r="D31" s="12" t="s">
-        <v>7</v>
+        <v>143</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="18"/>
-      <c r="B32" s="24" t="s">
-        <v>123</v>
+      <c r="A32" s="40"/>
+      <c r="B32" s="21" t="s">
+        <v>124</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>144</v>
+        <v>128</v>
       </c>
       <c r="D32" s="12" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="33" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="18"/>
-      <c r="B33" s="24" t="s">
-        <v>124</v>
+      <c r="A33" s="40"/>
+      <c r="B33" s="21" t="s">
+        <v>125</v>
       </c>
       <c r="C33" s="11" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D33" s="12" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="34" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="18"/>
-      <c r="B34" s="24" t="s">
-        <v>125</v>
+      <c r="A34" s="40"/>
+      <c r="B34" s="21" t="s">
+        <v>126</v>
       </c>
       <c r="C34" s="11" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D34" s="12" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="35" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="18"/>
-      <c r="B35" s="24" t="s">
-        <v>126</v>
+      <c r="A35" s="40"/>
+      <c r="B35" s="21" t="s">
+        <v>127</v>
       </c>
       <c r="C35" s="11" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D35" s="12" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="36" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="18"/>
-      <c r="B36" s="24" t="s">
-        <v>127</v>
+      <c r="A36" s="40"/>
+      <c r="B36" s="21" t="s">
+        <v>132</v>
       </c>
       <c r="C36" s="11" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="D36" s="12" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="37" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="18"/>
-      <c r="B37" s="24" t="s">
-        <v>132</v>
+      <c r="A37" s="40"/>
+      <c r="B37" s="21" t="s">
+        <v>134</v>
       </c>
       <c r="C37" s="11" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="D37" s="12" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="38" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="18"/>
-      <c r="B38" s="24" t="s">
-        <v>134</v>
+    <row r="38" spans="1:24" s="30" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A38" s="42" t="s">
+        <v>100</v>
+      </c>
+      <c r="B38" s="21" t="s">
+        <v>30</v>
       </c>
       <c r="C38" s="11" t="s">
-        <v>135</v>
+        <v>53</v>
       </c>
       <c r="D38" s="12" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="39" spans="1:24" s="34" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A39" s="19" t="s">
-        <v>100</v>
-      </c>
-      <c r="B39" s="24" t="s">
-        <v>30</v>
-      </c>
-      <c r="C39" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="D39" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="E39" s="25"/>
-      <c r="F39" s="25"/>
-      <c r="G39" s="25"/>
-      <c r="H39" s="25"/>
-      <c r="I39" s="25"/>
-      <c r="J39" s="25"/>
-      <c r="K39" s="25"/>
-      <c r="L39" s="25"/>
-      <c r="M39" s="25"/>
-      <c r="N39" s="25"/>
-      <c r="O39" s="25"/>
-      <c r="P39" s="25"/>
-      <c r="Q39" s="25"/>
-      <c r="R39" s="25"/>
-      <c r="S39" s="25"/>
-      <c r="T39" s="25"/>
-      <c r="U39" s="25"/>
-      <c r="V39" s="25"/>
-      <c r="W39" s="25"/>
-      <c r="X39" s="25"/>
-    </row>
-    <row r="40" spans="1:24" s="35" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A40" s="19"/>
-      <c r="B40" s="29" t="s">
+      <c r="E38" s="22"/>
+      <c r="F38" s="22"/>
+      <c r="G38" s="22"/>
+      <c r="H38" s="22"/>
+      <c r="I38" s="22"/>
+      <c r="J38" s="22"/>
+      <c r="K38" s="22"/>
+      <c r="L38" s="22"/>
+      <c r="M38" s="22"/>
+      <c r="N38" s="22"/>
+      <c r="O38" s="22"/>
+      <c r="P38" s="22"/>
+      <c r="Q38" s="22"/>
+      <c r="R38" s="22"/>
+      <c r="S38" s="22"/>
+      <c r="T38" s="22"/>
+      <c r="U38" s="22"/>
+      <c r="V38" s="22"/>
+      <c r="W38" s="22"/>
+      <c r="X38" s="22"/>
+    </row>
+    <row r="39" spans="1:24" s="31" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A39" s="42"/>
+      <c r="B39" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="C40" s="10" t="s">
+      <c r="C39" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="D40" s="31" t="s">
+      <c r="D39" s="27" t="s">
         <v>50</v>
       </c>
-      <c r="E40" s="25"/>
-      <c r="F40" s="25"/>
-      <c r="G40" s="25"/>
-      <c r="H40" s="25"/>
-      <c r="I40" s="25"/>
-      <c r="J40" s="25"/>
-      <c r="K40" s="25"/>
-      <c r="L40" s="25"/>
-      <c r="M40" s="25"/>
-      <c r="N40" s="25"/>
-      <c r="O40" s="25"/>
-      <c r="P40" s="25"/>
-      <c r="Q40" s="25"/>
-      <c r="R40" s="25"/>
-      <c r="S40" s="25"/>
-      <c r="T40" s="25"/>
-      <c r="U40" s="25"/>
-      <c r="V40" s="25"/>
-      <c r="W40" s="25"/>
-      <c r="X40" s="25"/>
-    </row>
-    <row r="41" spans="1:24" s="34" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A41" s="19"/>
-      <c r="B41" s="24" t="s">
+      <c r="E39" s="22"/>
+      <c r="F39" s="22"/>
+      <c r="G39" s="22"/>
+      <c r="H39" s="22"/>
+      <c r="I39" s="22"/>
+      <c r="J39" s="22"/>
+      <c r="K39" s="22"/>
+      <c r="L39" s="22"/>
+      <c r="M39" s="22"/>
+      <c r="N39" s="22"/>
+      <c r="O39" s="22"/>
+      <c r="P39" s="22"/>
+      <c r="Q39" s="22"/>
+      <c r="R39" s="22"/>
+      <c r="S39" s="22"/>
+      <c r="T39" s="22"/>
+      <c r="U39" s="22"/>
+      <c r="V39" s="22"/>
+      <c r="W39" s="22"/>
+      <c r="X39" s="22"/>
+    </row>
+    <row r="40" spans="1:24" s="30" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A40" s="42"/>
+      <c r="B40" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="C41" s="11" t="s">
+      <c r="C40" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="D41" s="12" t="s">
+      <c r="D40" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="E41" s="25"/>
-      <c r="F41" s="25"/>
-      <c r="G41" s="25"/>
-      <c r="H41" s="25"/>
-      <c r="I41" s="25"/>
-      <c r="J41" s="25"/>
-      <c r="K41" s="25"/>
-      <c r="L41" s="25"/>
-      <c r="M41" s="25"/>
-      <c r="N41" s="25"/>
-      <c r="O41" s="25"/>
-      <c r="P41" s="25"/>
-      <c r="Q41" s="25"/>
-      <c r="R41" s="25"/>
-      <c r="S41" s="25"/>
-      <c r="T41" s="25"/>
-      <c r="U41" s="25"/>
-      <c r="V41" s="25"/>
-      <c r="W41" s="25"/>
-      <c r="X41" s="25"/>
-    </row>
-    <row r="42" spans="1:24" s="34" customFormat="1" ht="78.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="17" t="s">
+      <c r="E40" s="22"/>
+      <c r="F40" s="22"/>
+      <c r="G40" s="22"/>
+      <c r="H40" s="22"/>
+      <c r="I40" s="22"/>
+      <c r="J40" s="22"/>
+      <c r="K40" s="22"/>
+      <c r="L40" s="22"/>
+      <c r="M40" s="22"/>
+      <c r="N40" s="22"/>
+      <c r="O40" s="22"/>
+      <c r="P40" s="22"/>
+      <c r="Q40" s="22"/>
+      <c r="R40" s="22"/>
+      <c r="S40" s="22"/>
+      <c r="T40" s="22"/>
+      <c r="U40" s="22"/>
+      <c r="V40" s="22"/>
+      <c r="W40" s="22"/>
+      <c r="X40" s="22"/>
+    </row>
+    <row r="41" spans="1:24" s="30" customFormat="1" ht="78.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="39" t="s">
         <v>101</v>
       </c>
-      <c r="B42" s="15" t="s">
+      <c r="B41" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="C42" s="10" t="s">
+      <c r="C41" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="D42" s="26" t="s">
+      <c r="D41" s="23" t="s">
         <v>54</v>
       </c>
-      <c r="E42" s="25"/>
-      <c r="F42" s="25"/>
-      <c r="G42" s="25"/>
-      <c r="H42" s="25"/>
-      <c r="I42" s="25"/>
-      <c r="J42" s="25"/>
-      <c r="K42" s="25"/>
-      <c r="L42" s="25"/>
-      <c r="M42" s="25"/>
-      <c r="N42" s="25"/>
-      <c r="O42" s="25"/>
-      <c r="P42" s="25"/>
-      <c r="Q42" s="25"/>
-      <c r="R42" s="25"/>
-      <c r="S42" s="25"/>
-      <c r="T42" s="25"/>
-      <c r="U42" s="25"/>
-      <c r="V42" s="25"/>
-      <c r="W42" s="25"/>
-      <c r="X42" s="25"/>
-    </row>
-    <row r="43" spans="1:24" s="35" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="18"/>
-      <c r="B43" s="24" t="s">
+      <c r="E41" s="22"/>
+      <c r="F41" s="22"/>
+      <c r="G41" s="22"/>
+      <c r="H41" s="22"/>
+      <c r="I41" s="22"/>
+      <c r="J41" s="22"/>
+      <c r="K41" s="22"/>
+      <c r="L41" s="22"/>
+      <c r="M41" s="22"/>
+      <c r="N41" s="22"/>
+      <c r="O41" s="22"/>
+      <c r="P41" s="22"/>
+      <c r="Q41" s="22"/>
+      <c r="R41" s="22"/>
+      <c r="S41" s="22"/>
+      <c r="T41" s="22"/>
+      <c r="U41" s="22"/>
+      <c r="V41" s="22"/>
+      <c r="W41" s="22"/>
+      <c r="X41" s="22"/>
+    </row>
+    <row r="42" spans="1:24" s="31" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="40"/>
+      <c r="B42" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="C43" s="11" t="s">
+      <c r="C42" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="D43" s="12" t="s">
+      <c r="D42" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="E43" s="25"/>
-      <c r="F43" s="25"/>
-      <c r="G43" s="25"/>
-      <c r="H43" s="25"/>
-      <c r="I43" s="25"/>
-      <c r="J43" s="25"/>
-      <c r="K43" s="25"/>
-      <c r="L43" s="25"/>
-      <c r="M43" s="25"/>
-      <c r="N43" s="25"/>
-      <c r="O43" s="25"/>
-      <c r="P43" s="25"/>
-      <c r="Q43" s="25"/>
-      <c r="R43" s="25"/>
-      <c r="S43" s="25"/>
-      <c r="T43" s="25"/>
-      <c r="U43" s="25"/>
-      <c r="V43" s="25"/>
-      <c r="W43" s="25"/>
-      <c r="X43" s="25"/>
-    </row>
-    <row r="44" spans="1:24" s="34" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="28"/>
-      <c r="B44" s="15" t="s">
+      <c r="E42" s="22"/>
+      <c r="F42" s="22"/>
+      <c r="G42" s="22"/>
+      <c r="H42" s="22"/>
+      <c r="I42" s="22"/>
+      <c r="J42" s="22"/>
+      <c r="K42" s="22"/>
+      <c r="L42" s="22"/>
+      <c r="M42" s="22"/>
+      <c r="N42" s="22"/>
+      <c r="O42" s="22"/>
+      <c r="P42" s="22"/>
+      <c r="Q42" s="22"/>
+      <c r="R42" s="22"/>
+      <c r="S42" s="22"/>
+      <c r="T42" s="22"/>
+      <c r="U42" s="22"/>
+      <c r="V42" s="22"/>
+      <c r="W42" s="22"/>
+      <c r="X42" s="22"/>
+    </row>
+    <row r="43" spans="1:24" s="30" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="41"/>
+      <c r="B43" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="C44" s="10" t="s">
+      <c r="C43" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="D44" s="26" t="s">
+      <c r="D43" s="23" t="s">
         <v>54</v>
       </c>
-      <c r="E44" s="25"/>
-      <c r="F44" s="25"/>
-      <c r="G44" s="25"/>
-      <c r="H44" s="25"/>
-      <c r="I44" s="25"/>
-      <c r="J44" s="25"/>
-      <c r="K44" s="25"/>
-      <c r="L44" s="25"/>
-      <c r="M44" s="25"/>
-      <c r="N44" s="25"/>
-      <c r="O44" s="25"/>
-      <c r="P44" s="25"/>
-      <c r="Q44" s="25"/>
-      <c r="R44" s="25"/>
-      <c r="S44" s="25"/>
-      <c r="T44" s="25"/>
-      <c r="U44" s="25"/>
-      <c r="V44" s="25"/>
-      <c r="W44" s="25"/>
-      <c r="X44" s="25"/>
-    </row>
-    <row r="45" spans="1:24" s="35" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="19" t="s">
+      <c r="E43" s="22"/>
+      <c r="F43" s="22"/>
+      <c r="G43" s="22"/>
+      <c r="H43" s="22"/>
+      <c r="I43" s="22"/>
+      <c r="J43" s="22"/>
+      <c r="K43" s="22"/>
+      <c r="L43" s="22"/>
+      <c r="M43" s="22"/>
+      <c r="N43" s="22"/>
+      <c r="O43" s="22"/>
+      <c r="P43" s="22"/>
+      <c r="Q43" s="22"/>
+      <c r="R43" s="22"/>
+      <c r="S43" s="22"/>
+      <c r="T43" s="22"/>
+      <c r="U43" s="22"/>
+      <c r="V43" s="22"/>
+      <c r="W43" s="22"/>
+      <c r="X43" s="22"/>
+    </row>
+    <row r="44" spans="1:24" s="31" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="42" t="s">
         <v>102</v>
       </c>
-      <c r="B45" s="24" t="s">
+      <c r="B44" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="C45" s="11" t="s">
+      <c r="C44" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="D45" s="12" t="s">
+      <c r="D44" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="E45" s="25"/>
-      <c r="F45" s="25"/>
-      <c r="G45" s="25"/>
-      <c r="H45" s="25"/>
-      <c r="I45" s="25"/>
-      <c r="J45" s="25"/>
-      <c r="K45" s="25"/>
-      <c r="L45" s="25"/>
-      <c r="M45" s="25"/>
-      <c r="N45" s="25"/>
-      <c r="O45" s="25"/>
-      <c r="P45" s="25"/>
-      <c r="Q45" s="25"/>
-      <c r="R45" s="25"/>
-      <c r="S45" s="25"/>
-      <c r="T45" s="25"/>
-      <c r="U45" s="25"/>
-      <c r="V45" s="25"/>
-      <c r="W45" s="25"/>
-      <c r="X45" s="25"/>
-    </row>
-    <row r="46" spans="1:24" s="34" customFormat="1" ht="48.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="19"/>
-      <c r="B46" s="15" t="s">
+      <c r="E44" s="22"/>
+      <c r="F44" s="22"/>
+      <c r="G44" s="22"/>
+      <c r="H44" s="22"/>
+      <c r="I44" s="22"/>
+      <c r="J44" s="22"/>
+      <c r="K44" s="22"/>
+      <c r="L44" s="22"/>
+      <c r="M44" s="22"/>
+      <c r="N44" s="22"/>
+      <c r="O44" s="22"/>
+      <c r="P44" s="22"/>
+      <c r="Q44" s="22"/>
+      <c r="R44" s="22"/>
+      <c r="S44" s="22"/>
+      <c r="T44" s="22"/>
+      <c r="U44" s="22"/>
+      <c r="V44" s="22"/>
+      <c r="W44" s="22"/>
+      <c r="X44" s="22"/>
+    </row>
+    <row r="45" spans="1:24" s="30" customFormat="1" ht="48.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="42"/>
+      <c r="B45" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="C46" s="10" t="s">
+      <c r="C45" s="10" t="s">
         <v>138</v>
       </c>
-      <c r="D46" s="26" t="s">
+      <c r="D45" s="23" t="s">
         <v>54</v>
       </c>
-      <c r="E46" s="25"/>
-      <c r="F46" s="25"/>
-      <c r="G46" s="25"/>
-      <c r="H46" s="25"/>
-      <c r="I46" s="25"/>
-      <c r="J46" s="25"/>
-      <c r="K46" s="25"/>
-      <c r="L46" s="25"/>
-      <c r="M46" s="25"/>
-      <c r="N46" s="25"/>
-      <c r="O46" s="25"/>
-      <c r="P46" s="25"/>
-      <c r="Q46" s="25"/>
-      <c r="R46" s="25"/>
-      <c r="S46" s="25"/>
-      <c r="T46" s="25"/>
-      <c r="U46" s="25"/>
-      <c r="V46" s="25"/>
-      <c r="W46" s="25"/>
-      <c r="X46" s="25"/>
-    </row>
-    <row r="47" spans="1:24" s="34" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="19"/>
-      <c r="B47" s="24" t="s">
+      <c r="E45" s="22"/>
+      <c r="F45" s="22"/>
+      <c r="G45" s="22"/>
+      <c r="H45" s="22"/>
+      <c r="I45" s="22"/>
+      <c r="J45" s="22"/>
+      <c r="K45" s="22"/>
+      <c r="L45" s="22"/>
+      <c r="M45" s="22"/>
+      <c r="N45" s="22"/>
+      <c r="O45" s="22"/>
+      <c r="P45" s="22"/>
+      <c r="Q45" s="22"/>
+      <c r="R45" s="22"/>
+      <c r="S45" s="22"/>
+      <c r="T45" s="22"/>
+      <c r="U45" s="22"/>
+      <c r="V45" s="22"/>
+      <c r="W45" s="22"/>
+      <c r="X45" s="22"/>
+    </row>
+    <row r="46" spans="1:24" s="30" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="42"/>
+      <c r="B46" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="C47" s="11" t="s">
+      <c r="C46" s="11" t="s">
         <v>139</v>
       </c>
-      <c r="D47" s="12" t="s">
+      <c r="D46" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="E47" s="25"/>
-      <c r="F47" s="25"/>
-      <c r="G47" s="25"/>
-      <c r="H47" s="25"/>
-      <c r="I47" s="25"/>
-      <c r="J47" s="25"/>
-      <c r="K47" s="25"/>
-      <c r="L47" s="25"/>
-      <c r="M47" s="25"/>
-      <c r="N47" s="25"/>
-      <c r="O47" s="25"/>
-      <c r="P47" s="25"/>
-      <c r="Q47" s="25"/>
-      <c r="R47" s="25"/>
-      <c r="S47" s="25"/>
-      <c r="T47" s="25"/>
-      <c r="U47" s="25"/>
-      <c r="V47" s="25"/>
-      <c r="W47" s="25"/>
-      <c r="X47" s="25"/>
-    </row>
-    <row r="48" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="19"/>
-      <c r="B48" s="15" t="s">
+      <c r="E46" s="22"/>
+      <c r="F46" s="22"/>
+      <c r="G46" s="22"/>
+      <c r="H46" s="22"/>
+      <c r="I46" s="22"/>
+      <c r="J46" s="22"/>
+      <c r="K46" s="22"/>
+      <c r="L46" s="22"/>
+      <c r="M46" s="22"/>
+      <c r="N46" s="22"/>
+      <c r="O46" s="22"/>
+      <c r="P46" s="22"/>
+      <c r="Q46" s="22"/>
+      <c r="R46" s="22"/>
+      <c r="S46" s="22"/>
+      <c r="T46" s="22"/>
+      <c r="U46" s="22"/>
+      <c r="V46" s="22"/>
+      <c r="W46" s="22"/>
+      <c r="X46" s="22"/>
+    </row>
+    <row r="47" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="42"/>
+      <c r="B47" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="C48" s="10" t="s">
+      <c r="C47" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="D48" s="26" t="s">
+      <c r="D47" s="23" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A49" s="17" t="s">
+    <row r="48" spans="1:24" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A48" s="39" t="s">
         <v>103</v>
       </c>
-      <c r="B49" s="24" t="s">
+      <c r="B48" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="C49" s="11" t="s">
+      <c r="C48" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="D49" s="12" t="s">
+      <c r="D48" s="12" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="18"/>
-      <c r="B50" s="15" t="s">
+    <row r="49" spans="1:4" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="40"/>
+      <c r="B49" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="C50" s="10" t="s">
+      <c r="C49" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="D50" s="26" t="s">
+      <c r="D49" s="23" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="48.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="18"/>
-      <c r="B51" s="24" t="s">
+    <row r="50" spans="1:4" ht="48.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="40"/>
+      <c r="B50" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="C51" s="11" t="s">
+      <c r="C50" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="D51" s="12" t="s">
+      <c r="D50" s="12" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="18"/>
-      <c r="B52" s="15" t="s">
+    <row r="51" spans="1:4" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="40"/>
+      <c r="B51" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="C52" s="10" t="s">
+      <c r="C51" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="D52" s="26" t="s">
+      <c r="D51" s="23" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="28"/>
-      <c r="B53" s="24" t="s">
+    <row r="52" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="41"/>
+      <c r="B52" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="C53" s="11" t="s">
+      <c r="C52" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="D53" s="12" t="s">
+      <c r="D52" s="12" t="s">
         <v>54</v>
       </c>
     </row>
+    <row r="53" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A53" s="36" t="s">
+        <v>104</v>
+      </c>
+      <c r="B53" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="C53" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="D53" s="23" t="s">
+        <v>50</v>
+      </c>
+    </row>
     <row r="54" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A54" s="36" t="s">
-        <v>104</v>
-      </c>
-      <c r="B54" s="15" t="s">
-        <v>77</v>
-      </c>
-      <c r="C54" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="D54" s="26" t="s">
+      <c r="A54" s="37"/>
+      <c r="B54" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="C54" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="D54" s="12" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" s="37"/>
-      <c r="B55" s="24" t="s">
-        <v>78</v>
-      </c>
-      <c r="C55" s="11" t="s">
-        <v>91</v>
-      </c>
-      <c r="D55" s="12" t="s">
+      <c r="B55" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="C55" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="D55" s="23" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A56" s="37"/>
-      <c r="B56" s="15" t="s">
-        <v>79</v>
-      </c>
-      <c r="C56" s="14" t="s">
-        <v>83</v>
-      </c>
-      <c r="D56" s="26" t="s">
+      <c r="B56" s="21" t="s">
+        <v>80</v>
+      </c>
+      <c r="C56" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="D56" s="12" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A57" s="37"/>
-      <c r="B57" s="24" t="s">
-        <v>80</v>
-      </c>
-      <c r="C57" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="D57" s="12" t="s">
+    <row r="57" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A57" s="38"/>
+      <c r="B57" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="C57" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="D57" s="23" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A58" s="38"/>
-      <c r="B58" s="15" t="s">
-        <v>81</v>
-      </c>
-      <c r="C58" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="D58" s="26" t="s">
+    <row r="58" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A58" s="39" t="s">
+        <v>105</v>
+      </c>
+      <c r="B58" s="21" t="s">
+        <v>85</v>
+      </c>
+      <c r="C58" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="D58" s="12" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="59" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A59" s="17" t="s">
-        <v>105</v>
-      </c>
-      <c r="B59" s="24" t="s">
-        <v>85</v>
-      </c>
-      <c r="C59" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="D59" s="12" t="s">
+    <row r="59" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A59" s="40"/>
+      <c r="B59" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="C59" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="D59" s="23" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="60" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A60" s="18"/>
-      <c r="B60" s="15" t="s">
-        <v>86</v>
-      </c>
-      <c r="C60" s="10" t="s">
-        <v>92</v>
-      </c>
-      <c r="D60" s="26" t="s">
+    <row r="60" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A60" s="40"/>
+      <c r="B60" s="21" t="s">
+        <v>87</v>
+      </c>
+      <c r="C60" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="D60" s="12" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="61" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A61" s="18"/>
-      <c r="B61" s="24" t="s">
-        <v>87</v>
-      </c>
-      <c r="C61" s="11" t="s">
-        <v>93</v>
-      </c>
-      <c r="D61" s="12" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="28"/>
-      <c r="B62" s="15" t="s">
+    <row r="61" spans="1:4" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="41"/>
+      <c r="B61" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="C62" s="10" t="s">
+      <c r="C61" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="D62" s="26" t="s">
+      <c r="D61" s="23" t="s">
         <v>50</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A54:A58"/>
-    <mergeCell ref="A59:A62"/>
-    <mergeCell ref="A24:A26"/>
-    <mergeCell ref="A49:A53"/>
-    <mergeCell ref="A42:A44"/>
-    <mergeCell ref="A45:A48"/>
-    <mergeCell ref="A39:A41"/>
-    <mergeCell ref="A12:A21"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="A27:A38"/>
-    <mergeCell ref="A2:A11"/>
+    <mergeCell ref="A11:A20"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="A26:A37"/>
+    <mergeCell ref="A2:A10"/>
+    <mergeCell ref="A53:A57"/>
+    <mergeCell ref="A58:A61"/>
+    <mergeCell ref="A23:A25"/>
+    <mergeCell ref="A48:A52"/>
+    <mergeCell ref="A41:A43"/>
+    <mergeCell ref="A44:A47"/>
+    <mergeCell ref="A38:A40"/>
   </mergeCells>
   <phoneticPr fontId="9" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation allowBlank="1" showDropDown="1" sqref="A22 A12 D2 D22:D41 A2 A25 A27 D59 D55 D57" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
+    <dataValidation allowBlank="1" showDropDown="1" sqref="A21 A11 D2 D21:D40 A2 A24 A26 D58 D54 D56" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2165,10 +2153,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView topLeftCell="A12" zoomScale="111" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2391,16 +2379,30 @@
     </row>
     <row r="16" spans="1:4" ht="55.8" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="D16" s="2">
         <v>45779</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="37.200000000000003" x14ac:dyDescent="0.3">
+      <c r="A17" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="D17" s="2">
+        <v>45780</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
V1.8 updating the crs for the publish article
</commit_message>
<xml_diff>
--- a/LH_REQUIREMENTS/LH_CRS.xlsx
+++ b/LH_REQUIREMENTS/LH_CRS.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BF69CC4-3F6B-4C84-B25B-C5CBCF9DF413}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="20730" windowHeight="11760" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="LH_CRS" sheetId="1" r:id="rId1"/>
@@ -278,17 +277,7 @@
     <t>LH-CRS-PUBLISHARTICLE-004</t>
   </si>
   <si>
-    <t>LH-CRS-PUBLISHARTICLE-005</t>
-  </si>
-  <si>
-    <t>The "Publish" button must remain disabled until the user enters content in the article text area. It must only become active when the input is not empty and within the allowed word count limit.</t>
-  </si>
-  <si>
     <t>Articles must not exceed 1,000 words. The word counter must visibly track the word count as the user types.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">If the word count exceeds 1,000, an error message must be displayed, and the "Publish" button must remain disabled until the word count is reduced within the allowed limit.
-</t>
   </si>
   <si>
     <t>LH-CRS-PUBLISHAUDIO-001</t>
@@ -571,13 +560,23 @@
   </si>
   <si>
     <t>Updated the CRS to reflect the current Registration after Review</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If the word count exceeds 1,000, an error message must be displayed
+</t>
+  </si>
+  <si>
+    <t>V2.8</t>
+  </si>
+  <si>
+    <t>Delete LH_CRS_PUBLISHARTICLE delete the restriction on the publish button to be clickable all the time</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -874,26 +873,26 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1167,30 +1166,30 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:X61"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:X60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="76" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView topLeftCell="A51" zoomScaleNormal="76" workbookViewId="0">
+      <selection activeCell="B57" sqref="A57:XFD57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.109375" style="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.5546875" style="32" customWidth="1"/>
+    <col min="1" max="1" width="18.140625" style="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.5703125" style="32" customWidth="1"/>
     <col min="3" max="3" width="104" style="22" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.109375" style="23" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.88671875" style="22"/>
+    <col min="4" max="4" width="18.140625" style="23" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.85546875" style="22"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="20" customFormat="1" ht="19.2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" s="20" customFormat="1" ht="19.5">
       <c r="A1" s="17" t="s">
         <v>3</v>
       </c>
@@ -1204,22 +1203,22 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="39" t="s">
-        <v>96</v>
+    <row r="2" spans="1:4" ht="30">
+      <c r="A2" s="37" t="s">
+        <v>93</v>
       </c>
       <c r="B2" s="21" t="s">
         <v>9</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="D2" s="12" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="40"/>
+    <row r="3" spans="1:4">
+      <c r="A3" s="39"/>
       <c r="B3" s="15" t="s">
         <v>11</v>
       </c>
@@ -1230,215 +1229,215 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="40"/>
+    <row r="4" spans="1:4">
+      <c r="A4" s="39"/>
       <c r="B4" s="21" t="s">
         <v>12</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="D4" s="12" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="40"/>
+    <row r="5" spans="1:4" ht="30">
+      <c r="A5" s="39"/>
       <c r="B5" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="D5" s="23" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="40"/>
+    <row r="6" spans="1:4">
+      <c r="A6" s="39"/>
       <c r="B6" s="21" t="s">
         <v>14</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="D6" s="12" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="40"/>
+    <row r="7" spans="1:4" ht="30">
+      <c r="A7" s="39"/>
       <c r="B7" s="15" t="s">
         <v>15</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="D7" s="23" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="40"/>
+    <row r="8" spans="1:4" ht="45">
+      <c r="A8" s="39"/>
       <c r="B8" s="21" t="s">
         <v>35</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="D8" s="12" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A9" s="40"/>
+    <row r="9" spans="1:4" ht="30">
+      <c r="A9" s="39"/>
       <c r="B9" s="15" t="s">
         <v>37</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="D9" s="23" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A10" s="41"/>
+    <row r="10" spans="1:4" ht="30">
+      <c r="A10" s="38"/>
       <c r="B10" s="21" t="s">
         <v>38</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="D10" s="12" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="42" t="s">
+    <row r="11" spans="1:4">
+      <c r="A11" s="36" t="s">
+        <v>147</v>
+      </c>
+      <c r="B11" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>158</v>
+      </c>
+      <c r="D11" s="33" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="36"/>
+      <c r="B12" s="25" t="s">
+        <v>149</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>159</v>
+      </c>
+      <c r="D12" s="27" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="36"/>
+      <c r="B13" s="21" t="s">
         <v>150</v>
       </c>
-      <c r="B11" s="21" t="s">
+      <c r="C13" s="11" t="s">
+        <v>160</v>
+      </c>
+      <c r="D13" s="33" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="30">
+      <c r="A14" s="36"/>
+      <c r="B14" s="25" t="s">
         <v>151</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="C14" s="10" t="s">
         <v>161</v>
       </c>
-      <c r="D11" s="33" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="42"/>
-      <c r="B12" s="25" t="s">
+      <c r="D14" s="27" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="36"/>
+      <c r="B15" s="21" t="s">
         <v>152</v>
       </c>
-      <c r="C12" s="10" t="s">
+      <c r="C15" s="34" t="s">
         <v>162</v>
       </c>
-      <c r="D12" s="27" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="42"/>
-      <c r="B13" s="21" t="s">
+      <c r="D15" s="12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="30">
+      <c r="A16" s="36"/>
+      <c r="B16" s="25" t="s">
         <v>153</v>
       </c>
-      <c r="C13" s="11" t="s">
+      <c r="C16" s="10" t="s">
         <v>163</v>
       </c>
-      <c r="D13" s="33" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A14" s="42"/>
-      <c r="B14" s="25" t="s">
+      <c r="D16" s="27" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="30">
+      <c r="A17" s="36"/>
+      <c r="B17" s="21" t="s">
         <v>154</v>
       </c>
-      <c r="C14" s="10" t="s">
+      <c r="C17" s="34" t="s">
         <v>164</v>
       </c>
-      <c r="D14" s="27" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="42"/>
-      <c r="B15" s="21" t="s">
+      <c r="D17" s="12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="36"/>
+      <c r="B18" s="25" t="s">
         <v>155</v>
       </c>
-      <c r="C15" s="34" t="s">
+      <c r="C18" s="10" t="s">
         <v>165</v>
       </c>
-      <c r="D15" s="12" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" s="42"/>
-      <c r="B16" s="25" t="s">
+      <c r="D18" s="27" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="36"/>
+      <c r="B19" s="21" t="s">
         <v>156</v>
       </c>
-      <c r="C16" s="10" t="s">
+      <c r="C19" s="34" t="s">
         <v>166</v>
       </c>
-      <c r="D16" s="27" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="42"/>
-      <c r="B17" s="21" t="s">
+      <c r="D19" s="12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="36"/>
+      <c r="B20" s="25" t="s">
         <v>157</v>
       </c>
-      <c r="C17" s="34" t="s">
+      <c r="C20" s="26" t="s">
         <v>167</v>
       </c>
-      <c r="D17" s="12" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="42"/>
-      <c r="B18" s="25" t="s">
-        <v>158</v>
-      </c>
-      <c r="C18" s="10" t="s">
-        <v>168</v>
-      </c>
-      <c r="D18" s="27" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="42"/>
-      <c r="B19" s="21" t="s">
-        <v>159</v>
-      </c>
-      <c r="C19" s="34" t="s">
-        <v>169</v>
-      </c>
-      <c r="D19" s="12" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="42"/>
-      <c r="B20" s="25" t="s">
-        <v>160</v>
-      </c>
-      <c r="C20" s="26" t="s">
-        <v>170</v>
-      </c>
       <c r="D20" s="27" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="39" t="s">
-        <v>97</v>
+    <row r="21" spans="1:4">
+      <c r="A21" s="37" t="s">
+        <v>94</v>
       </c>
       <c r="B21" s="24" t="s">
         <v>26</v>
@@ -1450,8 +1449,8 @@
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="41"/>
+    <row r="22" spans="1:4">
+      <c r="A22" s="38"/>
       <c r="B22" s="21" t="s">
         <v>29</v>
       </c>
@@ -1462,9 +1461,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" s="42" t="s">
-        <v>98</v>
+    <row r="23" spans="1:4">
+      <c r="A23" s="36" t="s">
+        <v>95</v>
       </c>
       <c r="B23" s="25" t="s">
         <v>27</v>
@@ -1476,8 +1475,8 @@
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" s="42" t="s">
+    <row r="24" spans="1:4">
+      <c r="A24" s="36" t="s">
         <v>4</v>
       </c>
       <c r="B24" s="21" t="s">
@@ -1490,8 +1489,8 @@
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" s="42"/>
+    <row r="25" spans="1:4">
+      <c r="A25" s="36"/>
       <c r="B25" s="15" t="s">
         <v>39</v>
       </c>
@@ -1502,155 +1501,155 @@
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" s="39" t="s">
-        <v>99</v>
+    <row r="26" spans="1:4" ht="30">
+      <c r="A26" s="37" t="s">
+        <v>96</v>
       </c>
       <c r="B26" s="21" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="D26" s="12" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" s="40"/>
+    <row r="27" spans="1:4">
+      <c r="A27" s="39"/>
       <c r="B27" s="28" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C27" s="26" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D27" s="29" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A28" s="40"/>
+    <row r="28" spans="1:4">
+      <c r="A28" s="39"/>
       <c r="B28" s="21" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="D28" s="12" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A29" s="40"/>
+    <row r="29" spans="1:4">
+      <c r="A29" s="39"/>
       <c r="B29" s="28" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C29" s="26" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="D29" s="29" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="40"/>
+    <row r="30" spans="1:4" ht="15" customHeight="1">
+      <c r="A30" s="39"/>
       <c r="B30" s="21" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D30" s="12" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="40"/>
+    <row r="31" spans="1:4" ht="15" customHeight="1">
+      <c r="A31" s="39"/>
       <c r="B31" s="21" t="s">
+        <v>120</v>
+      </c>
+      <c r="C31" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="D31" s="12" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="15" customHeight="1">
+      <c r="A32" s="39"/>
+      <c r="B32" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="C32" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="D32" s="12" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="33" spans="1:24" ht="15" customHeight="1">
+      <c r="A33" s="39"/>
+      <c r="B33" s="21" t="s">
+        <v>122</v>
+      </c>
+      <c r="C33" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="D33" s="12" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="34" spans="1:24" ht="15" customHeight="1">
+      <c r="A34" s="39"/>
+      <c r="B34" s="21" t="s">
         <v>123</v>
       </c>
-      <c r="C31" s="11" t="s">
-        <v>144</v>
-      </c>
-      <c r="D31" s="12" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="40"/>
-      <c r="B32" s="21" t="s">
+      <c r="C34" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="D34" s="12" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="35" spans="1:24" ht="15" customHeight="1">
+      <c r="A35" s="39"/>
+      <c r="B35" s="21" t="s">
         <v>124</v>
       </c>
-      <c r="C32" s="11" t="s">
+      <c r="C35" s="11" t="s">
         <v>128</v>
       </c>
-      <c r="D32" s="12" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="33" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="40"/>
-      <c r="B33" s="21" t="s">
-        <v>125</v>
-      </c>
-      <c r="C33" s="11" t="s">
+      <c r="D35" s="12" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="36" spans="1:24" ht="15" customHeight="1">
+      <c r="A36" s="39"/>
+      <c r="B36" s="21" t="s">
         <v>129</v>
       </c>
-      <c r="D33" s="12" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="34" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="40"/>
-      <c r="B34" s="21" t="s">
-        <v>126</v>
-      </c>
-      <c r="C34" s="11" t="s">
+      <c r="C36" s="11" t="s">
         <v>130</v>
       </c>
-      <c r="D34" s="12" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="35" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="40"/>
-      <c r="B35" s="21" t="s">
-        <v>127</v>
-      </c>
-      <c r="C35" s="11" t="s">
+      <c r="D36" s="12" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="37" spans="1:24" ht="15" customHeight="1">
+      <c r="A37" s="39"/>
+      <c r="B37" s="21" t="s">
         <v>131</v>
       </c>
-      <c r="D35" s="12" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="36" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="40"/>
-      <c r="B36" s="21" t="s">
+      <c r="C37" s="11" t="s">
         <v>132</v>
       </c>
-      <c r="C36" s="11" t="s">
-        <v>133</v>
-      </c>
-      <c r="D36" s="12" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="37" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="40"/>
-      <c r="B37" s="21" t="s">
-        <v>134</v>
-      </c>
-      <c r="C37" s="11" t="s">
-        <v>135</v>
-      </c>
       <c r="D37" s="12" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="38" spans="1:24" s="30" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A38" s="42" t="s">
-        <v>100</v>
+        <v>140</v>
+      </c>
+    </row>
+    <row r="38" spans="1:24" s="30" customFormat="1" ht="45">
+      <c r="A38" s="36" t="s">
+        <v>97</v>
       </c>
       <c r="B38" s="21" t="s">
         <v>30</v>
@@ -1682,8 +1681,8 @@
       <c r="W38" s="22"/>
       <c r="X38" s="22"/>
     </row>
-    <row r="39" spans="1:24" s="31" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A39" s="42"/>
+    <row r="39" spans="1:24" s="31" customFormat="1" ht="45">
+      <c r="A39" s="36"/>
       <c r="B39" s="25" t="s">
         <v>31</v>
       </c>
@@ -1714,8 +1713,8 @@
       <c r="W39" s="22"/>
       <c r="X39" s="22"/>
     </row>
-    <row r="40" spans="1:24" s="30" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A40" s="42"/>
+    <row r="40" spans="1:24" s="30" customFormat="1" ht="30">
+      <c r="A40" s="36"/>
       <c r="B40" s="21" t="s">
         <v>32</v>
       </c>
@@ -1746,9 +1745,9 @@
       <c r="W40" s="22"/>
       <c r="X40" s="22"/>
     </row>
-    <row r="41" spans="1:24" s="30" customFormat="1" ht="78.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="39" t="s">
-        <v>101</v>
+    <row r="41" spans="1:24" s="30" customFormat="1" ht="78.75" customHeight="1">
+      <c r="A41" s="37" t="s">
+        <v>98</v>
       </c>
       <c r="B41" s="15" t="s">
         <v>55</v>
@@ -1780,8 +1779,8 @@
       <c r="W41" s="22"/>
       <c r="X41" s="22"/>
     </row>
-    <row r="42" spans="1:24" s="31" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="40"/>
+    <row r="42" spans="1:24" s="31" customFormat="1" ht="34.5" customHeight="1">
+      <c r="A42" s="39"/>
       <c r="B42" s="21" t="s">
         <v>57</v>
       </c>
@@ -1812,8 +1811,8 @@
       <c r="W42" s="22"/>
       <c r="X42" s="22"/>
     </row>
-    <row r="43" spans="1:24" s="30" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="41"/>
+    <row r="43" spans="1:24" s="30" customFormat="1" ht="34.5" customHeight="1">
+      <c r="A43" s="38"/>
       <c r="B43" s="15" t="s">
         <v>58</v>
       </c>
@@ -1844,9 +1843,9 @@
       <c r="W43" s="22"/>
       <c r="X43" s="22"/>
     </row>
-    <row r="44" spans="1:24" s="31" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="42" t="s">
-        <v>102</v>
+    <row r="44" spans="1:24" s="31" customFormat="1" ht="45" customHeight="1">
+      <c r="A44" s="36" t="s">
+        <v>99</v>
       </c>
       <c r="B44" s="21" t="s">
         <v>60</v>
@@ -1878,13 +1877,13 @@
       <c r="W44" s="22"/>
       <c r="X44" s="22"/>
     </row>
-    <row r="45" spans="1:24" s="30" customFormat="1" ht="48.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="42"/>
+    <row r="45" spans="1:24" s="30" customFormat="1" ht="48.75" customHeight="1">
+      <c r="A45" s="36"/>
       <c r="B45" s="15" t="s">
         <v>61</v>
       </c>
       <c r="C45" s="10" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="D45" s="23" t="s">
         <v>54</v>
@@ -1910,13 +1909,13 @@
       <c r="W45" s="22"/>
       <c r="X45" s="22"/>
     </row>
-    <row r="46" spans="1:24" s="30" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="42"/>
+    <row r="46" spans="1:24" s="30" customFormat="1" ht="35.25" customHeight="1">
+      <c r="A46" s="36"/>
       <c r="B46" s="21" t="s">
         <v>62</v>
       </c>
       <c r="C46" s="11" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D46" s="12" t="s">
         <v>54</v>
@@ -1942,8 +1941,8 @@
       <c r="W46" s="22"/>
       <c r="X46" s="22"/>
     </row>
-    <row r="47" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="42"/>
+    <row r="47" spans="1:24" ht="21" customHeight="1">
+      <c r="A47" s="36"/>
       <c r="B47" s="15" t="s">
         <v>63</v>
       </c>
@@ -1954,9 +1953,9 @@
         <v>54</v>
       </c>
     </row>
-    <row r="48" spans="1:24" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A48" s="39" t="s">
-        <v>103</v>
+    <row r="48" spans="1:24" ht="45">
+      <c r="A48" s="37" t="s">
+        <v>100</v>
       </c>
       <c r="B48" s="21" t="s">
         <v>67</v>
@@ -1968,8 +1967,8 @@
         <v>54</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="40"/>
+    <row r="49" spans="1:4" ht="38.25" customHeight="1">
+      <c r="A49" s="39"/>
       <c r="B49" s="15" t="s">
         <v>68</v>
       </c>
@@ -1980,8 +1979,8 @@
         <v>54</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="48.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="40"/>
+    <row r="50" spans="1:4" ht="48.75" customHeight="1">
+      <c r="A50" s="39"/>
       <c r="B50" s="21" t="s">
         <v>69</v>
       </c>
@@ -1992,8 +1991,8 @@
         <v>54</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="40"/>
+    <row r="51" spans="1:4" ht="50.25" customHeight="1">
+      <c r="A51" s="39"/>
       <c r="B51" s="15" t="s">
         <v>70</v>
       </c>
@@ -2004,8 +2003,8 @@
         <v>54</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="41"/>
+    <row r="52" spans="1:4" ht="36" customHeight="1">
+      <c r="A52" s="38"/>
       <c r="B52" s="21" t="s">
         <v>74</v>
       </c>
@@ -2016,135 +2015,123 @@
         <v>54</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A53" s="36" t="s">
-        <v>104</v>
+    <row r="53" spans="1:4" ht="30">
+      <c r="A53" s="40" t="s">
+        <v>101</v>
       </c>
       <c r="B53" s="15" t="s">
         <v>77</v>
       </c>
       <c r="C53" s="13" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D53" s="23" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A54" s="37"/>
+    <row r="54" spans="1:4" ht="30">
+      <c r="A54" s="41"/>
       <c r="B54" s="21" t="s">
         <v>78</v>
       </c>
       <c r="C54" s="11" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D54" s="12" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A55" s="37"/>
+    <row r="55" spans="1:4">
+      <c r="A55" s="41"/>
       <c r="B55" s="15" t="s">
         <v>79</v>
       </c>
       <c r="C55" s="14" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D55" s="23" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A56" s="37"/>
+    <row r="56" spans="1:4" ht="30">
+      <c r="A56" s="41"/>
       <c r="B56" s="21" t="s">
         <v>80</v>
       </c>
       <c r="C56" s="11" t="s">
-        <v>84</v>
+        <v>175</v>
       </c>
       <c r="D56" s="12" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A57" s="38"/>
-      <c r="B57" s="15" t="s">
-        <v>81</v>
-      </c>
-      <c r="C57" s="10" t="s">
+    <row r="57" spans="1:4" ht="45">
+      <c r="A57" s="37" t="s">
+        <v>102</v>
+      </c>
+      <c r="B57" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="D57" s="23" t="s">
+      <c r="C57" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="D57" s="12" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A58" s="39" t="s">
-        <v>105</v>
-      </c>
-      <c r="B58" s="21" t="s">
+    <row r="58" spans="1:4" ht="30">
+      <c r="A58" s="39"/>
+      <c r="B58" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="C58" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="D58" s="23" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" ht="45">
+      <c r="A59" s="39"/>
+      <c r="B59" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="C59" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="D59" s="12" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" ht="34.5" customHeight="1">
+      <c r="A60" s="38"/>
+      <c r="B60" s="15" t="s">
         <v>85</v>
       </c>
-      <c r="C58" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="D58" s="12" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A59" s="40"/>
-      <c r="B59" s="15" t="s">
-        <v>86</v>
-      </c>
-      <c r="C59" s="10" t="s">
-        <v>92</v>
-      </c>
-      <c r="D59" s="23" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A60" s="40"/>
-      <c r="B60" s="21" t="s">
-        <v>87</v>
-      </c>
-      <c r="C60" s="11" t="s">
-        <v>93</v>
-      </c>
-      <c r="D60" s="12" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="41"/>
-      <c r="B61" s="15" t="s">
-        <v>88</v>
-      </c>
-      <c r="C61" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="D61" s="23" t="s">
+      <c r="C60" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="D60" s="23" t="s">
         <v>50</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A11:A20"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="A26:A37"/>
-    <mergeCell ref="A2:A10"/>
-    <mergeCell ref="A53:A57"/>
-    <mergeCell ref="A58:A61"/>
+    <mergeCell ref="A57:A60"/>
     <mergeCell ref="A23:A25"/>
     <mergeCell ref="A48:A52"/>
     <mergeCell ref="A41:A43"/>
     <mergeCell ref="A44:A47"/>
     <mergeCell ref="A38:A40"/>
+    <mergeCell ref="A11:A20"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="A26:A37"/>
+    <mergeCell ref="A2:A10"/>
+    <mergeCell ref="A53:A56"/>
   </mergeCells>
   <phoneticPr fontId="9" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation allowBlank="1" showDropDown="1" sqref="A21 A11 D2 D21:D40 A2 A24 A26 D58 D54 D56" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
+    <dataValidation allowBlank="1" showDropDown="1" sqref="A21 A11 D2 D21:D40 A2 A24 A26 D57 D54 D56"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2152,22 +2139,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" zoomScale="111" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="111" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17:D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15.44140625" customWidth="1"/>
-    <col min="2" max="2" width="22.6640625" customWidth="1"/>
-    <col min="3" max="3" width="62.109375" customWidth="1"/>
-    <col min="4" max="4" width="18.6640625" customWidth="1"/>
+    <col min="1" max="1" width="15.42578125" customWidth="1"/>
+    <col min="2" max="2" width="22.7109375" customWidth="1"/>
+    <col min="3" max="3" width="62.140625" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="9" customFormat="1" ht="42" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4" s="9" customFormat="1" ht="40.5">
       <c r="A1" s="7" t="s">
         <v>16</v>
       </c>
@@ -2181,7 +2168,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="37.200000000000003" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="37.5">
       <c r="A2" s="5" t="s">
         <v>21</v>
       </c>
@@ -2195,7 +2182,7 @@
         <v>45754</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="37.200000000000003" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="37.5">
       <c r="A3" s="6" t="s">
         <v>22</v>
       </c>
@@ -2209,7 +2196,7 @@
         <v>45754</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="37.200000000000003" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="37.5">
       <c r="A4" s="5" t="s">
         <v>25</v>
       </c>
@@ -2223,7 +2210,7 @@
         <v>45759</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="37.200000000000003" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="37.5">
       <c r="A5" s="6" t="s">
         <v>33</v>
       </c>
@@ -2237,7 +2224,7 @@
         <v>45759</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="37.200000000000003" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" ht="37.5">
       <c r="A6" s="5" t="s">
         <v>40</v>
       </c>
@@ -2251,7 +2238,7 @@
         <v>45765</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="18.600000000000001" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="18.75">
       <c r="A7" s="6" t="s">
         <v>43</v>
       </c>
@@ -2265,7 +2252,7 @@
         <v>45766</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="18.600000000000001" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" ht="18.75">
       <c r="A8" s="5" t="s">
         <v>46</v>
       </c>
@@ -2279,7 +2266,7 @@
         <v>45768</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="18.600000000000001" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" ht="18.75">
       <c r="A9" s="6" t="s">
         <v>51</v>
       </c>
@@ -2293,115 +2280,129 @@
         <v>45776</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="37.200000000000003" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" ht="37.5">
       <c r="A10" s="5" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>54</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D10" s="2">
         <v>45776</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="37.200000000000003" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" ht="37.5">
       <c r="A11" s="6" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="D11" s="4">
         <v>45777</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="55.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" ht="56.25">
       <c r="A12" s="5" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>50</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D12" s="2">
         <v>45777</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="37.200000000000003" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" ht="37.5">
       <c r="A13" s="5" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="D13" s="2">
         <v>45777</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="18.600000000000001" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" ht="18.75">
       <c r="A14" s="5" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>54</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="D14" s="2">
         <v>45778</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="37.200000000000003" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" ht="37.5">
       <c r="A15" s="5" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="D15" s="2">
         <v>45779</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="55.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" ht="56.25">
       <c r="A16" s="5" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="D16" s="2">
         <v>45779</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="37.200000000000003" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" ht="37.5">
       <c r="A17" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="D17" s="2">
+        <v>45780</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="56.25">
+      <c r="A18" s="5" t="s">
         <v>176</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C17" s="1" t="s">
+      <c r="B18" s="42" t="s">
+        <v>138</v>
+      </c>
+      <c r="C18" s="42" t="s">
         <v>177</v>
       </c>
-      <c r="D17" s="2">
+      <c r="D18" s="2">
         <v>45780</v>
       </c>
     </row>

</xml_diff>

<commit_message>
v1.8 updating crs for publish article
</commit_message>
<xml_diff>
--- a/LH_REQUIREMENTS/LH_CRS.xlsx
+++ b/LH_REQUIREMENTS/LH_CRS.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="180">
   <si>
     <t>ID</t>
   </si>
@@ -277,9 +277,6 @@
     <t>LH-CRS-PUBLISHARTICLE-004</t>
   </si>
   <si>
-    <t>Articles must not exceed 1,000 words. The word counter must visibly track the word count as the user types.</t>
-  </si>
-  <si>
     <t>LH-CRS-PUBLISHAUDIO-001</t>
   </si>
   <si>
@@ -299,9 +296,6 @@
     <t>Only registered and logged-in users can access the article publishing interface. After login, users must be able to navigate to the categories page, open a dropdown menu, and select the option to publish an article.</t>
   </si>
   <si>
-    <t>The article interface must include fields for the article title, a text area for article input, a word counter, a cancellation button, and a "Publish" button.</t>
-  </si>
-  <si>
     <t>The audio interface must include an input field for the audio title, an audio length counter that updates in real time as the audio plays, and four buttons: Record, Pause, Cancel, and Publish.</t>
   </si>
   <si>
@@ -569,7 +563,19 @@
     <t>V2.8</t>
   </si>
   <si>
-    <t>Delete LH_CRS_PUBLISHARTICLE delete the restriction on the publish button to be clickable all the time</t>
+    <t>The article interface must include fields for the article title, a text area for article body, a cancellation button, and a "Publish" button.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Article title and article body should not be empty </t>
+  </si>
+  <si>
+    <t>If the article title empty ,error message must be displayed</t>
+  </si>
+  <si>
+    <t>LH-CRS-PUBLISHARTICLE-005</t>
+  </si>
+  <si>
+    <t>update LH_CRS_PUBLISHARTICLE delete the restriction on the publish button to be clickable all the time and error message for empty title</t>
   </si>
 </sst>
 </file>
@@ -873,26 +879,26 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1166,7 +1172,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1174,10 +1180,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X60"/>
+  <dimension ref="A1:X61"/>
   <sheetViews>
     <sheetView topLeftCell="A51" zoomScaleNormal="76" workbookViewId="0">
-      <selection activeCell="B57" sqref="A57:XFD57"/>
+      <selection activeCell="B57" sqref="B57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -1205,20 +1211,20 @@
     </row>
     <row r="2" spans="1:4" ht="30">
       <c r="A2" s="37" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B2" s="21" t="s">
         <v>9</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D2" s="12" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="39"/>
+      <c r="A3" s="38"/>
       <c r="B3" s="15" t="s">
         <v>11</v>
       </c>
@@ -1230,206 +1236,206 @@
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="39"/>
+      <c r="A4" s="38"/>
       <c r="B4" s="21" t="s">
         <v>12</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D4" s="12" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="30">
-      <c r="A5" s="39"/>
+      <c r="A5" s="38"/>
       <c r="B5" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D5" s="23" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="39"/>
+      <c r="A6" s="38"/>
       <c r="B6" s="21" t="s">
         <v>14</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D6" s="12" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="30">
-      <c r="A7" s="39"/>
+      <c r="A7" s="38"/>
       <c r="B7" s="15" t="s">
         <v>15</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D7" s="23" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="45">
-      <c r="A8" s="39"/>
+      <c r="A8" s="38"/>
       <c r="B8" s="21" t="s">
         <v>35</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D8" s="12" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="30">
-      <c r="A9" s="39"/>
+      <c r="A9" s="38"/>
       <c r="B9" s="15" t="s">
         <v>37</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D9" s="23" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="30">
-      <c r="A10" s="38"/>
+      <c r="A10" s="39"/>
       <c r="B10" s="21" t="s">
         <v>38</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D10" s="12" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11" s="36" t="s">
+      <c r="A11" s="40" t="s">
+        <v>145</v>
+      </c>
+      <c r="B11" s="21" t="s">
+        <v>146</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="D11" s="33" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="40"/>
+      <c r="B12" s="25" t="s">
         <v>147</v>
       </c>
-      <c r="B11" s="21" t="s">
+      <c r="C12" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="D12" s="27" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="40"/>
+      <c r="B13" s="21" t="s">
         <v>148</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="C13" s="11" t="s">
         <v>158</v>
       </c>
-      <c r="D11" s="33" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" s="36"/>
-      <c r="B12" s="25" t="s">
+      <c r="D13" s="33" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="30">
+      <c r="A14" s="40"/>
+      <c r="B14" s="25" t="s">
         <v>149</v>
       </c>
-      <c r="C12" s="10" t="s">
+      <c r="C14" s="10" t="s">
         <v>159</v>
       </c>
-      <c r="D12" s="27" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13" s="36"/>
-      <c r="B13" s="21" t="s">
+      <c r="D14" s="27" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="40"/>
+      <c r="B15" s="21" t="s">
         <v>150</v>
       </c>
-      <c r="C13" s="11" t="s">
+      <c r="C15" s="34" t="s">
         <v>160</v>
       </c>
-      <c r="D13" s="33" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="30">
-      <c r="A14" s="36"/>
-      <c r="B14" s="25" t="s">
+      <c r="D15" s="12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="30">
+      <c r="A16" s="40"/>
+      <c r="B16" s="25" t="s">
         <v>151</v>
       </c>
-      <c r="C14" s="10" t="s">
+      <c r="C16" s="10" t="s">
         <v>161</v>
       </c>
-      <c r="D14" s="27" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15" s="36"/>
-      <c r="B15" s="21" t="s">
+      <c r="D16" s="27" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="30">
+      <c r="A17" s="40"/>
+      <c r="B17" s="21" t="s">
         <v>152</v>
       </c>
-      <c r="C15" s="34" t="s">
+      <c r="C17" s="34" t="s">
         <v>162</v>
       </c>
-      <c r="D15" s="12" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="30">
-      <c r="A16" s="36"/>
-      <c r="B16" s="25" t="s">
+      <c r="D17" s="12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="40"/>
+      <c r="B18" s="25" t="s">
         <v>153</v>
       </c>
-      <c r="C16" s="10" t="s">
+      <c r="C18" s="10" t="s">
         <v>163</v>
       </c>
-      <c r="D16" s="27" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="30">
-      <c r="A17" s="36"/>
-      <c r="B17" s="21" t="s">
+      <c r="D18" s="27" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="40"/>
+      <c r="B19" s="21" t="s">
         <v>154</v>
       </c>
-      <c r="C17" s="34" t="s">
+      <c r="C19" s="34" t="s">
         <v>164</v>
       </c>
-      <c r="D17" s="12" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18" s="36"/>
-      <c r="B18" s="25" t="s">
+      <c r="D19" s="12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="40"/>
+      <c r="B20" s="25" t="s">
         <v>155</v>
       </c>
-      <c r="C18" s="10" t="s">
+      <c r="C20" s="26" t="s">
         <v>165</v>
-      </c>
-      <c r="D18" s="27" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19" s="36"/>
-      <c r="B19" s="21" t="s">
-        <v>156</v>
-      </c>
-      <c r="C19" s="34" t="s">
-        <v>166</v>
-      </c>
-      <c r="D19" s="12" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
-      <c r="A20" s="36"/>
-      <c r="B20" s="25" t="s">
-        <v>157</v>
-      </c>
-      <c r="C20" s="26" t="s">
-        <v>167</v>
       </c>
       <c r="D20" s="27" t="s">
         <v>8</v>
@@ -1437,7 +1443,7 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="37" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B21" s="24" t="s">
         <v>26</v>
@@ -1450,7 +1456,7 @@
       </c>
     </row>
     <row r="22" spans="1:4">
-      <c r="A22" s="38"/>
+      <c r="A22" s="39"/>
       <c r="B22" s="21" t="s">
         <v>29</v>
       </c>
@@ -1462,8 +1468,8 @@
       </c>
     </row>
     <row r="23" spans="1:4">
-      <c r="A23" s="36" t="s">
-        <v>95</v>
+      <c r="A23" s="40" t="s">
+        <v>93</v>
       </c>
       <c r="B23" s="25" t="s">
         <v>27</v>
@@ -1476,7 +1482,7 @@
       </c>
     </row>
     <row r="24" spans="1:4">
-      <c r="A24" s="36" t="s">
+      <c r="A24" s="40" t="s">
         <v>4</v>
       </c>
       <c r="B24" s="21" t="s">
@@ -1490,7 +1496,7 @@
       </c>
     </row>
     <row r="25" spans="1:4">
-      <c r="A25" s="36"/>
+      <c r="A25" s="40"/>
       <c r="B25" s="15" t="s">
         <v>39</v>
       </c>
@@ -1503,153 +1509,153 @@
     </row>
     <row r="26" spans="1:4" ht="30">
       <c r="A26" s="37" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B26" s="21" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D26" s="12" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="27" spans="1:4">
-      <c r="A27" s="39"/>
+      <c r="A27" s="38"/>
       <c r="B27" s="28" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C27" s="26" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D27" s="29" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="28" spans="1:4">
-      <c r="A28" s="39"/>
+      <c r="A28" s="38"/>
       <c r="B28" s="21" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D28" s="12" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="29" spans="1:4">
-      <c r="A29" s="39"/>
+      <c r="A29" s="38"/>
       <c r="B29" s="28" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C29" s="26" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D29" s="29" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="15" customHeight="1">
-      <c r="A30" s="39"/>
+      <c r="A30" s="38"/>
       <c r="B30" s="21" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D30" s="12" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="15" customHeight="1">
-      <c r="A31" s="39"/>
+      <c r="A31" s="38"/>
       <c r="B31" s="21" t="s">
+        <v>118</v>
+      </c>
+      <c r="C31" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="D31" s="12" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="15" customHeight="1">
+      <c r="A32" s="38"/>
+      <c r="B32" s="21" t="s">
+        <v>119</v>
+      </c>
+      <c r="C32" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="D32" s="12" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="33" spans="1:24" ht="15" customHeight="1">
+      <c r="A33" s="38"/>
+      <c r="B33" s="21" t="s">
         <v>120</v>
       </c>
-      <c r="C31" s="11" t="s">
-        <v>141</v>
-      </c>
-      <c r="D31" s="12" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="15" customHeight="1">
-      <c r="A32" s="39"/>
-      <c r="B32" s="21" t="s">
+      <c r="C33" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="D33" s="12" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="34" spans="1:24" ht="15" customHeight="1">
+      <c r="A34" s="38"/>
+      <c r="B34" s="21" t="s">
         <v>121</v>
       </c>
-      <c r="C32" s="11" t="s">
+      <c r="C34" s="11" t="s">
         <v>125</v>
       </c>
-      <c r="D32" s="12" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="33" spans="1:24" ht="15" customHeight="1">
-      <c r="A33" s="39"/>
-      <c r="B33" s="21" t="s">
+      <c r="D34" s="12" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="35" spans="1:24" ht="15" customHeight="1">
+      <c r="A35" s="38"/>
+      <c r="B35" s="21" t="s">
         <v>122</v>
       </c>
-      <c r="C33" s="11" t="s">
+      <c r="C35" s="11" t="s">
         <v>126</v>
       </c>
-      <c r="D33" s="12" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="34" spans="1:24" ht="15" customHeight="1">
-      <c r="A34" s="39"/>
-      <c r="B34" s="21" t="s">
-        <v>123</v>
-      </c>
-      <c r="C34" s="11" t="s">
+      <c r="D35" s="12" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="36" spans="1:24" ht="15" customHeight="1">
+      <c r="A36" s="38"/>
+      <c r="B36" s="21" t="s">
         <v>127</v>
       </c>
-      <c r="D34" s="12" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="35" spans="1:24" ht="15" customHeight="1">
-      <c r="A35" s="39"/>
-      <c r="B35" s="21" t="s">
-        <v>124</v>
-      </c>
-      <c r="C35" s="11" t="s">
+      <c r="C36" s="11" t="s">
         <v>128</v>
       </c>
-      <c r="D35" s="12" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="36" spans="1:24" ht="15" customHeight="1">
-      <c r="A36" s="39"/>
-      <c r="B36" s="21" t="s">
+      <c r="D36" s="12" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="37" spans="1:24" ht="15" customHeight="1">
+      <c r="A37" s="38"/>
+      <c r="B37" s="21" t="s">
         <v>129</v>
       </c>
-      <c r="C36" s="11" t="s">
+      <c r="C37" s="11" t="s">
         <v>130</v>
       </c>
-      <c r="D36" s="12" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="37" spans="1:24" ht="15" customHeight="1">
-      <c r="A37" s="39"/>
-      <c r="B37" s="21" t="s">
-        <v>131</v>
-      </c>
-      <c r="C37" s="11" t="s">
-        <v>132</v>
-      </c>
       <c r="D37" s="12" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="38" spans="1:24" s="30" customFormat="1" ht="45">
-      <c r="A38" s="36" t="s">
-        <v>97</v>
+      <c r="A38" s="40" t="s">
+        <v>95</v>
       </c>
       <c r="B38" s="21" t="s">
         <v>30</v>
@@ -1682,7 +1688,7 @@
       <c r="X38" s="22"/>
     </row>
     <row r="39" spans="1:24" s="31" customFormat="1" ht="45">
-      <c r="A39" s="36"/>
+      <c r="A39" s="40"/>
       <c r="B39" s="25" t="s">
         <v>31</v>
       </c>
@@ -1714,7 +1720,7 @@
       <c r="X39" s="22"/>
     </row>
     <row r="40" spans="1:24" s="30" customFormat="1" ht="30">
-      <c r="A40" s="36"/>
+      <c r="A40" s="40"/>
       <c r="B40" s="21" t="s">
         <v>32</v>
       </c>
@@ -1747,7 +1753,7 @@
     </row>
     <row r="41" spans="1:24" s="30" customFormat="1" ht="78.75" customHeight="1">
       <c r="A41" s="37" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B41" s="15" t="s">
         <v>55</v>
@@ -1780,7 +1786,7 @@
       <c r="X41" s="22"/>
     </row>
     <row r="42" spans="1:24" s="31" customFormat="1" ht="34.5" customHeight="1">
-      <c r="A42" s="39"/>
+      <c r="A42" s="38"/>
       <c r="B42" s="21" t="s">
         <v>57</v>
       </c>
@@ -1812,7 +1818,7 @@
       <c r="X42" s="22"/>
     </row>
     <row r="43" spans="1:24" s="30" customFormat="1" ht="34.5" customHeight="1">
-      <c r="A43" s="38"/>
+      <c r="A43" s="39"/>
       <c r="B43" s="15" t="s">
         <v>58</v>
       </c>
@@ -1844,8 +1850,8 @@
       <c r="X43" s="22"/>
     </row>
     <row r="44" spans="1:24" s="31" customFormat="1" ht="45" customHeight="1">
-      <c r="A44" s="36" t="s">
-        <v>99</v>
+      <c r="A44" s="40" t="s">
+        <v>97</v>
       </c>
       <c r="B44" s="21" t="s">
         <v>60</v>
@@ -1878,12 +1884,12 @@
       <c r="X44" s="22"/>
     </row>
     <row r="45" spans="1:24" s="30" customFormat="1" ht="48.75" customHeight="1">
-      <c r="A45" s="36"/>
+      <c r="A45" s="40"/>
       <c r="B45" s="15" t="s">
         <v>61</v>
       </c>
       <c r="C45" s="10" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D45" s="23" t="s">
         <v>54</v>
@@ -1910,12 +1916,12 @@
       <c r="X45" s="22"/>
     </row>
     <row r="46" spans="1:24" s="30" customFormat="1" ht="35.25" customHeight="1">
-      <c r="A46" s="36"/>
+      <c r="A46" s="40"/>
       <c r="B46" s="21" t="s">
         <v>62</v>
       </c>
       <c r="C46" s="11" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D46" s="12" t="s">
         <v>54</v>
@@ -1942,7 +1948,7 @@
       <c r="X46" s="22"/>
     </row>
     <row r="47" spans="1:24" ht="21" customHeight="1">
-      <c r="A47" s="36"/>
+      <c r="A47" s="40"/>
       <c r="B47" s="15" t="s">
         <v>63</v>
       </c>
@@ -1955,7 +1961,7 @@
     </row>
     <row r="48" spans="1:24" ht="45">
       <c r="A48" s="37" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B48" s="21" t="s">
         <v>67</v>
@@ -1968,7 +1974,7 @@
       </c>
     </row>
     <row r="49" spans="1:4" ht="38.25" customHeight="1">
-      <c r="A49" s="39"/>
+      <c r="A49" s="38"/>
       <c r="B49" s="15" t="s">
         <v>68</v>
       </c>
@@ -1980,7 +1986,7 @@
       </c>
     </row>
     <row r="50" spans="1:4" ht="48.75" customHeight="1">
-      <c r="A50" s="39"/>
+      <c r="A50" s="38"/>
       <c r="B50" s="21" t="s">
         <v>69</v>
       </c>
@@ -1992,7 +1998,7 @@
       </c>
     </row>
     <row r="51" spans="1:4" ht="50.25" customHeight="1">
-      <c r="A51" s="39"/>
+      <c r="A51" s="38"/>
       <c r="B51" s="15" t="s">
         <v>70</v>
       </c>
@@ -2004,7 +2010,7 @@
       </c>
     </row>
     <row r="52" spans="1:4" ht="36" customHeight="1">
-      <c r="A52" s="38"/>
+      <c r="A52" s="39"/>
       <c r="B52" s="21" t="s">
         <v>74</v>
       </c>
@@ -2016,122 +2022,134 @@
       </c>
     </row>
     <row r="53" spans="1:4" ht="30">
-      <c r="A53" s="40" t="s">
-        <v>101</v>
+      <c r="A53" s="41" t="s">
+        <v>99</v>
       </c>
       <c r="B53" s="15" t="s">
         <v>77</v>
       </c>
       <c r="C53" s="13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D53" s="23" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="30">
-      <c r="A54" s="41"/>
+      <c r="A54" s="42"/>
       <c r="B54" s="21" t="s">
         <v>78</v>
       </c>
       <c r="C54" s="11" t="s">
-        <v>88</v>
+        <v>175</v>
       </c>
       <c r="D54" s="12" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="55" spans="1:4">
-      <c r="A55" s="41"/>
+      <c r="A55" s="42"/>
       <c r="B55" s="15" t="s">
         <v>79</v>
       </c>
       <c r="C55" s="14" t="s">
-        <v>81</v>
+        <v>176</v>
       </c>
       <c r="D55" s="23" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="30">
-      <c r="A56" s="41"/>
-      <c r="B56" s="21" t="s">
+    <row r="56" spans="1:4">
+      <c r="A56" s="42"/>
+      <c r="B56" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="C56" s="11" t="s">
-        <v>175</v>
-      </c>
-      <c r="D56" s="12" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" ht="45">
-      <c r="A57" s="37" t="s">
-        <v>102</v>
-      </c>
+      <c r="C56" s="14" t="s">
+        <v>177</v>
+      </c>
+      <c r="D56" s="23" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" ht="30">
+      <c r="A57" s="42"/>
       <c r="B57" s="21" t="s">
-        <v>82</v>
+        <v>178</v>
       </c>
       <c r="C57" s="11" t="s">
-        <v>86</v>
+        <v>173</v>
       </c>
       <c r="D57" s="12" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="30">
-      <c r="A58" s="39"/>
-      <c r="B58" s="15" t="s">
+    <row r="58" spans="1:4" ht="45">
+      <c r="A58" s="37" t="s">
+        <v>100</v>
+      </c>
+      <c r="B58" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="C58" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="D58" s="12" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" ht="30">
+      <c r="A59" s="38"/>
+      <c r="B59" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="C59" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="D59" s="23" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" ht="45">
+      <c r="A60" s="38"/>
+      <c r="B60" s="21" t="s">
         <v>83</v>
       </c>
-      <c r="C58" s="10" t="s">
+      <c r="C60" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="D60" s="12" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" ht="34.5" customHeight="1">
+      <c r="A61" s="39"/>
+      <c r="B61" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="C61" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="D58" s="23" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" ht="45">
-      <c r="A59" s="39"/>
-      <c r="B59" s="21" t="s">
-        <v>84</v>
-      </c>
-      <c r="C59" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="D59" s="12" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" ht="34.5" customHeight="1">
-      <c r="A60" s="38"/>
-      <c r="B60" s="15" t="s">
-        <v>85</v>
-      </c>
-      <c r="C60" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="D60" s="23" t="s">
+      <c r="D61" s="23" t="s">
         <v>50</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A57:A60"/>
+    <mergeCell ref="A11:A20"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="A26:A37"/>
+    <mergeCell ref="A2:A10"/>
+    <mergeCell ref="A53:A57"/>
+    <mergeCell ref="A58:A61"/>
     <mergeCell ref="A23:A25"/>
     <mergeCell ref="A48:A52"/>
     <mergeCell ref="A41:A43"/>
     <mergeCell ref="A44:A47"/>
     <mergeCell ref="A38:A40"/>
-    <mergeCell ref="A11:A20"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="A26:A37"/>
-    <mergeCell ref="A2:A10"/>
-    <mergeCell ref="A53:A56"/>
   </mergeCells>
   <phoneticPr fontId="9" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation allowBlank="1" showDropDown="1" sqref="A21 A11 D2 D21:D40 A2 A24 A26 D57 D54 D56"/>
+    <dataValidation allowBlank="1" showDropDown="1" sqref="A21 A11 D2 D21:D40 A2 A24 A26 D54 D57:D58"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2143,7 +2161,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A12" zoomScale="111" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17:D18"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2282,13 +2300,13 @@
     </row>
     <row r="10" spans="1:4" ht="37.5">
       <c r="A10" s="5" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>54</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D10" s="2">
         <v>45776</v>
@@ -2296,13 +2314,13 @@
     </row>
     <row r="11" spans="1:4" ht="37.5">
       <c r="A11" s="6" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D11" s="4">
         <v>45777</v>
@@ -2310,13 +2328,13 @@
     </row>
     <row r="12" spans="1:4" ht="56.25">
       <c r="A12" s="5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>50</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D12" s="2">
         <v>45777</v>
@@ -2324,13 +2342,13 @@
     </row>
     <row r="13" spans="1:4" ht="37.5">
       <c r="A13" s="5" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D13" s="2">
         <v>45777</v>
@@ -2338,13 +2356,13 @@
     </row>
     <row r="14" spans="1:4" ht="18.75">
       <c r="A14" s="5" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>54</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D14" s="2">
         <v>45778</v>
@@ -2352,13 +2370,13 @@
     </row>
     <row r="15" spans="1:4" ht="37.5">
       <c r="A15" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>137</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>139</v>
       </c>
       <c r="D15" s="2">
         <v>45779</v>
@@ -2366,13 +2384,13 @@
     </row>
     <row r="16" spans="1:4" ht="56.25">
       <c r="A16" s="5" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D16" s="2">
         <v>45779</v>
@@ -2380,13 +2398,13 @@
     </row>
     <row r="17" spans="1:4" ht="37.5">
       <c r="A17" s="5" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D17" s="2">
         <v>45780</v>
@@ -2394,13 +2412,13 @@
     </row>
     <row r="18" spans="1:4" ht="56.25">
       <c r="A18" s="5" t="s">
-        <v>176</v>
-      </c>
-      <c r="B18" s="42" t="s">
-        <v>138</v>
-      </c>
-      <c r="C18" s="42" t="s">
-        <v>177</v>
+        <v>174</v>
+      </c>
+      <c r="B18" s="36" t="s">
+        <v>136</v>
+      </c>
+      <c r="C18" s="36" t="s">
+        <v>179</v>
       </c>
       <c r="D18" s="2">
         <v>45780</v>

</xml_diff>

<commit_message>
v2.9 updated publish audio feature
</commit_message>
<xml_diff>
--- a/LH_REQUIREMENTS/LH_CRS.xlsx
+++ b/LH_REQUIREMENTS/LH_CRS.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20417"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="8_{DE6D1FF1-3C9B-40C5-9432-277D1219FD8E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{3584282E-462C-498C-811A-A8066852D4C8}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="20730" windowHeight="11760" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6945" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LH_CRS" sheetId="1" r:id="rId1"/>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="182">
   <si>
     <t>ID</t>
   </si>
@@ -289,17 +290,7 @@
     <t>LH-CRS-PUBLISHAUDIO-004</t>
   </si>
   <si>
-    <t xml:space="preserve">Only registered and logged-in users can access the audio publishing interface. After login, users must be able to navigate to the categories page, open a dropdown menu, and select the option to publish an audio recording.
-</t>
-  </si>
-  <si>
     <t>Only registered and logged-in users can access the article publishing interface. After login, users must be able to navigate to the categories page, open a dropdown menu, and select the option to publish an article.</t>
-  </si>
-  <si>
-    <t>The audio interface must include an input field for the audio title, an audio length counter that updates in real time as the audio plays, and four buttons: Record, Pause, Cancel, and Publish.</t>
-  </si>
-  <si>
-    <t>The maximum allowed upload size for audio recordings must be 20 MB. In addition, the duration of the audio must not exceed 5 minutes. If either limit is exceeded, an appropriate error message must be displayed, and the "Publish" button must remain inactive until the issue is resolved.</t>
   </si>
   <si>
     <t>The "Publish" button must remain disabled until the user records an audio clip and provides a title. It must only become active when both the audio duration is within the allowed limit and the title input is not empty.</t>
@@ -556,32 +547,47 @@
     <t>Updated the CRS to reflect the current Registration after Review</t>
   </si>
   <si>
-    <t xml:space="preserve">If the word count exceeds 1,000, an error message must be displayed
+    <t>V2.8</t>
+  </si>
+  <si>
+    <t>The article interface must include fields for the article title, a text area for article body, a cancellation button, and a "Publish" button.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Article title and article body should not be empty </t>
+  </si>
+  <si>
+    <t>If the article title empty ,error message must be displayed</t>
+  </si>
+  <si>
+    <t>LH-CRS-PUBLISHARTICLE-005</t>
+  </si>
+  <si>
+    <t>update LH_CRS_PUBLISHARTICLE delete the restriction on the publish button to be clickable all the time and error message for empty title</t>
+  </si>
+  <si>
+    <t>Only registered and logged-in users can access the audio publishing interface that found in a publish drop down in categories page.</t>
+  </si>
+  <si>
+    <t>Only registered and logged-in users can recored a voice note and set a title for it then publish it.</t>
+  </si>
+  <si>
+    <t>The user can record a voice message for up to 5 minutes. If the time limit is exceeded,a message will appear explaining this.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If the word count exceeds 1,000, an error message must be displayed.
 </t>
   </si>
   <si>
-    <t>V2.8</t>
-  </si>
-  <si>
-    <t>The article interface must include fields for the article title, a text area for article body, a cancellation button, and a "Publish" button.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Article title and article body should not be empty </t>
-  </si>
-  <si>
-    <t>If the article title empty ,error message must be displayed</t>
-  </si>
-  <si>
-    <t>LH-CRS-PUBLISHARTICLE-005</t>
-  </si>
-  <si>
-    <t>update LH_CRS_PUBLISHARTICLE delete the restriction on the publish button to be clickable all the time and error message for empty title</t>
+    <t>v2.9</t>
+  </si>
+  <si>
+    <t>updated publish audio feature according to the review</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="10">
     <font>
       <sz val="11"/>
@@ -882,16 +888,16 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1172,18 +1178,18 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X61"/>
   <sheetViews>
-    <sheetView topLeftCell="A51" zoomScaleNormal="76" workbookViewId="0">
-      <selection activeCell="B57" sqref="B57"/>
+    <sheetView topLeftCell="A52" zoomScaleNormal="76" workbookViewId="0">
+      <selection activeCell="C57" sqref="C57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -1210,21 +1216,21 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="30">
-      <c r="A2" s="37" t="s">
-        <v>91</v>
+      <c r="A2" s="38" t="s">
+        <v>88</v>
       </c>
       <c r="B2" s="21" t="s">
         <v>9</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="D2" s="12" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="38"/>
+      <c r="A3" s="40"/>
       <c r="B3" s="15" t="s">
         <v>11</v>
       </c>
@@ -1236,72 +1242,72 @@
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="38"/>
+      <c r="A4" s="40"/>
       <c r="B4" s="21" t="s">
         <v>12</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D4" s="12" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="30">
-      <c r="A5" s="38"/>
+      <c r="A5" s="40"/>
       <c r="B5" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="D5" s="23" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="38"/>
+      <c r="A6" s="40"/>
       <c r="B6" s="21" t="s">
         <v>14</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="D6" s="12" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="30">
-      <c r="A7" s="38"/>
+      <c r="A7" s="40"/>
       <c r="B7" s="15" t="s">
         <v>15</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="D7" s="23" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="45">
-      <c r="A8" s="38"/>
+      <c r="A8" s="40"/>
       <c r="B8" s="21" t="s">
         <v>35</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="D8" s="12" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="30">
-      <c r="A9" s="38"/>
+      <c r="A9" s="40"/>
       <c r="B9" s="15" t="s">
         <v>37</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="D9" s="23" t="s">
         <v>8</v>
@@ -1313,137 +1319,137 @@
         <v>38</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="D10" s="12" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11" s="40" t="s">
+      <c r="A11" s="37" t="s">
+        <v>142</v>
+      </c>
+      <c r="B11" s="21" t="s">
+        <v>143</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="D11" s="33" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="37"/>
+      <c r="B12" s="25" t="s">
+        <v>144</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>154</v>
+      </c>
+      <c r="D12" s="27" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="37"/>
+      <c r="B13" s="21" t="s">
         <v>145</v>
       </c>
-      <c r="B11" s="21" t="s">
+      <c r="C13" s="11" t="s">
+        <v>155</v>
+      </c>
+      <c r="D13" s="33" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="30">
+      <c r="A14" s="37"/>
+      <c r="B14" s="25" t="s">
         <v>146</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="C14" s="10" t="s">
         <v>156</v>
       </c>
-      <c r="D11" s="33" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" s="40"/>
-      <c r="B12" s="25" t="s">
+      <c r="D14" s="27" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="37"/>
+      <c r="B15" s="21" t="s">
         <v>147</v>
       </c>
-      <c r="C12" s="10" t="s">
+      <c r="C15" s="34" t="s">
         <v>157</v>
       </c>
-      <c r="D12" s="27" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13" s="40"/>
-      <c r="B13" s="21" t="s">
+      <c r="D15" s="12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="30">
+      <c r="A16" s="37"/>
+      <c r="B16" s="25" t="s">
         <v>148</v>
       </c>
-      <c r="C13" s="11" t="s">
+      <c r="C16" s="10" t="s">
         <v>158</v>
       </c>
-      <c r="D13" s="33" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="30">
-      <c r="A14" s="40"/>
-      <c r="B14" s="25" t="s">
+      <c r="D16" s="27" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="30">
+      <c r="A17" s="37"/>
+      <c r="B17" s="21" t="s">
         <v>149</v>
       </c>
-      <c r="C14" s="10" t="s">
+      <c r="C17" s="34" t="s">
         <v>159</v>
       </c>
-      <c r="D14" s="27" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15" s="40"/>
-      <c r="B15" s="21" t="s">
+      <c r="D17" s="12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="37"/>
+      <c r="B18" s="25" t="s">
         <v>150</v>
       </c>
-      <c r="C15" s="34" t="s">
+      <c r="C18" s="10" t="s">
         <v>160</v>
       </c>
-      <c r="D15" s="12" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="30">
-      <c r="A16" s="40"/>
-      <c r="B16" s="25" t="s">
+      <c r="D18" s="27" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="37"/>
+      <c r="B19" s="21" t="s">
         <v>151</v>
       </c>
-      <c r="C16" s="10" t="s">
+      <c r="C19" s="34" t="s">
         <v>161</v>
       </c>
-      <c r="D16" s="27" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="30">
-      <c r="A17" s="40"/>
-      <c r="B17" s="21" t="s">
+      <c r="D19" s="12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="37"/>
+      <c r="B20" s="25" t="s">
         <v>152</v>
       </c>
-      <c r="C17" s="34" t="s">
+      <c r="C20" s="26" t="s">
         <v>162</v>
       </c>
-      <c r="D17" s="12" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18" s="40"/>
-      <c r="B18" s="25" t="s">
-        <v>153</v>
-      </c>
-      <c r="C18" s="10" t="s">
-        <v>163</v>
-      </c>
-      <c r="D18" s="27" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19" s="40"/>
-      <c r="B19" s="21" t="s">
-        <v>154</v>
-      </c>
-      <c r="C19" s="34" t="s">
-        <v>164</v>
-      </c>
-      <c r="D19" s="12" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
-      <c r="A20" s="40"/>
-      <c r="B20" s="25" t="s">
-        <v>155</v>
-      </c>
-      <c r="C20" s="26" t="s">
-        <v>165</v>
-      </c>
       <c r="D20" s="27" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="21" spans="1:4">
-      <c r="A21" s="37" t="s">
-        <v>92</v>
+      <c r="A21" s="38" t="s">
+        <v>89</v>
       </c>
       <c r="B21" s="24" t="s">
         <v>26</v>
@@ -1468,8 +1474,8 @@
       </c>
     </row>
     <row r="23" spans="1:4">
-      <c r="A23" s="40" t="s">
-        <v>93</v>
+      <c r="A23" s="37" t="s">
+        <v>90</v>
       </c>
       <c r="B23" s="25" t="s">
         <v>27</v>
@@ -1482,7 +1488,7 @@
       </c>
     </row>
     <row r="24" spans="1:4">
-      <c r="A24" s="40" t="s">
+      <c r="A24" s="37" t="s">
         <v>4</v>
       </c>
       <c r="B24" s="21" t="s">
@@ -1496,7 +1502,7 @@
       </c>
     </row>
     <row r="25" spans="1:4">
-      <c r="A25" s="40"/>
+      <c r="A25" s="37"/>
       <c r="B25" s="15" t="s">
         <v>39</v>
       </c>
@@ -1508,154 +1514,154 @@
       </c>
     </row>
     <row r="26" spans="1:4" ht="30">
-      <c r="A26" s="37" t="s">
-        <v>94</v>
+      <c r="A26" s="38" t="s">
+        <v>91</v>
       </c>
       <c r="B26" s="21" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D26" s="12" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="27" spans="1:4">
-      <c r="A27" s="38"/>
+      <c r="A27" s="40"/>
       <c r="B27" s="28" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C27" s="26" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D27" s="29" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="28" spans="1:4">
-      <c r="A28" s="38"/>
+      <c r="A28" s="40"/>
       <c r="B28" s="21" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="D28" s="12" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="29" spans="1:4">
-      <c r="A29" s="38"/>
+      <c r="A29" s="40"/>
       <c r="B29" s="28" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C29" s="26" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D29" s="29" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="15" customHeight="1">
-      <c r="A30" s="38"/>
+      <c r="A30" s="40"/>
       <c r="B30" s="21" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="D30" s="12" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="15" customHeight="1">
-      <c r="A31" s="38"/>
+      <c r="A31" s="40"/>
       <c r="B31" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="C31" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="D31" s="12" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="15" customHeight="1">
+      <c r="A32" s="40"/>
+      <c r="B32" s="21" t="s">
+        <v>116</v>
+      </c>
+      <c r="C32" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="D32" s="12" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="33" spans="1:24" ht="15" customHeight="1">
+      <c r="A33" s="40"/>
+      <c r="B33" s="21" t="s">
+        <v>117</v>
+      </c>
+      <c r="C33" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="D33" s="12" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="34" spans="1:24" ht="15" customHeight="1">
+      <c r="A34" s="40"/>
+      <c r="B34" s="21" t="s">
         <v>118</v>
       </c>
-      <c r="C31" s="11" t="s">
-        <v>139</v>
-      </c>
-      <c r="D31" s="12" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="15" customHeight="1">
-      <c r="A32" s="38"/>
-      <c r="B32" s="21" t="s">
+      <c r="C34" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="D34" s="12" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="35" spans="1:24" ht="15" customHeight="1">
+      <c r="A35" s="40"/>
+      <c r="B35" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="C32" s="11" t="s">
+      <c r="C35" s="11" t="s">
         <v>123</v>
       </c>
-      <c r="D32" s="12" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="33" spans="1:24" ht="15" customHeight="1">
-      <c r="A33" s="38"/>
-      <c r="B33" s="21" t="s">
-        <v>120</v>
-      </c>
-      <c r="C33" s="11" t="s">
+      <c r="D35" s="12" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="36" spans="1:24" ht="15" customHeight="1">
+      <c r="A36" s="40"/>
+      <c r="B36" s="21" t="s">
         <v>124</v>
       </c>
-      <c r="D33" s="12" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="34" spans="1:24" ht="15" customHeight="1">
-      <c r="A34" s="38"/>
-      <c r="B34" s="21" t="s">
-        <v>121</v>
-      </c>
-      <c r="C34" s="11" t="s">
+      <c r="C36" s="11" t="s">
         <v>125</v>
       </c>
-      <c r="D34" s="12" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="35" spans="1:24" ht="15" customHeight="1">
-      <c r="A35" s="38"/>
-      <c r="B35" s="21" t="s">
-        <v>122</v>
-      </c>
-      <c r="C35" s="11" t="s">
+      <c r="D36" s="12" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="37" spans="1:24" ht="15" customHeight="1">
+      <c r="A37" s="40"/>
+      <c r="B37" s="21" t="s">
         <v>126</v>
       </c>
-      <c r="D35" s="12" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="36" spans="1:24" ht="15" customHeight="1">
-      <c r="A36" s="38"/>
-      <c r="B36" s="21" t="s">
+      <c r="C37" s="11" t="s">
         <v>127</v>
       </c>
-      <c r="C36" s="11" t="s">
-        <v>128</v>
-      </c>
-      <c r="D36" s="12" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="37" spans="1:24" ht="15" customHeight="1">
-      <c r="A37" s="38"/>
-      <c r="B37" s="21" t="s">
-        <v>129</v>
-      </c>
-      <c r="C37" s="11" t="s">
-        <v>130</v>
-      </c>
       <c r="D37" s="12" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="38" spans="1:24" s="30" customFormat="1" ht="45">
-      <c r="A38" s="40" t="s">
-        <v>95</v>
+      <c r="A38" s="37" t="s">
+        <v>92</v>
       </c>
       <c r="B38" s="21" t="s">
         <v>30</v>
@@ -1688,7 +1694,7 @@
       <c r="X38" s="22"/>
     </row>
     <row r="39" spans="1:24" s="31" customFormat="1" ht="45">
-      <c r="A39" s="40"/>
+      <c r="A39" s="37"/>
       <c r="B39" s="25" t="s">
         <v>31</v>
       </c>
@@ -1720,7 +1726,7 @@
       <c r="X39" s="22"/>
     </row>
     <row r="40" spans="1:24" s="30" customFormat="1" ht="30">
-      <c r="A40" s="40"/>
+      <c r="A40" s="37"/>
       <c r="B40" s="21" t="s">
         <v>32</v>
       </c>
@@ -1752,8 +1758,8 @@
       <c r="X40" s="22"/>
     </row>
     <row r="41" spans="1:24" s="30" customFormat="1" ht="78.75" customHeight="1">
-      <c r="A41" s="37" t="s">
-        <v>96</v>
+      <c r="A41" s="38" t="s">
+        <v>93</v>
       </c>
       <c r="B41" s="15" t="s">
         <v>55</v>
@@ -1786,7 +1792,7 @@
       <c r="X41" s="22"/>
     </row>
     <row r="42" spans="1:24" s="31" customFormat="1" ht="34.5" customHeight="1">
-      <c r="A42" s="38"/>
+      <c r="A42" s="40"/>
       <c r="B42" s="21" t="s">
         <v>57</v>
       </c>
@@ -1850,8 +1856,8 @@
       <c r="X43" s="22"/>
     </row>
     <row r="44" spans="1:24" s="31" customFormat="1" ht="45" customHeight="1">
-      <c r="A44" s="40" t="s">
-        <v>97</v>
+      <c r="A44" s="37" t="s">
+        <v>94</v>
       </c>
       <c r="B44" s="21" t="s">
         <v>60</v>
@@ -1884,12 +1890,12 @@
       <c r="X44" s="22"/>
     </row>
     <row r="45" spans="1:24" s="30" customFormat="1" ht="48.75" customHeight="1">
-      <c r="A45" s="40"/>
+      <c r="A45" s="37"/>
       <c r="B45" s="15" t="s">
         <v>61</v>
       </c>
       <c r="C45" s="10" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D45" s="23" t="s">
         <v>54</v>
@@ -1916,12 +1922,12 @@
       <c r="X45" s="22"/>
     </row>
     <row r="46" spans="1:24" s="30" customFormat="1" ht="35.25" customHeight="1">
-      <c r="A46" s="40"/>
+      <c r="A46" s="37"/>
       <c r="B46" s="21" t="s">
         <v>62</v>
       </c>
       <c r="C46" s="11" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="D46" s="12" t="s">
         <v>54</v>
@@ -1948,7 +1954,7 @@
       <c r="X46" s="22"/>
     </row>
     <row r="47" spans="1:24" ht="21" customHeight="1">
-      <c r="A47" s="40"/>
+      <c r="A47" s="37"/>
       <c r="B47" s="15" t="s">
         <v>63</v>
       </c>
@@ -1960,8 +1966,8 @@
       </c>
     </row>
     <row r="48" spans="1:24" ht="45">
-      <c r="A48" s="37" t="s">
-        <v>98</v>
+      <c r="A48" s="38" t="s">
+        <v>95</v>
       </c>
       <c r="B48" s="21" t="s">
         <v>67</v>
@@ -1974,7 +1980,7 @@
       </c>
     </row>
     <row r="49" spans="1:4" ht="38.25" customHeight="1">
-      <c r="A49" s="38"/>
+      <c r="A49" s="40"/>
       <c r="B49" s="15" t="s">
         <v>68</v>
       </c>
@@ -1986,7 +1992,7 @@
       </c>
     </row>
     <row r="50" spans="1:4" ht="48.75" customHeight="1">
-      <c r="A50" s="38"/>
+      <c r="A50" s="40"/>
       <c r="B50" s="21" t="s">
         <v>69</v>
       </c>
@@ -1998,7 +2004,7 @@
       </c>
     </row>
     <row r="51" spans="1:4" ht="50.25" customHeight="1">
-      <c r="A51" s="38"/>
+      <c r="A51" s="40"/>
       <c r="B51" s="15" t="s">
         <v>70</v>
       </c>
@@ -2023,13 +2029,13 @@
     </row>
     <row r="53" spans="1:4" ht="30">
       <c r="A53" s="41" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B53" s="15" t="s">
         <v>77</v>
       </c>
       <c r="C53" s="13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D53" s="23" t="s">
         <v>50</v>
@@ -2041,7 +2047,7 @@
         <v>78</v>
       </c>
       <c r="C54" s="11" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D54" s="12" t="s">
         <v>50</v>
@@ -2053,7 +2059,7 @@
         <v>79</v>
       </c>
       <c r="C55" s="14" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="D55" s="23" t="s">
         <v>50</v>
@@ -2065,57 +2071,57 @@
         <v>80</v>
       </c>
       <c r="C56" s="14" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="D56" s="23" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="30">
       <c r="A57" s="42"/>
       <c r="B57" s="21" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="C57" s="11" t="s">
-        <v>173</v>
+        <v>179</v>
       </c>
       <c r="D57" s="12" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="45">
-      <c r="A58" s="37" t="s">
-        <v>100</v>
+    <row r="58" spans="1:4" ht="30">
+      <c r="A58" s="38" t="s">
+        <v>97</v>
       </c>
       <c r="B58" s="21" t="s">
         <v>81</v>
       </c>
       <c r="C58" s="11" t="s">
-        <v>85</v>
+        <v>176</v>
       </c>
       <c r="D58" s="12" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="59" spans="1:4" ht="30">
-      <c r="A59" s="38"/>
+    <row r="59" spans="1:4">
+      <c r="A59" s="40"/>
       <c r="B59" s="15" t="s">
         <v>82</v>
       </c>
       <c r="C59" s="10" t="s">
-        <v>87</v>
+        <v>177</v>
       </c>
       <c r="D59" s="23" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="60" spans="1:4" ht="45">
-      <c r="A60" s="38"/>
+    <row r="60" spans="1:4" ht="30">
+      <c r="A60" s="40"/>
       <c r="B60" s="21" t="s">
         <v>83</v>
       </c>
       <c r="C60" s="11" t="s">
-        <v>88</v>
+        <v>178</v>
       </c>
       <c r="D60" s="12" t="s">
         <v>50</v>
@@ -2127,7 +2133,7 @@
         <v>84</v>
       </c>
       <c r="C61" s="10" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D61" s="23" t="s">
         <v>50</v>
@@ -2135,21 +2141,21 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A11:A20"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="A26:A37"/>
-    <mergeCell ref="A2:A10"/>
-    <mergeCell ref="A53:A57"/>
     <mergeCell ref="A58:A61"/>
     <mergeCell ref="A23:A25"/>
     <mergeCell ref="A48:A52"/>
     <mergeCell ref="A41:A43"/>
     <mergeCell ref="A44:A47"/>
     <mergeCell ref="A38:A40"/>
+    <mergeCell ref="A11:A20"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="A26:A37"/>
+    <mergeCell ref="A2:A10"/>
+    <mergeCell ref="A53:A57"/>
   </mergeCells>
   <phoneticPr fontId="9" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation allowBlank="1" showDropDown="1" sqref="A21 A11 D2 D21:D40 A2 A24 A26 D54 D57:D58"/>
+    <dataValidation allowBlank="1" showDropDown="1" sqref="A21 A11 D2 D21:D40 A2 A24 A26 D54 D57:D58" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2157,11 +2163,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="111" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="111" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2300,13 +2306,13 @@
     </row>
     <row r="10" spans="1:4" ht="37.5">
       <c r="A10" s="5" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>54</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="D10" s="2">
         <v>45776</v>
@@ -2314,13 +2320,13 @@
     </row>
     <row r="11" spans="1:4" ht="37.5">
       <c r="A11" s="6" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D11" s="4">
         <v>45777</v>
@@ -2328,13 +2334,13 @@
     </row>
     <row r="12" spans="1:4" ht="56.25">
       <c r="A12" s="5" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>50</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D12" s="2">
         <v>45777</v>
@@ -2342,13 +2348,13 @@
     </row>
     <row r="13" spans="1:4" ht="37.5">
       <c r="A13" s="5" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="D13" s="2">
         <v>45777</v>
@@ -2356,13 +2362,13 @@
     </row>
     <row r="14" spans="1:4" ht="18.75">
       <c r="A14" s="5" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>54</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="D14" s="2">
         <v>45778</v>
@@ -2370,13 +2376,13 @@
     </row>
     <row r="15" spans="1:4" ht="37.5">
       <c r="A15" s="5" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="D15" s="2">
         <v>45779</v>
@@ -2384,13 +2390,13 @@
     </row>
     <row r="16" spans="1:4" ht="56.25">
       <c r="A16" s="5" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D16" s="2">
         <v>45779</v>
@@ -2398,13 +2404,13 @@
     </row>
     <row r="17" spans="1:4" ht="37.5">
       <c r="A17" s="5" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="D17" s="2">
         <v>45780</v>
@@ -2412,16 +2418,30 @@
     </row>
     <row r="18" spans="1:4" ht="56.25">
       <c r="A18" s="5" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="B18" s="36" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C18" s="36" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="D18" s="2">
         <v>45780</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="37.5">
+      <c r="A19" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="B19" s="36" t="s">
+        <v>50</v>
+      </c>
+      <c r="C19" s="36" t="s">
+        <v>181</v>
+      </c>
+      <c r="D19" s="2">
+        <v>45781</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
v3.0 Updated ADMIN HOME and PUBLISH VIDEO features according to the review
</commit_message>
<xml_diff>
--- a/LH_REQUIREMENTS/LH_CRS.xlsx
+++ b/LH_REQUIREMENTS/LH_CRS.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20417"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="6" documentId="8_{DE6D1FF1-3C9B-40C5-9432-277D1219FD8E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{3584282E-462C-498C-811A-A8066852D4C8}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6945" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6945" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="LH_CRS" sheetId="1" r:id="rId1"/>
@@ -21,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="184">
   <si>
     <t>ID</t>
   </si>
@@ -243,14 +242,6 @@
     <t>LH-CRS-PUBLISHVIDEO-004</t>
   </si>
   <si>
-    <t xml:space="preserve">he system must enforce a file size limit of 100MB for video uploads. If a user attempts to upload a file exceeding this limit, an error message must be displayed informing them of the restriction.
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The "Upload Video" button must enable users to select a video file from their device. Upon selection, the system should validate the file format and size before allowing the upload to proceed. Supported formats must be clearly stated on the page.
-</t>
-  </si>
-  <si>
     <t xml:space="preserve">The "Publish Video" button must become active only after a valid video file is uploaded and a title is entered. Clicking this button must trigger a process that stores the video securely and makes it accessible to the intended audience.
 </t>
   </si>
@@ -582,12 +573,26 @@
   </si>
   <si>
     <t>updated publish audio feature according to the review</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The system must enforce a file size limit of 100MB for video uploads. If a user attempts to upload a file exceeding this limit, an error message must be displayed informing them of the restriction.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The "Upload Video" button must enable users to select a video file from their device. Upon selection, the system should validate the file format and size before allowing the upload to proceed. Supported format must be clearly stated on the page.
+</t>
+  </si>
+  <si>
+    <t>v3.0</t>
+  </si>
+  <si>
+    <t>Updated ADMIN HOME and PUBLISH VIDEO features according to the review</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="10">
     <font>
       <sz val="11"/>
@@ -778,7 +783,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -884,9 +889,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -966,7 +968,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -1001,7 +1003,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1185,11 +1187,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X61"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" zoomScaleNormal="76" workbookViewId="0">
-      <selection activeCell="C57" sqref="C57"/>
+    <sheetView topLeftCell="A41" zoomScaleNormal="76" workbookViewId="0">
+      <selection activeCell="A44" sqref="A44:A47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -1216,21 +1218,21 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="30">
-      <c r="A2" s="38" t="s">
-        <v>88</v>
+      <c r="A2" s="37" t="s">
+        <v>86</v>
       </c>
       <c r="B2" s="21" t="s">
         <v>9</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D2" s="12" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="40"/>
+      <c r="A3" s="39"/>
       <c r="B3" s="15" t="s">
         <v>11</v>
       </c>
@@ -1242,214 +1244,214 @@
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="40"/>
+      <c r="A4" s="39"/>
       <c r="B4" s="21" t="s">
         <v>12</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D4" s="12" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="30">
-      <c r="A5" s="40"/>
+      <c r="A5" s="39"/>
       <c r="B5" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D5" s="23" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="40"/>
+      <c r="A6" s="39"/>
       <c r="B6" s="21" t="s">
         <v>14</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D6" s="12" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="30">
-      <c r="A7" s="40"/>
+      <c r="A7" s="39"/>
       <c r="B7" s="15" t="s">
         <v>15</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D7" s="23" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="45">
-      <c r="A8" s="40"/>
+      <c r="A8" s="39"/>
       <c r="B8" s="21" t="s">
         <v>35</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D8" s="12" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="30">
-      <c r="A9" s="40"/>
+      <c r="A9" s="39"/>
       <c r="B9" s="15" t="s">
         <v>37</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D9" s="23" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="30">
-      <c r="A10" s="39"/>
+      <c r="A10" s="38"/>
       <c r="B10" s="21" t="s">
         <v>38</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D10" s="12" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11" s="37" t="s">
+      <c r="A11" s="36" t="s">
+        <v>140</v>
+      </c>
+      <c r="B11" s="21" t="s">
+        <v>141</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="D11" s="33" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="36"/>
+      <c r="B12" s="25" t="s">
         <v>142</v>
       </c>
-      <c r="B11" s="21" t="s">
+      <c r="C12" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="D12" s="27" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="36"/>
+      <c r="B13" s="21" t="s">
         <v>143</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="C13" s="11" t="s">
         <v>153</v>
       </c>
-      <c r="D11" s="33" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" s="37"/>
-      <c r="B12" s="25" t="s">
+      <c r="D13" s="33" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="30">
+      <c r="A14" s="36"/>
+      <c r="B14" s="25" t="s">
         <v>144</v>
       </c>
-      <c r="C12" s="10" t="s">
+      <c r="C14" s="10" t="s">
         <v>154</v>
       </c>
-      <c r="D12" s="27" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13" s="37"/>
-      <c r="B13" s="21" t="s">
+      <c r="D14" s="27" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="36"/>
+      <c r="B15" s="21" t="s">
         <v>145</v>
       </c>
-      <c r="C13" s="11" t="s">
+      <c r="C15" s="34" t="s">
         <v>155</v>
       </c>
-      <c r="D13" s="33" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="30">
-      <c r="A14" s="37"/>
-      <c r="B14" s="25" t="s">
+      <c r="D15" s="12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="30">
+      <c r="A16" s="36"/>
+      <c r="B16" s="25" t="s">
         <v>146</v>
       </c>
-      <c r="C14" s="10" t="s">
+      <c r="C16" s="10" t="s">
         <v>156</v>
       </c>
-      <c r="D14" s="27" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15" s="37"/>
-      <c r="B15" s="21" t="s">
+      <c r="D16" s="27" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="30">
+      <c r="A17" s="36"/>
+      <c r="B17" s="21" t="s">
         <v>147</v>
       </c>
-      <c r="C15" s="34" t="s">
+      <c r="C17" s="34" t="s">
         <v>157</v>
       </c>
-      <c r="D15" s="12" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="30">
-      <c r="A16" s="37"/>
-      <c r="B16" s="25" t="s">
+      <c r="D17" s="12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="36"/>
+      <c r="B18" s="25" t="s">
         <v>148</v>
       </c>
-      <c r="C16" s="10" t="s">
+      <c r="C18" s="10" t="s">
         <v>158</v>
       </c>
-      <c r="D16" s="27" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="30">
-      <c r="A17" s="37"/>
-      <c r="B17" s="21" t="s">
+      <c r="D18" s="27" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="36"/>
+      <c r="B19" s="21" t="s">
         <v>149</v>
       </c>
-      <c r="C17" s="34" t="s">
+      <c r="C19" s="34" t="s">
         <v>159</v>
       </c>
-      <c r="D17" s="12" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18" s="37"/>
-      <c r="B18" s="25" t="s">
+      <c r="D19" s="12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="36"/>
+      <c r="B20" s="25" t="s">
         <v>150</v>
       </c>
-      <c r="C18" s="10" t="s">
+      <c r="C20" s="26" t="s">
         <v>160</v>
       </c>
-      <c r="D18" s="27" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19" s="37"/>
-      <c r="B19" s="21" t="s">
-        <v>151</v>
-      </c>
-      <c r="C19" s="34" t="s">
-        <v>161</v>
-      </c>
-      <c r="D19" s="12" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
-      <c r="A20" s="37"/>
-      <c r="B20" s="25" t="s">
-        <v>152</v>
-      </c>
-      <c r="C20" s="26" t="s">
-        <v>162</v>
-      </c>
       <c r="D20" s="27" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="21" spans="1:4">
-      <c r="A21" s="38" t="s">
-        <v>89</v>
+      <c r="A21" s="37" t="s">
+        <v>87</v>
       </c>
       <c r="B21" s="24" t="s">
         <v>26</v>
@@ -1462,7 +1464,7 @@
       </c>
     </row>
     <row r="22" spans="1:4">
-      <c r="A22" s="39"/>
+      <c r="A22" s="38"/>
       <c r="B22" s="21" t="s">
         <v>29</v>
       </c>
@@ -1474,8 +1476,8 @@
       </c>
     </row>
     <row r="23" spans="1:4">
-      <c r="A23" s="37" t="s">
-        <v>90</v>
+      <c r="A23" s="36" t="s">
+        <v>88</v>
       </c>
       <c r="B23" s="25" t="s">
         <v>27</v>
@@ -1488,7 +1490,7 @@
       </c>
     </row>
     <row r="24" spans="1:4">
-      <c r="A24" s="37" t="s">
+      <c r="A24" s="36" t="s">
         <v>4</v>
       </c>
       <c r="B24" s="21" t="s">
@@ -1502,7 +1504,7 @@
       </c>
     </row>
     <row r="25" spans="1:4">
-      <c r="A25" s="37"/>
+      <c r="A25" s="36"/>
       <c r="B25" s="15" t="s">
         <v>39</v>
       </c>
@@ -1514,154 +1516,154 @@
       </c>
     </row>
     <row r="26" spans="1:4" ht="30">
-      <c r="A26" s="38" t="s">
-        <v>91</v>
+      <c r="A26" s="37" t="s">
+        <v>89</v>
       </c>
       <c r="B26" s="21" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D26" s="12" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="27" spans="1:4">
-      <c r="A27" s="40"/>
+      <c r="A27" s="39"/>
       <c r="B27" s="28" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C27" s="26" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D27" s="29" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="28" spans="1:4">
-      <c r="A28" s="40"/>
+      <c r="A28" s="39"/>
       <c r="B28" s="21" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D28" s="12" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="29" spans="1:4">
-      <c r="A29" s="40"/>
+      <c r="A29" s="39"/>
       <c r="B29" s="28" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C29" s="26" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D29" s="29" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="15" customHeight="1">
-      <c r="A30" s="40"/>
+      <c r="A30" s="39"/>
       <c r="B30" s="21" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D30" s="12" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="15" customHeight="1">
-      <c r="A31" s="40"/>
+      <c r="A31" s="39"/>
       <c r="B31" s="21" t="s">
+        <v>113</v>
+      </c>
+      <c r="C31" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="D31" s="12" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="15" customHeight="1">
+      <c r="A32" s="39"/>
+      <c r="B32" s="21" t="s">
+        <v>114</v>
+      </c>
+      <c r="C32" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="D32" s="12" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="33" spans="1:24" ht="15" customHeight="1">
+      <c r="A33" s="39"/>
+      <c r="B33" s="21" t="s">
         <v>115</v>
       </c>
-      <c r="C31" s="11" t="s">
-        <v>136</v>
-      </c>
-      <c r="D31" s="12" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="15" customHeight="1">
-      <c r="A32" s="40"/>
-      <c r="B32" s="21" t="s">
+      <c r="C33" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="D33" s="12" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="34" spans="1:24" ht="15" customHeight="1">
+      <c r="A34" s="39"/>
+      <c r="B34" s="21" t="s">
         <v>116</v>
       </c>
-      <c r="C32" s="11" t="s">
+      <c r="C34" s="11" t="s">
         <v>120</v>
       </c>
-      <c r="D32" s="12" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="33" spans="1:24" ht="15" customHeight="1">
-      <c r="A33" s="40"/>
-      <c r="B33" s="21" t="s">
+      <c r="D34" s="12" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="35" spans="1:24" ht="15" customHeight="1">
+      <c r="A35" s="39"/>
+      <c r="B35" s="21" t="s">
         <v>117</v>
       </c>
-      <c r="C33" s="11" t="s">
+      <c r="C35" s="11" t="s">
         <v>121</v>
       </c>
-      <c r="D33" s="12" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="34" spans="1:24" ht="15" customHeight="1">
-      <c r="A34" s="40"/>
-      <c r="B34" s="21" t="s">
-        <v>118</v>
-      </c>
-      <c r="C34" s="11" t="s">
+      <c r="D35" s="12" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="36" spans="1:24" ht="15" customHeight="1">
+      <c r="A36" s="39"/>
+      <c r="B36" s="21" t="s">
         <v>122</v>
       </c>
-      <c r="D34" s="12" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="35" spans="1:24" ht="15" customHeight="1">
-      <c r="A35" s="40"/>
-      <c r="B35" s="21" t="s">
-        <v>119</v>
-      </c>
-      <c r="C35" s="11" t="s">
+      <c r="C36" s="11" t="s">
         <v>123</v>
       </c>
-      <c r="D35" s="12" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="36" spans="1:24" ht="15" customHeight="1">
-      <c r="A36" s="40"/>
-      <c r="B36" s="21" t="s">
+      <c r="D36" s="12" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="37" spans="1:24" ht="15" customHeight="1">
+      <c r="A37" s="39"/>
+      <c r="B37" s="21" t="s">
         <v>124</v>
       </c>
-      <c r="C36" s="11" t="s">
+      <c r="C37" s="11" t="s">
         <v>125</v>
       </c>
-      <c r="D36" s="12" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="37" spans="1:24" ht="15" customHeight="1">
-      <c r="A37" s="40"/>
-      <c r="B37" s="21" t="s">
-        <v>126</v>
-      </c>
-      <c r="C37" s="11" t="s">
-        <v>127</v>
-      </c>
       <c r="D37" s="12" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="38" spans="1:24" s="30" customFormat="1" ht="45">
-      <c r="A38" s="37" t="s">
-        <v>92</v>
+      <c r="A38" s="36" t="s">
+        <v>90</v>
       </c>
       <c r="B38" s="21" t="s">
         <v>30</v>
@@ -1694,7 +1696,7 @@
       <c r="X38" s="22"/>
     </row>
     <row r="39" spans="1:24" s="31" customFormat="1" ht="45">
-      <c r="A39" s="37"/>
+      <c r="A39" s="36"/>
       <c r="B39" s="25" t="s">
         <v>31</v>
       </c>
@@ -1726,7 +1728,7 @@
       <c r="X39" s="22"/>
     </row>
     <row r="40" spans="1:24" s="30" customFormat="1" ht="30">
-      <c r="A40" s="37"/>
+      <c r="A40" s="36"/>
       <c r="B40" s="21" t="s">
         <v>32</v>
       </c>
@@ -1758,8 +1760,8 @@
       <c r="X40" s="22"/>
     </row>
     <row r="41" spans="1:24" s="30" customFormat="1" ht="78.75" customHeight="1">
-      <c r="A41" s="38" t="s">
-        <v>93</v>
+      <c r="A41" s="37" t="s">
+        <v>91</v>
       </c>
       <c r="B41" s="15" t="s">
         <v>55</v>
@@ -1792,7 +1794,7 @@
       <c r="X41" s="22"/>
     </row>
     <row r="42" spans="1:24" s="31" customFormat="1" ht="34.5" customHeight="1">
-      <c r="A42" s="40"/>
+      <c r="A42" s="39"/>
       <c r="B42" s="21" t="s">
         <v>57</v>
       </c>
@@ -1824,7 +1826,7 @@
       <c r="X42" s="22"/>
     </row>
     <row r="43" spans="1:24" s="30" customFormat="1" ht="34.5" customHeight="1">
-      <c r="A43" s="39"/>
+      <c r="A43" s="38"/>
       <c r="B43" s="15" t="s">
         <v>58</v>
       </c>
@@ -1856,8 +1858,8 @@
       <c r="X43" s="22"/>
     </row>
     <row r="44" spans="1:24" s="31" customFormat="1" ht="45" customHeight="1">
-      <c r="A44" s="37" t="s">
-        <v>94</v>
+      <c r="A44" s="36" t="s">
+        <v>92</v>
       </c>
       <c r="B44" s="21" t="s">
         <v>60</v>
@@ -1890,12 +1892,12 @@
       <c r="X44" s="22"/>
     </row>
     <row r="45" spans="1:24" s="30" customFormat="1" ht="48.75" customHeight="1">
-      <c r="A45" s="37"/>
+      <c r="A45" s="36"/>
       <c r="B45" s="15" t="s">
         <v>61</v>
       </c>
       <c r="C45" s="10" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D45" s="23" t="s">
         <v>54</v>
@@ -1922,12 +1924,12 @@
       <c r="X45" s="22"/>
     </row>
     <row r="46" spans="1:24" s="30" customFormat="1" ht="35.25" customHeight="1">
-      <c r="A46" s="37"/>
+      <c r="A46" s="36"/>
       <c r="B46" s="21" t="s">
         <v>62</v>
       </c>
       <c r="C46" s="11" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D46" s="12" t="s">
         <v>54</v>
@@ -1954,7 +1956,7 @@
       <c r="X46" s="22"/>
     </row>
     <row r="47" spans="1:24" ht="21" customHeight="1">
-      <c r="A47" s="37"/>
+      <c r="A47" s="36"/>
       <c r="B47" s="15" t="s">
         <v>63</v>
       </c>
@@ -1966,174 +1968,174 @@
       </c>
     </row>
     <row r="48" spans="1:24" ht="45">
-      <c r="A48" s="38" t="s">
-        <v>95</v>
+      <c r="A48" s="37" t="s">
+        <v>93</v>
       </c>
       <c r="B48" s="21" t="s">
         <v>67</v>
       </c>
       <c r="C48" s="11" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D48" s="12" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="38.25" customHeight="1">
-      <c r="A49" s="40"/>
+      <c r="A49" s="39"/>
       <c r="B49" s="15" t="s">
         <v>68</v>
       </c>
       <c r="C49" s="10" t="s">
-        <v>71</v>
+        <v>180</v>
       </c>
       <c r="D49" s="23" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="48.75" customHeight="1">
-      <c r="A50" s="40"/>
+      <c r="A50" s="39"/>
       <c r="B50" s="21" t="s">
         <v>69</v>
       </c>
       <c r="C50" s="11" t="s">
-        <v>72</v>
+        <v>181</v>
       </c>
       <c r="D50" s="12" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="50.25" customHeight="1">
-      <c r="A51" s="40"/>
+      <c r="A51" s="39"/>
       <c r="B51" s="15" t="s">
         <v>70</v>
       </c>
       <c r="C51" s="10" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D51" s="23" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="36" customHeight="1">
-      <c r="A52" s="39"/>
+      <c r="A52" s="38"/>
       <c r="B52" s="21" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C52" s="11" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D52" s="12" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="30">
-      <c r="A53" s="41" t="s">
-        <v>96</v>
+      <c r="A53" s="40" t="s">
+        <v>94</v>
       </c>
       <c r="B53" s="15" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C53" s="13" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D53" s="23" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="30">
-      <c r="A54" s="42"/>
+      <c r="A54" s="41"/>
       <c r="B54" s="21" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C54" s="11" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D54" s="12" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="55" spans="1:4">
-      <c r="A55" s="42"/>
+      <c r="A55" s="41"/>
       <c r="B55" s="15" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C55" s="14" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D55" s="23" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="56" spans="1:4">
-      <c r="A56" s="42"/>
+      <c r="A56" s="41"/>
       <c r="B56" s="15" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C56" s="14" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D56" s="23" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="30">
-      <c r="A57" s="42"/>
+      <c r="A57" s="41"/>
       <c r="B57" s="21" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C57" s="11" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D57" s="12" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="30">
-      <c r="A58" s="38" t="s">
-        <v>97</v>
+      <c r="A58" s="37" t="s">
+        <v>95</v>
       </c>
       <c r="B58" s="21" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C58" s="11" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D58" s="12" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="59" spans="1:4">
-      <c r="A59" s="40"/>
+      <c r="A59" s="39"/>
       <c r="B59" s="15" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C59" s="10" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D59" s="23" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="30">
-      <c r="A60" s="40"/>
+      <c r="A60" s="39"/>
       <c r="B60" s="21" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C60" s="11" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D60" s="12" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="34.5" customHeight="1">
-      <c r="A61" s="39"/>
+      <c r="A61" s="38"/>
       <c r="B61" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="C61" s="10" t="s">
         <v>84</v>
-      </c>
-      <c r="C61" s="10" t="s">
-        <v>86</v>
       </c>
       <c r="D61" s="23" t="s">
         <v>50</v>
@@ -2155,7 +2157,7 @@
   </mergeCells>
   <phoneticPr fontId="9" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation allowBlank="1" showDropDown="1" sqref="A21 A11 D2 D21:D40 A2 A24 A26 D54 D57:D58" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
+    <dataValidation allowBlank="1" showDropDown="1" sqref="A21 A11 D2 D21:D40 A2 A24 A26 D54 D57:D58"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2163,11 +2165,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="111" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="111" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2306,13 +2308,13 @@
     </row>
     <row r="10" spans="1:4" ht="37.5">
       <c r="A10" s="5" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>54</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D10" s="2">
         <v>45776</v>
@@ -2320,13 +2322,13 @@
     </row>
     <row r="11" spans="1:4" ht="37.5">
       <c r="A11" s="6" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D11" s="4">
         <v>45777</v>
@@ -2334,13 +2336,13 @@
     </row>
     <row r="12" spans="1:4" ht="56.25">
       <c r="A12" s="5" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>50</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D12" s="2">
         <v>45777</v>
@@ -2348,13 +2350,13 @@
     </row>
     <row r="13" spans="1:4" ht="37.5">
       <c r="A13" s="5" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D13" s="2">
         <v>45777</v>
@@ -2362,13 +2364,13 @@
     </row>
     <row r="14" spans="1:4" ht="18.75">
       <c r="A14" s="5" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>54</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D14" s="2">
         <v>45778</v>
@@ -2376,13 +2378,13 @@
     </row>
     <row r="15" spans="1:4" ht="37.5">
       <c r="A15" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>132</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>134</v>
       </c>
       <c r="D15" s="2">
         <v>45779</v>
@@ -2390,13 +2392,13 @@
     </row>
     <row r="16" spans="1:4" ht="56.25">
       <c r="A16" s="5" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D16" s="2">
         <v>45779</v>
@@ -2404,27 +2406,27 @@
     </row>
     <row r="17" spans="1:4" ht="37.5">
       <c r="A17" s="5" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D17" s="2">
         <v>45780</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="56.25">
+    <row r="18" spans="1:4" ht="75">
       <c r="A18" s="5" t="s">
-        <v>170</v>
-      </c>
-      <c r="B18" s="36" t="s">
-        <v>133</v>
-      </c>
-      <c r="C18" s="36" t="s">
-        <v>175</v>
+        <v>168</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>173</v>
       </c>
       <c r="D18" s="2">
         <v>45780</v>
@@ -2432,15 +2434,29 @@
     </row>
     <row r="19" spans="1:4" ht="37.5">
       <c r="A19" s="5" t="s">
-        <v>180</v>
-      </c>
-      <c r="B19" s="36" t="s">
+        <v>178</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C19" s="36" t="s">
-        <v>181</v>
+      <c r="C19" s="1" t="s">
+        <v>179</v>
       </c>
       <c r="D19" s="2">
+        <v>45781</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="37.5">
+      <c r="A20" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="D20" s="2">
         <v>45781</v>
       </c>
     </row>

</xml_diff>

<commit_message>
v3.2 edited a mistake
</commit_message>
<xml_diff>
--- a/LH_REQUIREMENTS/LH_CRS.xlsx
+++ b/LH_REQUIREMENTS/LH_CRS.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="186">
   <si>
     <t>Feature</t>
   </si>
@@ -114,31 +114,31 @@
     <t xml:space="preserve">LH-CRS-CATEGORIES-002	</t>
   </si>
   <si>
-    <t xml:space="preserve">	The page must include a dropdown list of available categories (e.g., “Category 1”, “Category 2”).</t>
+    <t>The page must include a dropdown list of available categories (e.g., “Category 1”, “Category 2”).</t>
   </si>
   <si>
     <t xml:space="preserve">LH-CRS-CATEGORIES-003	</t>
   </si>
   <si>
-    <t xml:space="preserve">	Users must be able to select a category from the dropdown list.</t>
+    <t>Users must be able to select a category from the dropdown list.</t>
   </si>
   <si>
     <t xml:space="preserve">LH-CRS-CATEGORIES-004	</t>
   </si>
   <si>
-    <t xml:space="preserve">	Upon category selection, the system must dynamically display a list of posts associated with the selected category in the same page view.</t>
+    <t>Upon category selection, the system must dynamically display a list of posts associated with the selected category in the same page view.</t>
   </si>
   <si>
     <t xml:space="preserve">LH-CRS-CATEGORIES-005	</t>
   </si>
   <si>
-    <t xml:space="preserve">	Each displayed post must show its title and content snippet (e.g., “Post 1: Title – Content…”).</t>
+    <t>Each displayed post must show its title and content snippet (e.g., “Post 1: Title – Content…”).</t>
   </si>
   <si>
     <t xml:space="preserve">LH-CRS-CATEGORIES-006	</t>
   </si>
   <si>
-    <t xml:space="preserve">	A “Follow” button must be provided next to the category dropdown to allow the user to follow the selected category.</t>
+    <t>A “Follow” button must be provided next to the category dropdown to allow the user to follow the selected category.</t>
   </si>
   <si>
     <t xml:space="preserve">LH-CRS-CATEGORIES-007	</t>
@@ -150,7 +150,7 @@
     <t xml:space="preserve">LH-CRS-CATEGORIES-008	</t>
   </si>
   <si>
-    <t>The bottom of the page must include a second dropdown list for publishing options.</t>
+    <t>The page must include a second dropdown list for publishing options.</t>
   </si>
   <si>
     <t xml:space="preserve">LH-CRS-CATEGORIES-009	</t>
@@ -595,6 +595,12 @@
   </si>
   <si>
     <t>Removed out of scope CRS</t>
+  </si>
+  <si>
+    <t>v3.2</t>
+  </si>
+  <si>
+    <t>Edited a small mistake in Categories feature</t>
   </si>
 </sst>
 </file>
@@ -607,7 +613,7 @@
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="29">
+  <fonts count="28">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -671,13 +677,6 @@
       <color theme="0"/>
       <name val="Roboto"/>
       <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <u/>
@@ -824,7 +823,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="41">
+  <fills count="39">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -929,12 +928,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -1020,12 +1013,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1227,133 +1214,139 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="176" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="12" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="13" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1362,13 +1355,7 @@
     <xf numFmtId="0" fontId="27" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1815,8 +1802,8 @@
   <sheetPr/>
   <dimension ref="A1:X60"/>
   <sheetViews>
-    <sheetView topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38:A39"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85714285714286" defaultRowHeight="15"/>
@@ -2749,10 +2736,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="111" zoomScaleNormal="111" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" zoomScale="111" zoomScaleNormal="111" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="3"/>
@@ -3057,6 +3044,20 @@
         <v>45792</v>
       </c>
     </row>
+    <row r="22" ht="18.75" spans="1:4">
+      <c r="A22" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="D22" s="6">
+        <v>45792</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="1" orientation="portrait"/>

</xml_diff>

<commit_message>
v3.3 Updated the CRS according to change request
</commit_message>
<xml_diff>
--- a/LH_REQUIREMENTS/LH_CRS.xlsx
+++ b/LH_REQUIREMENTS/LH_CRS.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="7620" activeTab="1"/>
+    <workbookView windowWidth="20490" windowHeight="7620"/>
   </bookViews>
   <sheets>
     <sheet name="LH_CRS" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="192">
   <si>
     <t>Feature</t>
   </si>
@@ -369,32 +369,38 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">The system must allow users to upload a video file through the "Upload Video" button. Supported formats must include .mp4 only accoring to siq , with a maximum file size of 5MB:100MB. 
+    <t xml:space="preserve">The system must allow users to upload a video file through the "Upload Video" button. Supported formats must include .mp4 only accoring to SIQ , with a maximum file size of 100MB. 
 </t>
   </si>
   <si>
     <t>LH-CRS-PUBLISHVIDEO-002</t>
+  </si>
+  <si>
+    <t>The Title may contain alphanumeric values or special characters, with a maximum length of 40 characters. If the title exceeds the maximum length, the system should display an error message.</t>
+  </si>
+  <si>
+    <t>LH-CRS-PUBLISHVIDEO-003</t>
   </si>
   <si>
     <t xml:space="preserve">The system must enforce a file size limit of 100MB for video uploads. If a user attempts to upload a file exceeding this limit, an error message must be displayed informing them of the restriction.
 </t>
   </si>
   <si>
-    <t>LH-CRS-PUBLISHVIDEO-003</t>
+    <t>LH-CRS-PUBLISHVIDEO-004</t>
   </si>
   <si>
     <t xml:space="preserve">The "Upload Video" button must enable users to select a video file from their device. Upon selection, the system should validate the file format and size before allowing the upload to proceed. Supported format must be clearly stated on the page.
 </t>
   </si>
   <si>
-    <t>LH-CRS-PUBLISHVIDEO-004</t>
+    <t>LH-CRS-PUBLISHVIDEO-005</t>
   </si>
   <si>
     <t xml:space="preserve">The "Publish Video" button must become active only after a valid video file is uploaded and a title is entered. Clicking this button must trigger a process that stores the video securely and makes it accessible to the intended audience.
 </t>
   </si>
   <si>
-    <t>LH-CRS-PUBLISHVIDEO-005</t>
+    <t>LH-CRS-PUBLISHVIDEO-006</t>
   </si>
   <si>
     <t xml:space="preserve">If the user attempts to publish without entering a title or uploading a valid video file, an appropriate error message must be displayed, guiding them to complete the required steps.
@@ -425,10 +431,13 @@
     <t>LH-CRS-PUBLISHARTICLE-004</t>
   </si>
   <si>
+    <t>LH-CRS-PUBLISHARTICLE-005</t>
+  </si>
+  <si>
     <t>If the article title empty ,error message must be displayed</t>
   </si>
   <si>
-    <t>LH-CRS-PUBLISHARTICLE-005</t>
+    <t>LH-CRS-PUBLISHARTICLE-006</t>
   </si>
   <si>
     <t xml:space="preserve">If the word count exceeds 1,000, an error message must be displayed.
@@ -453,10 +462,13 @@
     <t>LH-CRS-PUBLISHAUDIO-003</t>
   </si>
   <si>
+    <t>LH-CRS-PUBLISHAUDIO-004</t>
+  </si>
+  <si>
     <t>The user can record a voice message for up to 5 minutes. If the time limit is exceeded,a message will appear explaining this.</t>
   </si>
   <si>
-    <t>LH-CRS-PUBLISHAUDIO-004</t>
+    <t>LH-CRS-PUBLISHAUDIO-005</t>
   </si>
   <si>
     <t>The "Publish" button must remain disabled until the user records an audio clip and provides a title. It must only become active when both the audio duration is within the allowed limit and the title input is not empty.</t>
@@ -601,6 +613,12 @@
   </si>
   <si>
     <t>Edited a small mistake in Categories feature</t>
+  </si>
+  <si>
+    <t>v3.3</t>
+  </si>
+  <si>
+    <t>Added CRS to match the change request</t>
   </si>
 </sst>
 </file>
@@ -1359,7 +1377,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1468,6 +1486,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1800,10 +1821,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:X60"/>
+  <dimension ref="A1:X63"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="E61" sqref="E61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85714285714286" defaultRowHeight="15"/>
@@ -2551,7 +2572,7 @@
       </c>
     </row>
     <row r="48" ht="38.25" customHeight="1" spans="1:4">
-      <c r="A48" s="24"/>
+      <c r="A48" s="37"/>
       <c r="B48" s="25" t="s">
         <v>111</v>
       </c>
@@ -2559,154 +2580,190 @@
         <v>112</v>
       </c>
       <c r="D48" s="16" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="49" ht="38.25" customHeight="1" spans="1:4">
+      <c r="A49" s="24"/>
+      <c r="B49" s="25" t="s">
+        <v>113</v>
+      </c>
+      <c r="C49" s="26" t="s">
+        <v>114</v>
+      </c>
+      <c r="D49" s="16" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="49" ht="48.75" customHeight="1" spans="1:4">
-      <c r="A49" s="24"/>
-      <c r="B49" s="21" t="s">
-        <v>113</v>
-      </c>
-      <c r="C49" s="22" t="s">
-        <v>114</v>
-      </c>
-      <c r="D49" s="23" t="s">
+    <row r="50" ht="48.75" customHeight="1" spans="1:4">
+      <c r="A50" s="24"/>
+      <c r="B50" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="C50" s="22" t="s">
+        <v>116</v>
+      </c>
+      <c r="D50" s="23" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="50" ht="50.25" customHeight="1" spans="1:4">
-      <c r="A50" s="24"/>
-      <c r="B50" s="25" t="s">
-        <v>115</v>
-      </c>
-      <c r="C50" s="26" t="s">
-        <v>116</v>
-      </c>
-      <c r="D50" s="16" t="s">
+    <row r="51" ht="50.25" customHeight="1" spans="1:4">
+      <c r="A51" s="24"/>
+      <c r="B51" s="25" t="s">
+        <v>117</v>
+      </c>
+      <c r="C51" s="26" t="s">
+        <v>118</v>
+      </c>
+      <c r="D51" s="16" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="51" ht="36" customHeight="1" spans="1:4">
-      <c r="A51" s="27"/>
-      <c r="B51" s="21" t="s">
-        <v>117</v>
-      </c>
-      <c r="C51" s="22" t="s">
-        <v>118</v>
-      </c>
-      <c r="D51" s="23" t="s">
+    <row r="52" ht="36" customHeight="1" spans="1:4">
+      <c r="A52" s="27"/>
+      <c r="B52" s="21" t="s">
+        <v>119</v>
+      </c>
+      <c r="C52" s="22" t="s">
+        <v>120</v>
+      </c>
+      <c r="D52" s="23" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="52" ht="30" spans="1:4">
-      <c r="A52" s="37" t="s">
-        <v>119</v>
-      </c>
-      <c r="B52" s="25" t="s">
-        <v>120</v>
-      </c>
-      <c r="C52" s="38" t="s">
+    <row r="53" ht="30" spans="1:4">
+      <c r="A53" s="38" t="s">
         <v>121</v>
       </c>
-      <c r="D52" s="16" t="s">
+      <c r="B53" s="25" t="s">
+        <v>122</v>
+      </c>
+      <c r="C53" s="39" t="s">
+        <v>123</v>
+      </c>
+      <c r="D53" s="16" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="53" ht="30" spans="1:4">
-      <c r="A53" s="39"/>
-      <c r="B53" s="21" t="s">
-        <v>122</v>
-      </c>
-      <c r="C53" s="22" t="s">
-        <v>123</v>
-      </c>
-      <c r="D53" s="23" t="s">
+    <row r="54" ht="30" spans="1:4">
+      <c r="A54" s="40"/>
+      <c r="B54" s="21" t="s">
+        <v>124</v>
+      </c>
+      <c r="C54" s="22" t="s">
+        <v>125</v>
+      </c>
+      <c r="D54" s="23" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="54" spans="1:4">
-      <c r="A54" s="39"/>
-      <c r="B54" s="25" t="s">
-        <v>124</v>
-      </c>
-      <c r="C54" s="40" t="s">
-        <v>125</v>
-      </c>
-      <c r="D54" s="16" t="s">
-        <v>88</v>
-      </c>
-    </row>
     <row r="55" spans="1:4">
-      <c r="A55" s="39"/>
+      <c r="A55" s="40"/>
       <c r="B55" s="25" t="s">
         <v>126</v>
       </c>
-      <c r="C55" s="40" t="s">
+      <c r="C55" s="41" t="s">
         <v>127</v>
       </c>
       <c r="D55" s="16" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="56" ht="30" spans="1:4">
+      <c r="A56" s="40"/>
+      <c r="B56" s="25" t="s">
+        <v>128</v>
+      </c>
+      <c r="C56" s="26" t="s">
+        <v>112</v>
+      </c>
+      <c r="D56" s="16" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4">
+      <c r="A57" s="40"/>
+      <c r="B57" s="25" t="s">
+        <v>129</v>
+      </c>
+      <c r="C57" s="41" t="s">
+        <v>130</v>
+      </c>
+      <c r="D57" s="16" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="56" ht="30" spans="1:4">
-      <c r="A56" s="39"/>
-      <c r="B56" s="21" t="s">
-        <v>128</v>
-      </c>
-      <c r="C56" s="22" t="s">
-        <v>129</v>
-      </c>
-      <c r="D56" s="23" t="s">
+    <row r="58" ht="30" spans="1:4">
+      <c r="A58" s="40"/>
+      <c r="B58" s="21" t="s">
+        <v>131</v>
+      </c>
+      <c r="C58" s="22" t="s">
+        <v>132</v>
+      </c>
+      <c r="D58" s="23" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="57" ht="30" spans="1:4">
-      <c r="A57" s="20" t="s">
-        <v>130</v>
-      </c>
-      <c r="B57" s="21" t="s">
-        <v>131</v>
-      </c>
-      <c r="C57" s="22" t="s">
-        <v>132</v>
-      </c>
-      <c r="D57" s="23" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4">
-      <c r="A58" s="24"/>
-      <c r="B58" s="25" t="s">
+    <row r="59" ht="30" spans="1:4">
+      <c r="A59" s="20" t="s">
         <v>133</v>
       </c>
-      <c r="C58" s="26" t="s">
+      <c r="B59" s="21" t="s">
         <v>134</v>
       </c>
-      <c r="D58" s="16" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="59" ht="30" spans="1:4">
-      <c r="A59" s="24"/>
-      <c r="B59" s="21" t="s">
+      <c r="C59" s="22" t="s">
         <v>135</v>
-      </c>
-      <c r="C59" s="22" t="s">
-        <v>136</v>
       </c>
       <c r="D59" s="23" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="60" ht="34.5" customHeight="1" spans="1:4">
-      <c r="A60" s="27"/>
+    <row r="60" spans="1:4">
+      <c r="A60" s="24"/>
       <c r="B60" s="25" t="s">
+        <v>136</v>
+      </c>
+      <c r="C60" s="26" t="s">
         <v>137</v>
       </c>
-      <c r="C60" s="26" t="s">
+      <c r="D60" s="16" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="61" ht="30" spans="1:4">
+      <c r="A61" s="24"/>
+      <c r="B61" s="25" t="s">
         <v>138</v>
       </c>
-      <c r="D60" s="16" t="s">
+      <c r="C61" s="26" t="s">
+        <v>112</v>
+      </c>
+      <c r="D61" s="16" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="62" ht="30" spans="1:4">
+      <c r="A62" s="24"/>
+      <c r="B62" s="21" t="s">
+        <v>139</v>
+      </c>
+      <c r="C62" s="22" t="s">
+        <v>140</v>
+      </c>
+      <c r="D62" s="23" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="63" ht="34.5" customHeight="1" spans="1:4">
+      <c r="A63" s="27"/>
+      <c r="B63" s="25" t="s">
+        <v>141</v>
+      </c>
+      <c r="C63" s="26" t="s">
+        <v>142</v>
+      </c>
+      <c r="D63" s="16" t="s">
         <v>88</v>
       </c>
     </row>
@@ -2720,12 +2777,12 @@
     <mergeCell ref="A38:A39"/>
     <mergeCell ref="A40:A42"/>
     <mergeCell ref="A43:A46"/>
-    <mergeCell ref="A47:A51"/>
-    <mergeCell ref="A52:A56"/>
-    <mergeCell ref="A57:A60"/>
+    <mergeCell ref="A47:A52"/>
+    <mergeCell ref="A53:A58"/>
+    <mergeCell ref="A59:A63"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation allowBlank="1" sqref="A2 D2 A11 A21 A24 A26 D53 D21:D39 D56:D57"/>
+    <dataValidation allowBlank="1" sqref="A2 D2 A11 A21 A24 A26 D54 D21:D39 D58:D59"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="1" orientation="portrait"/>
@@ -2736,10 +2793,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="111" zoomScaleNormal="111" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView zoomScale="111" zoomScaleNormal="111" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="3"/>
@@ -2752,27 +2809,27 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" ht="40.5" spans="1:4">
       <c r="A1" s="2" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
     </row>
     <row r="2" ht="37.5" spans="1:4">
       <c r="A2" s="4" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>58</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="D2" s="6">
         <v>45754</v>
@@ -2780,13 +2837,13 @@
     </row>
     <row r="3" ht="37.5" spans="1:4">
       <c r="A3" s="7" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>7</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="D3" s="9">
         <v>45754</v>
@@ -2794,13 +2851,13 @@
     </row>
     <row r="4" ht="37.5" spans="1:4">
       <c r="A4" s="4" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>58</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="D4" s="6">
         <v>45759</v>
@@ -2808,13 +2865,13 @@
     </row>
     <row r="5" ht="37.5" spans="1:4">
       <c r="A5" s="7" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="B5" s="8" t="s">
         <v>7</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="D5" s="9">
         <v>45759</v>
@@ -2822,13 +2879,13 @@
     </row>
     <row r="6" ht="37.5" spans="1:4">
       <c r="A6" s="4" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>58</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="D6" s="6">
         <v>45765</v>
@@ -2836,13 +2893,13 @@
     </row>
     <row r="7" ht="18.75" spans="1:4">
       <c r="A7" s="7" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>58</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="D7" s="9">
         <v>45766</v>
@@ -2850,13 +2907,13 @@
     </row>
     <row r="8" ht="18.75" spans="1:4">
       <c r="A8" s="4" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>7</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="D8" s="6">
         <v>45768</v>
@@ -2864,13 +2921,13 @@
     </row>
     <row r="9" ht="18.75" spans="1:4">
       <c r="A9" s="7" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="B9" s="8" t="s">
         <v>88</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="D9" s="9">
         <v>45776</v>
@@ -2878,13 +2935,13 @@
     </row>
     <row r="10" ht="37.5" spans="1:4">
       <c r="A10" s="4" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>94</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="D10" s="6">
         <v>45776</v>
@@ -2892,13 +2949,13 @@
     </row>
     <row r="11" ht="37.5" spans="1:4">
       <c r="A11" s="7" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="B11" s="8" t="s">
         <v>58</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="D11" s="9">
         <v>45777</v>
@@ -2906,13 +2963,13 @@
     </row>
     <row r="12" ht="37.5" spans="1:4">
       <c r="A12" s="4" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>88</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="D12" s="6">
         <v>45777</v>
@@ -2920,13 +2977,13 @@
     </row>
     <row r="13" ht="37.5" spans="1:4">
       <c r="A13" s="4" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>58</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="D13" s="6">
         <v>45777</v>
@@ -2934,13 +2991,13 @@
     </row>
     <row r="14" ht="18.75" spans="1:4">
       <c r="A14" s="4" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>94</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="D14" s="6">
         <v>45778</v>
@@ -2948,13 +3005,13 @@
     </row>
     <row r="15" ht="37.5" spans="1:4">
       <c r="A15" s="4" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="D15" s="6">
         <v>45779</v>
@@ -2962,13 +3019,13 @@
     </row>
     <row r="16" ht="56.25" spans="1:4">
       <c r="A16" s="4" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>7</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="D16" s="6">
         <v>45779</v>
@@ -2976,13 +3033,13 @@
     </row>
     <row r="17" ht="37.5" spans="1:4">
       <c r="A17" s="4" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>7</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="D17" s="6">
         <v>45780</v>
@@ -2990,13 +3047,13 @@
     </row>
     <row r="18" ht="56.25" spans="1:4">
       <c r="A18" s="4" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="D18" s="6">
         <v>45780</v>
@@ -3004,13 +3061,13 @@
     </row>
     <row r="19" ht="37.5" spans="1:4">
       <c r="A19" s="4" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>88</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="D19" s="6">
         <v>45781</v>
@@ -3018,13 +3075,13 @@
     </row>
     <row r="20" ht="37.5" spans="1:4">
       <c r="A20" s="4" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>94</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="D20" s="6">
         <v>45781</v>
@@ -3032,13 +3089,13 @@
     </row>
     <row r="21" ht="18.75" spans="1:4">
       <c r="A21" s="4" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="B21" s="5" t="s">
         <v>88</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="D21" s="6">
         <v>45792</v>
@@ -3046,16 +3103,30 @@
     </row>
     <row r="22" ht="18.75" spans="1:4">
       <c r="A22" s="4" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>88</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="D22" s="6">
         <v>45792</v>
+      </c>
+    </row>
+    <row r="23" ht="18.75" spans="1:4">
+      <c r="A23" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="D23" s="6">
+        <v>45794</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
v3.4 edited the naming convention
</commit_message>
<xml_diff>
--- a/LH_REQUIREMENTS/LH_CRS.xlsx
+++ b/LH_REQUIREMENTS/LH_CRS.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="7620"/>
+    <workbookView windowWidth="20490" windowHeight="7620" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="LH_CRS" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="194">
   <si>
     <t>Feature</t>
   </si>
@@ -373,40 +373,52 @@
 </t>
   </si>
   <si>
-    <t>LH-CRS-PUBLISHVIDEO-002</t>
-  </si>
-  <si>
-    <t>The Title may contain alphanumeric values or special characters, with a maximum length of 40 characters. If the title exceeds the maximum length, the system should display an error message.</t>
-  </si>
-  <si>
-    <t>LH-CRS-PUBLISHVIDEO-003</t>
+    <r>
+      <t>LH-CRS-PUBLISHVIDEO-00</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">The system must enforce a file size limit of 100MB for video uploads. If a user attempts to upload a file exceeding this limit, an error message must be displayed informing them of the restriction.
 </t>
   </si>
   <si>
-    <t>LH-CRS-PUBLISHVIDEO-004</t>
+    <t>LH-CRS-PUBLISHVIDEO-003</t>
   </si>
   <si>
     <t xml:space="preserve">The "Upload Video" button must enable users to select a video file from their device. Upon selection, the system should validate the file format and size before allowing the upload to proceed. Supported format must be clearly stated on the page.
 </t>
   </si>
   <si>
-    <t>LH-CRS-PUBLISHVIDEO-005</t>
+    <t>LH-CRS-PUBLISHVIDEO-004</t>
   </si>
   <si>
     <t xml:space="preserve">The "Publish Video" button must become active only after a valid video file is uploaded and a title is entered. Clicking this button must trigger a process that stores the video securely and makes it accessible to the intended audience.
 </t>
   </si>
   <si>
-    <t>LH-CRS-PUBLISHVIDEO-006</t>
+    <t>LH-CRS-PUBLISHVIDEO-005</t>
   </si>
   <si>
     <t xml:space="preserve">If the user attempts to publish without entering a title or uploading a valid video file, an appropriate error message must be displayed, guiding them to complete the required steps.
 </t>
   </si>
   <si>
+    <t>LH-CRS-PUBLISHVIDEO-006</t>
+  </si>
+  <si>
+    <t>The Title may contain alphanumeric values or special characters, with a maximum length of 40 characters. If the title exceeds the maximum length, the system should display an error message.</t>
+  </si>
+  <si>
     <t>PUBLISH ARTICLE</t>
   </si>
   <si>
@@ -431,19 +443,19 @@
     <t>LH-CRS-PUBLISHARTICLE-004</t>
   </si>
   <si>
+    <t>If the article title empty ,error message must be displayed</t>
+  </si>
+  <si>
     <t>LH-CRS-PUBLISHARTICLE-005</t>
-  </si>
-  <si>
-    <t>If the article title empty ,error message must be displayed</t>
-  </si>
-  <si>
-    <t>LH-CRS-PUBLISHARTICLE-006</t>
   </si>
   <si>
     <t xml:space="preserve">If the word count exceeds 1,000, an error message must be displayed.
 </t>
   </si>
   <si>
+    <t>LH-CRS-PUBLISHARTICLE-006</t>
+  </si>
+  <si>
     <t>PUBLISH AUDIO</t>
   </si>
   <si>
@@ -462,18 +474,18 @@
     <t>LH-CRS-PUBLISHAUDIO-003</t>
   </si>
   <si>
+    <t>The user can record a voice message for up to 5 minutes. If the time limit is exceeded,a message will appear explaining this.</t>
+  </si>
+  <si>
     <t>LH-CRS-PUBLISHAUDIO-004</t>
   </si>
   <si>
-    <t>The user can record a voice message for up to 5 minutes. If the time limit is exceeded,a message will appear explaining this.</t>
+    <t>The "Publish" button must remain disabled until the user records an audio clip and provides a title. It must only become active when both the audio duration is within the allowed limit and the title input is not empty.</t>
   </si>
   <si>
     <t>LH-CRS-PUBLISHAUDIO-005</t>
   </si>
   <si>
-    <t>The "Publish" button must remain disabled until the user records an audio clip and provides a title. It must only become active when both the audio duration is within the allowed limit and the title input is not empty.</t>
-  </si>
-  <si>
     <t>Version number</t>
   </si>
   <si>
@@ -619,6 +631,12 @@
   </si>
   <si>
     <t>Added CRS to match the change request</t>
+  </si>
+  <si>
+    <t>v3.4</t>
+  </si>
+  <si>
+    <t>edited the naming convention</t>
   </si>
 </sst>
 </file>
@@ -1377,7 +1395,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1486,9 +1504,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1823,8 +1838,8 @@
   <sheetPr/>
   <dimension ref="A1:X63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="E61" sqref="E61"/>
+    <sheetView zoomScale="12" zoomScaleNormal="12" workbookViewId="0">
+      <selection activeCell="B58" sqref="B58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85714285714286" defaultRowHeight="15"/>
@@ -2572,7 +2587,7 @@
       </c>
     </row>
     <row r="48" ht="38.25" customHeight="1" spans="1:4">
-      <c r="A48" s="37"/>
+      <c r="A48" s="24"/>
       <c r="B48" s="25" t="s">
         <v>111</v>
       </c>
@@ -2580,15 +2595,15 @@
         <v>112</v>
       </c>
       <c r="D48" s="16" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="49" ht="38.25" customHeight="1" spans="1:4">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="49" ht="75" spans="1:4">
       <c r="A49" s="24"/>
-      <c r="B49" s="25" t="s">
+      <c r="B49" s="21" t="s">
         <v>113</v>
       </c>
-      <c r="C49" s="26" t="s">
+      <c r="C49" s="22" t="s">
         <v>114</v>
       </c>
       <c r="D49" s="16" t="s">
@@ -2597,10 +2612,10 @@
     </row>
     <row r="50" ht="48.75" customHeight="1" spans="1:4">
       <c r="A50" s="24"/>
-      <c r="B50" s="21" t="s">
+      <c r="B50" s="25" t="s">
         <v>115</v>
       </c>
-      <c r="C50" s="22" t="s">
+      <c r="C50" s="26" t="s">
         <v>116</v>
       </c>
       <c r="D50" s="23" t="s">
@@ -2609,10 +2624,10 @@
     </row>
     <row r="51" ht="50.25" customHeight="1" spans="1:4">
       <c r="A51" s="24"/>
-      <c r="B51" s="25" t="s">
+      <c r="B51" s="21" t="s">
         <v>117</v>
       </c>
-      <c r="C51" s="26" t="s">
+      <c r="C51" s="22" t="s">
         <v>118</v>
       </c>
       <c r="D51" s="16" t="s">
@@ -2621,24 +2636,24 @@
     </row>
     <row r="52" ht="36" customHeight="1" spans="1:4">
       <c r="A52" s="27"/>
-      <c r="B52" s="21" t="s">
+      <c r="B52" s="25" t="s">
         <v>119</v>
       </c>
-      <c r="C52" s="22" t="s">
+      <c r="C52" s="26" t="s">
         <v>120</v>
       </c>
       <c r="D52" s="23" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
     </row>
     <row r="53" ht="30" spans="1:4">
-      <c r="A53" s="38" t="s">
+      <c r="A53" s="37" t="s">
         <v>121</v>
       </c>
       <c r="B53" s="25" t="s">
         <v>122</v>
       </c>
-      <c r="C53" s="39" t="s">
+      <c r="C53" s="38" t="s">
         <v>123</v>
       </c>
       <c r="D53" s="16" t="s">
@@ -2646,7 +2661,7 @@
       </c>
     </row>
     <row r="54" ht="30" spans="1:4">
-      <c r="A54" s="40"/>
+      <c r="A54" s="39"/>
       <c r="B54" s="21" t="s">
         <v>124</v>
       </c>
@@ -2658,48 +2673,48 @@
       </c>
     </row>
     <row r="55" spans="1:4">
-      <c r="A55" s="40"/>
+      <c r="A55" s="39"/>
       <c r="B55" s="25" t="s">
         <v>126</v>
       </c>
-      <c r="C55" s="41" t="s">
+      <c r="C55" s="40" t="s">
         <v>127</v>
       </c>
       <c r="D55" s="16" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="56" ht="30" spans="1:4">
-      <c r="A56" s="40"/>
+    <row r="56" spans="1:4">
+      <c r="A56" s="39"/>
       <c r="B56" s="25" t="s">
         <v>128</v>
       </c>
-      <c r="C56" s="26" t="s">
-        <v>112</v>
+      <c r="C56" s="40" t="s">
+        <v>129</v>
       </c>
       <c r="D56" s="16" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="57" spans="1:4">
-      <c r="A57" s="40"/>
-      <c r="B57" s="25" t="s">
-        <v>129</v>
-      </c>
-      <c r="C57" s="41" t="s">
+    <row r="57" ht="30" spans="1:4">
+      <c r="A57" s="39"/>
+      <c r="B57" s="21" t="s">
         <v>130</v>
+      </c>
+      <c r="C57" s="22" t="s">
+        <v>131</v>
       </c>
       <c r="D57" s="16" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="58" ht="30" spans="1:4">
-      <c r="A58" s="40"/>
-      <c r="B58" s="21" t="s">
-        <v>131</v>
-      </c>
-      <c r="C58" s="22" t="s">
+      <c r="A58" s="39"/>
+      <c r="B58" s="25" t="s">
         <v>132</v>
+      </c>
+      <c r="C58" s="26" t="s">
+        <v>120</v>
       </c>
       <c r="D58" s="23" t="s">
         <v>88</v>
@@ -2733,11 +2748,11 @@
     </row>
     <row r="61" ht="30" spans="1:4">
       <c r="A61" s="24"/>
-      <c r="B61" s="25" t="s">
+      <c r="B61" s="21" t="s">
         <v>138</v>
       </c>
-      <c r="C61" s="26" t="s">
-        <v>112</v>
+      <c r="C61" s="22" t="s">
+        <v>139</v>
       </c>
       <c r="D61" s="16" t="s">
         <v>88</v>
@@ -2745,11 +2760,11 @@
     </row>
     <row r="62" ht="30" spans="1:4">
       <c r="A62" s="24"/>
-      <c r="B62" s="21" t="s">
-        <v>139</v>
-      </c>
-      <c r="C62" s="22" t="s">
+      <c r="B62" s="25" t="s">
         <v>140</v>
+      </c>
+      <c r="C62" s="26" t="s">
+        <v>141</v>
       </c>
       <c r="D62" s="23" t="s">
         <v>88</v>
@@ -2758,10 +2773,10 @@
     <row r="63" ht="34.5" customHeight="1" spans="1:4">
       <c r="A63" s="27"/>
       <c r="B63" s="25" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C63" s="26" t="s">
-        <v>142</v>
+        <v>120</v>
       </c>
       <c r="D63" s="16" t="s">
         <v>88</v>
@@ -2793,10 +2808,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView zoomScale="111" zoomScaleNormal="111" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" zoomScale="111" zoomScaleNormal="111" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="3"/>
@@ -3129,6 +3144,20 @@
         <v>45794</v>
       </c>
     </row>
+    <row r="24" ht="18.75" spans="1:4">
+      <c r="A24" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="D24" s="6">
+        <v>45794</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="1" orientation="portrait"/>

</xml_diff>